<commit_message>
Changed FL Boundary condition from 1E-8 - 10 to 0.01- 0.5
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation_moredata.xlsx
+++ b/Lacex_summary_FinalConfirmation_moredata.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700A6B80-B040-44E7-9BB2-E773A86B630D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BFFAC9-89A5-4BD0-825D-75787A35DFA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2835" windowWidth="17280" windowHeight="9030" xr2:uid="{B075899B-8E8B-4489-B096-777C4BA97E2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B075899B-8E8B-4489-B096-777C4BA97E2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,8 +33,88 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="24">
+  <si>
+    <t>HK-2</t>
+  </si>
+  <si>
+    <t>UMRC6</t>
+  </si>
+  <si>
+    <t>UOK262</t>
+  </si>
+  <si>
+    <t>UOK + DIDS</t>
+  </si>
+  <si>
+    <t>siRNA_c</t>
+  </si>
+  <si>
+    <t>siRNA</t>
+  </si>
+  <si>
+    <t>kPL</t>
+  </si>
+  <si>
+    <t>kMCT4</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>kLP</t>
+  </si>
+  <si>
+    <t>RsqP</t>
+  </si>
+  <si>
+    <t>RsqLin</t>
+  </si>
+  <si>
+    <t>RsqLex</t>
+  </si>
+  <si>
+    <t>RMSEP</t>
+  </si>
+  <si>
+    <t>RMSELin</t>
+  </si>
+  <si>
+    <t>RMSELex</t>
+  </si>
+  <si>
+    <t>R1P</t>
+  </si>
+  <si>
+    <t>R1Lex</t>
+  </si>
+  <si>
+    <t>R1Lin</t>
+  </si>
+  <si>
+    <t>kMCT1</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -61,13 +144,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -78,6 +177,1987 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kPL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$29:$F$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.3632467423976377E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.8102841025300172E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.0181144930654133E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.1957167148318739E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$29:$F$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.3632467423976377E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.8102841025300172E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.0181144930654133E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.1957167148318739E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$27:$F$27</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK + DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.6597166972760207E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2969578710698102E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9850373025406699E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7436370403402304E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA70-4335-90A7-C36AA9111C33}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="614816128"/>
+        <c:axId val="614817440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="614816128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="614817440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="614817440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="614816128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kMCT4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$G$45:$J$45</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.7887236211488991E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.12579716058654763</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.34452837581693579</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.44401386483779698</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$45:$J$45</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.7887236211488991E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.12579716058654763</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.34452837581693579</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.44401386483779698</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$G$43:$J$43</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK + DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$44:$J$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.14700895503484715</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51874426073426694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67733097633142481</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55341627633490109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DCC-4E3E-86E8-4C3C5C34006E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="551193376"/>
+        <c:axId val="551193704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="551193376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551193704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="551193704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551193376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E91B37CB-01EF-4B45-8C60-3C29F4BD4C9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3C964F-F561-4D04-AB09-C675C1097902}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="27">
+          <cell r="C27" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="E27" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>kMCT4</v>
+          </cell>
+          <cell r="C28">
+            <v>9.2535545750464687E-2</v>
+          </cell>
+          <cell r="D28">
+            <v>0.3541415185008206</v>
+          </cell>
+          <cell r="E28">
+            <v>0.75444268232926348</v>
+          </cell>
+          <cell r="F28">
+            <v>0.16916415025152015</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>1.2057455739979463E-2</v>
+          </cell>
+          <cell r="D29">
+            <v>5.7309495294150879E-2</v>
+          </cell>
+          <cell r="E29">
+            <v>0.39928208436858398</v>
+          </cell>
+          <cell r="F29">
+            <v>0.13741088889033834</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="D31" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="E31" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="F31" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="G31" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32" t="str">
+            <v>R1L</v>
+          </cell>
+          <cell r="D32">
+            <v>7.384890314233869E-2</v>
+          </cell>
+          <cell r="E32">
+            <v>5.0263555960985945E-2</v>
+          </cell>
+          <cell r="F32">
+            <v>6.3109847044927683E-2</v>
+          </cell>
+          <cell r="G32">
+            <v>8.0357873156810505E-2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="D33">
+            <v>2.3803754511435734E-2</v>
+          </cell>
+          <cell r="E33">
+            <v>2.3947765296666392E-2</v>
+          </cell>
+          <cell r="F33">
+            <v>1.0466686942143609E-2</v>
+          </cell>
+          <cell r="G33">
+            <v>1.4625933793160245E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,15 +2457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5426EC7D-B74E-4953-AA3A-EC81D60A2FE4}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2.0781114759556379E-2</v>
       </c>
@@ -441,7 +2521,7 @@
         <v>0.13102591930261462</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.9731495213395425E-2</v>
       </c>
@@ -497,7 +2577,7 @@
         <v>7.8981907325062134E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.0365465865092722E-2</v>
       </c>
@@ -553,7 +2633,7 @@
         <v>8.6621753913290897E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.9994972552697242E-2</v>
       </c>
@@ -608,8 +2688,35 @@
       <c r="R4">
         <v>0.25391303933089066</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V4" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.023647882476649E-2</v>
       </c>
@@ -664,8 +2771,41 @@
       <c r="R5">
         <v>0.11728586191248075</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T5" s="1">
+        <f>1/51</f>
+        <v>1.9607843137254902E-2</v>
+      </c>
+      <c r="U5">
+        <f>0.0001</f>
+        <v>1E-4</v>
+      </c>
+      <c r="V5">
+        <f>10^-8</f>
+        <v>1E-8</v>
+      </c>
+      <c r="W5" s="1">
+        <f>1/30-0.001</f>
+        <v>3.2333333333333332E-2</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>1E-3</v>
+      </c>
+      <c r="Z5" s="1">
+        <f>1/37.7</f>
+        <v>2.652519893899204E-2</v>
+      </c>
+      <c r="AA5">
+        <f>10^-8</f>
+        <v>1E-8</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.0231218059161282E-2</v>
       </c>
@@ -720,8 +2860,38 @@
       <c r="R6">
         <v>0.10849575202156349</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T6" s="1">
+        <f>1/47</f>
+        <v>2.1276595744680851E-2</v>
+      </c>
+      <c r="U6">
+        <v>0.08</v>
+      </c>
+      <c r="V6">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1">
+        <f>1/10+0.001</f>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="X6">
+        <v>0.1</v>
+      </c>
+      <c r="Y6">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="1">
+        <f>1/35.7</f>
+        <v>2.8011204481792715E-2</v>
+      </c>
+      <c r="AA6">
+        <v>10</v>
+      </c>
+      <c r="AB6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.0352218032308276E-2</v>
       </c>
@@ -777,7 +2947,7 @@
         <v>9.123185443573037E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.0420572162940933E-2</v>
       </c>
@@ -833,7 +3003,7 @@
         <v>0.21109361441809982</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.9856607624304978E-2</v>
       </c>
@@ -889,7 +3059,7 @@
         <v>0.19874222923660653</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.9607843138025917E-2</v>
       </c>
@@ -945,7 +3115,7 @@
         <v>0.13578312841773169</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.9607868588388273E-2</v>
       </c>
@@ -1001,7 +3171,7 @@
         <v>0.14608669072309458</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.9955136692618142E-2</v>
       </c>
@@ -1057,7 +3227,7 @@
         <v>0.25541943931821498</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.9932134010064936E-2</v>
       </c>
@@ -1113,7 +3283,7 @@
         <v>0.32512088803992523</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.9701617767527744E-2</v>
       </c>
@@ -1169,7 +3339,7 @@
         <v>0.12637696756741412</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.9647451233942632E-2</v>
       </c>
@@ -1225,7 +3395,7 @@
         <v>0.28282810134363656</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.0254106371624593E-2</v>
       </c>
@@ -1281,7 +3451,7 @@
         <v>0.24695341960909117</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2.0450312385911232E-2</v>
       </c>
@@ -1337,7 +3507,7 @@
         <v>6.8346251598520716E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.9778014887334602E-2</v>
       </c>
@@ -1393,7 +3563,7 @@
         <v>7.9032400824502233E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.9770622156745334E-2</v>
       </c>
@@ -1449,7 +3619,7 @@
         <v>0.49148438074501466</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.025226724750458E-2</v>
       </c>
@@ -1505,7 +3675,7 @@
         <v>0.10046394420079181</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.9645457395348342E-2</v>
       </c>
@@ -1561,7 +3731,7 @@
         <v>0.12648227289179581</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.9998083024111244E-2</v>
       </c>
@@ -1617,7 +3787,2416 @@
         <v>9.5764802955078374E-2</v>
       </c>
     </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" t="str">
+        <f>_xlfn.IFS(ABS(A1-T$5)&lt;=0.01*T$5,"Lower",ABS(A1-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" ref="O23:W38" si="0">_xlfn.IFS(ABS(B1-U$5)&lt;=0.01*U$5,"Lower",ABS(B1-U$6)&lt;=0.01*U$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W23" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD23" t="str">
+        <f t="shared" ref="AD23:AE44" si="1">_xlfn.IFS(ABS(Q1-AJ$5)&lt;=0.01*AJ$5,"Lower",ABS(Q1-AJ$6)&lt;=0.01*AJ$6,"Upper",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="AE23" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <f>AVERAGE(A$1:A$3)</f>
+        <v>2.0292691946014841E-2</v>
+      </c>
+      <c r="C24">
+        <f>AVERAGE(A$4:A$6)</f>
+        <v>2.0154223145541671E-2</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE(A$7:A$12,A$17:A$19)</f>
+        <v>1.9977688407619744E-2</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGE(A$13:A$16)</f>
+        <v>1.9883827345789976E-2</v>
+      </c>
+      <c r="F24">
+        <f>A$20</f>
+        <v>2.025226724750458E-2</v>
+      </c>
+      <c r="G24">
+        <f>AVERAGE(A$21:A$22)</f>
+        <v>1.9821770209729792E-2</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" ref="N24:W44" si="2">_xlfn.IFS(ABS(A2-T$5)&lt;=0.01*T$5,"Lower",ABS(A2-T$6)&lt;=0.01*T$6,"Upper",TRUE,"Ok")</f>
+        <v>Lower</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="R24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T24" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W24" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD24" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE24" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f>STDEV(A$1:A$3)/SQRT(COUNT(A$1:A$3))</f>
+        <v>3.0517608599749297E-4</v>
+      </c>
+      <c r="C25">
+        <f>STDEV(A$4:A$6)/SQRT(COUNT(A$4:A$6))</f>
+        <v>7.9639777340775558E-5</v>
+      </c>
+      <c r="D25">
+        <f>STDEV(A$7:A$12,A$17:A$19)/SQRT(COUNT(A$7:A$12,A$17:A$19))</f>
+        <v>1.1372842838082459E-4</v>
+      </c>
+      <c r="E25">
+        <f>STDEV(A$13:A$16)/SQRT(COUNT(A$13:A$16))</f>
+        <v>1.379957992866012E-4</v>
+      </c>
+      <c r="G25">
+        <f>STDEV(A$21:A$22)/SQRT(COUNT(A$21:A$22))</f>
+        <v>1.7631281438145079E-4</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T25" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W25" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD25" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE25" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N26" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD26" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE26" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>5</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T27" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W27" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD27" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE27" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <f>AVERAGE(B$1:B$3)</f>
+        <v>3.6597166972760207E-3</v>
+      </c>
+      <c r="D28">
+        <f>AVERAGE(B$4:B$6)</f>
+        <v>1.2969578710698102E-2</v>
+      </c>
+      <c r="E28">
+        <f>AVERAGE(B$7:B$12,B$17:B$19)</f>
+        <v>3.9850373025406699E-2</v>
+      </c>
+      <c r="F28">
+        <f>AVERAGE(B$13:B$16)</f>
+        <v>1.7436370403402304E-2</v>
+      </c>
+      <c r="G28">
+        <f>B$20</f>
+        <v>3.661038817423995E-2</v>
+      </c>
+      <c r="H28">
+        <f>AVERAGE(B$21:B$22)</f>
+        <v>7.9999999999977797E-2</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W28" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD28" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE28" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f>STDEV(B$1:B$3)/SQRT(COUNT(B$1:B$3))</f>
+        <v>1.3632467423976377E-4</v>
+      </c>
+      <c r="D29">
+        <f>STDEV(B$4:B$6)/SQRT(COUNT(B$4:B$6))</f>
+        <v>2.8102841025300172E-3</v>
+      </c>
+      <c r="E29">
+        <f>STDEV(B$7:B$12,B$17:B$19)/SQRT(COUNT(B$7:B$12,B$17:B$19))</f>
+        <v>1.0181144930654133E-2</v>
+      </c>
+      <c r="F29">
+        <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
+        <v>9.1957167148318739E-3</v>
+      </c>
+      <c r="H29">
+        <f>STDEV(B$21:B$22)/SQRT(COUNT(B$21:B$22))</f>
+        <v>0</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD29" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE29" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N30" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD30" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE30" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T31" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD31" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE31" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <f>AVERAGE(C$1:C$3)</f>
+        <v>0.19023535438688108</v>
+      </c>
+      <c r="E32">
+        <f>AVERAGE(C$4:C$6)</f>
+        <v>0.11098762168381754</v>
+      </c>
+      <c r="F32">
+        <f>AVERAGE(C$7:C$12,C$17:C$19)</f>
+        <v>0.31184021552856422</v>
+      </c>
+      <c r="G32">
+        <f>AVERAGE(C$13:C$16)</f>
+        <v>0.12473897964381199</v>
+      </c>
+      <c r="H32">
+        <f>C$20</f>
+        <v>0.58530339194918313</v>
+      </c>
+      <c r="I32">
+        <f>AVERAGE(C$21:C$22)</f>
+        <v>2.4738863416288659</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="U32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W32" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD32" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE32" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="33" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f>STDEV(C$1:C$3)/SQRT(COUNT(C$1:C$3))</f>
+        <v>3.4764251947037965E-2</v>
+      </c>
+      <c r="E33">
+        <f>STDEV(C$4:C$6)/SQRT(COUNT(C$4:C$6))</f>
+        <v>0.10709949468666879</v>
+      </c>
+      <c r="F33">
+        <f>STDEV(C$7:C$12,C$17:C$19)/SQRT(COUNT(C$7:C$12,C$17:C$19))</f>
+        <v>0.21648529436558617</v>
+      </c>
+      <c r="G33">
+        <f>STDEV(C$13:C$16)/SQRT(COUNT(C$13:C$16))</f>
+        <v>7.3357716046404037E-2</v>
+      </c>
+      <c r="I33">
+        <f>STDEV(C$21:C$22)/SQRT(COUNT(C$21:C$22))</f>
+        <v>1.3172879840323004E-2</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="U33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W33" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD33" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE33" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="34" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="N34" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T34" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="U34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W34" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD34" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE34" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="35" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" t="s">
+        <v>5</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="U35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD35" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE35" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="36" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36">
+        <f>AVERAGE(D$1:D$3)</f>
+        <v>5.9621023719336724E-2</v>
+      </c>
+      <c r="F36">
+        <f>AVERAGE(D$4:D$6)</f>
+        <v>5.8426894246005306E-2</v>
+      </c>
+      <c r="G36">
+        <f>AVERAGE(D$7:D$12,D$17:D$19)</f>
+        <v>5.408192058558043E-2</v>
+      </c>
+      <c r="H36">
+        <f>AVERAGE(D$13:D$16)</f>
+        <v>6.7749360389357263E-2</v>
+      </c>
+      <c r="I36">
+        <f>D$20</f>
+        <v>4.2860723219890554E-2</v>
+      </c>
+      <c r="J36">
+        <f>AVERAGE(D$21:D$22)</f>
+        <v>4.4012991541004708E-2</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="U36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD36" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE36" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="37" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f>STDEV(D$1:D$3)/SQRT(COUNT(D$1:D$3))</f>
+        <v>2.0792372896380848E-2</v>
+      </c>
+      <c r="F37">
+        <f>STDEV(D$4:D$6)/SQRT(COUNT(D$4:D$6))</f>
+        <v>1.7123224610862724E-2</v>
+      </c>
+      <c r="G37">
+        <f>STDEV(D$7:D$12,D$17:D$19)/SQRT(COUNT(D$7:D$12,D$17:D$19))</f>
+        <v>5.1216710439505198E-3</v>
+      </c>
+      <c r="H37">
+        <f>STDEV(D$13:D$16)/SQRT(COUNT(D$13:D$16))</f>
+        <v>1.5627247705565079E-2</v>
+      </c>
+      <c r="J37">
+        <f>STDEV(D$21:D$22)/SQRT(COUNT(D$21:D$22))</f>
+        <v>6.4496365750799079E-4</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="R37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T37" t="str">
+        <f t="shared" si="0"/>
+        <v>Lower</v>
+      </c>
+      <c r="U37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="V37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W37" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD37" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE37" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="38" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="N38" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="R38" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="T38" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="U38" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="V38" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="W38" t="str">
+        <f t="shared" si="0"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD38" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE38" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="39" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" t="s">
+        <v>5</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="R39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="S39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="T39" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper</v>
+      </c>
+      <c r="U39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="V39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="W39" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD39" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE39" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="40" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40">
+        <f>AVERAGE(E$1:E$3)</f>
+        <v>2.2210033221700154E-14</v>
+      </c>
+      <c r="G40">
+        <f>AVERAGE(E$4:E$6)</f>
+        <v>2.8172663076369224E-7</v>
+      </c>
+      <c r="H40">
+        <f>AVERAGE(E$7:E$12,E$17:E$19)</f>
+        <v>4.0146854743199973E-4</v>
+      </c>
+      <c r="I40">
+        <f>AVERAGE(E$13:E$16)</f>
+        <v>4.4129444733917032E-6</v>
+      </c>
+      <c r="J40">
+        <f>E$20</f>
+        <v>9.9999999999977801E-2</v>
+      </c>
+      <c r="K40">
+        <f>AVERAGE(E$21:E$22)</f>
+        <v>2.2207396253646659E-14</v>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="P40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="R40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="S40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="T40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="U40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="V40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="W40" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD40" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE40" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="41" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f>STDEV(E$1:E$3)/SQRT(COUNT(E$1:E$3))</f>
+        <v>4.8250618270174104E-18</v>
+      </c>
+      <c r="G41">
+        <f>STDEV(E$4:E$6)/SQRT(COUNT(E$4:E$6))</f>
+        <v>2.8172660276019622E-7</v>
+      </c>
+      <c r="H41">
+        <f>STDEV(E$7:E$12,E$17:E$19)/SQRT(COUNT(E$7:E$12,E$17:E$19))</f>
+        <v>2.8632212313389749E-4</v>
+      </c>
+      <c r="I41">
+        <f>STDEV(E$13:E$16)/SQRT(COUNT(E$13:E$16))</f>
+        <v>4.4127585456074152E-6</v>
+      </c>
+      <c r="K41">
+        <f>STDEV(E$21:E$22)/SQRT(COUNT(E$21:E$22))</f>
+        <v>2.2044986974114701E-18</v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper</v>
+      </c>
+      <c r="P41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="R41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="S41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="T41" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="U41" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="V41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="W41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD41" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE41" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="42" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="N42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="P42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="R42" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper</v>
+      </c>
+      <c r="S42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="T42" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="U42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="V42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="W42" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD42" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE42" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="43" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>2</v>
+      </c>
+      <c r="J43" t="s">
+        <v>3</v>
+      </c>
+      <c r="K43" t="s">
+        <v>4</v>
+      </c>
+      <c r="L43" t="s">
+        <v>5</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper</v>
+      </c>
+      <c r="P43" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="R43" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="S43" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="T43" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="U43" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="V43" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="W43" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD43" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE43" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="44" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44">
+        <f>AVERAGE(F$1:F$3)</f>
+        <v>0.14700895503484715</v>
+      </c>
+      <c r="H44">
+        <f>AVERAGE(F$4:F$6)</f>
+        <v>0.51874426073426694</v>
+      </c>
+      <c r="I44">
+        <f>AVERAGE(F$7:F$12,F$17:F$19)</f>
+        <v>0.67733097633142481</v>
+      </c>
+      <c r="J44">
+        <f>AVERAGE(F$13:F$16)</f>
+        <v>0.55341627633490109</v>
+      </c>
+      <c r="K44">
+        <f>F$20</f>
+        <v>0.13494299556910744</v>
+      </c>
+      <c r="L44">
+        <f>AVERAGE(F$21:F$22)</f>
+        <v>0.24225139350649832</v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper</v>
+      </c>
+      <c r="P44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="R44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="S44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="T44" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
+      </c>
+      <c r="U44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="V44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="W44" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="AD44" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="AE44" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="45" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
+        <v>3.7887236211488991E-2</v>
+      </c>
+      <c r="H45">
+        <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
+        <v>0.12579716058654763</v>
+      </c>
+      <c r="I45">
+        <f>STDEV(F$7:F$12,F$17:F$19)/SQRT(COUNT(F$7:F$12,F$17:F$19))</f>
+        <v>0.34452837581693579</v>
+      </c>
+      <c r="J45">
+        <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
+        <v>0.44401386483779698</v>
+      </c>
+      <c r="L45">
+        <f>STDEV(F$21:F$22)/SQRT(COUNT(F$21:F$22))</f>
+        <v>2.5042119599933226E-2</v>
+      </c>
+      <c r="N45" t="s">
+        <v>17</v>
+      </c>
+      <c r="O45" t="s">
+        <v>6</v>
+      </c>
+      <c r="P45" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>19</v>
+      </c>
+      <c r="R45" t="s">
+        <v>10</v>
+      </c>
+      <c r="S45" t="s">
+        <v>7</v>
+      </c>
+      <c r="T45" t="s">
+        <v>18</v>
+      </c>
+      <c r="U45" t="s">
+        <v>9</v>
+      </c>
+      <c r="V45" t="s">
+        <v>20</v>
+      </c>
+      <c r="W45" t="s">
+        <v>10</v>
+      </c>
+      <c r="X45" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>2</v>
+      </c>
+      <c r="K47" t="s">
+        <v>3</v>
+      </c>
+      <c r="L47" t="s">
+        <v>4</v>
+      </c>
+      <c r="M47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="4:31" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48">
+        <f>AVERAGE(G$1:G$3)</f>
+        <v>2.6612095404732927E-2</v>
+      </c>
+      <c r="I48">
+        <f>AVERAGE(G$4:G$6)</f>
+        <v>2.7473079382476524E-2</v>
+      </c>
+      <c r="J48">
+        <f>AVERAGE(G$7:G$12,G$17:G$19)</f>
+        <v>2.7283317623498213E-2</v>
+      </c>
+      <c r="K48">
+        <f>AVERAGE(G$13:G$16)</f>
+        <v>2.7369710249433226E-2</v>
+      </c>
+      <c r="L48">
+        <f>G$20</f>
+        <v>2.6595818555612983E-2</v>
+      </c>
+      <c r="M48">
+        <f>AVERAGE(G$21:G$22)</f>
+        <v>2.654766832169313E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <f>STDEV(G$1:G$3)/SQRT(COUNT(G$1:G$3))</f>
+        <v>4.5088837848277105E-5</v>
+      </c>
+      <c r="I49">
+        <f>STDEV(G$4:G$6)/SQRT(COUNT(G$4:G$6))</f>
+        <v>3.7252970632583378E-4</v>
+      </c>
+      <c r="J49">
+        <f>STDEV(G$7:G$12,G$17:G$19)/SQRT(COUNT(G$7:G$12,G$17:G$19))</f>
+        <v>1.9591704856672309E-4</v>
+      </c>
+      <c r="K49">
+        <f>STDEV(G$13:G$16)/SQRT(COUNT(G$13:G$16))</f>
+        <v>2.9674052868955972E-4</v>
+      </c>
+      <c r="M49">
+        <f>STDEV(G$21:G$22)/SQRT(COUNT(G$21:G$22))</f>
+        <v>5.3908646953891581E-6</v>
+      </c>
+    </row>
+    <row r="51" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>1</v>
+      </c>
+      <c r="K51" t="s">
+        <v>2</v>
+      </c>
+      <c r="L51" t="s">
+        <v>3</v>
+      </c>
+      <c r="M51" t="s">
+        <v>4</v>
+      </c>
+      <c r="N51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52">
+        <f>AVERAGE(H$1:H$3)</f>
+        <v>7.5917629324230532E-2</v>
+      </c>
+      <c r="J52">
+        <f>AVERAGE(H$4:H$6)</f>
+        <v>0.39118585551184881</v>
+      </c>
+      <c r="K52">
+        <f>AVERAGE(H$7:H$12,H$17:H$19)</f>
+        <v>1.4556807367818019</v>
+      </c>
+      <c r="L52">
+        <f>AVERAGE(H$13:H$16)</f>
+        <v>2.6891949704917932</v>
+      </c>
+      <c r="M52">
+        <f>H$20</f>
+        <v>0.20586204465426139</v>
+      </c>
+      <c r="N52">
+        <f>AVERAGE(H$21:H$22)</f>
+        <v>0.32625927521033604</v>
+      </c>
+    </row>
+    <row r="53" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <f>STDEV(H$1:H$3)/SQRT(COUNT(H$1:H$3))</f>
+        <v>2.1967251752266336E-2</v>
+      </c>
+      <c r="J53">
+        <f>STDEV(H$4:H$6)/SQRT(COUNT(H$4:H$6))</f>
+        <v>0.14380117024004904</v>
+      </c>
+      <c r="K53">
+        <f>STDEV(H$7:H$12,H$17:H$19)/SQRT(COUNT(H$7:H$12,H$17:H$19))</f>
+        <v>1.0473379060285419</v>
+      </c>
+      <c r="L53">
+        <f>STDEV(H$13:H$16)/SQRT(COUNT(H$13:H$16))</f>
+        <v>2.4385643271491557</v>
+      </c>
+      <c r="N53">
+        <f>STDEV(H$21:H$22)/SQRT(COUNT(H$21:H$22))</f>
+        <v>4.6557772084041354E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>0</v>
+      </c>
+      <c r="K55" t="s">
+        <v>1</v>
+      </c>
+      <c r="L55" t="s">
+        <v>2</v>
+      </c>
+      <c r="M55" t="s">
+        <v>3</v>
+      </c>
+      <c r="N55" t="s">
+        <v>4</v>
+      </c>
+      <c r="O55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56">
+        <f>AVERAGE(I$1:I$3)</f>
+        <v>4.7043281897724644E-2</v>
+      </c>
+      <c r="K56">
+        <f>AVERAGE(I$4:I$6)</f>
+        <v>3.4991609077748002E-14</v>
+      </c>
+      <c r="L56">
+        <f>AVERAGE(I$7:I$12,I$17:I$19)</f>
+        <v>7.4630219943887829E-4</v>
+      </c>
+      <c r="M56">
+        <f>AVERAGE(I$13:I$16)</f>
+        <v>4.0530954529238379E-6</v>
+      </c>
+      <c r="N56">
+        <f>I$20</f>
+        <v>2.2204503459977956E-14</v>
+      </c>
+      <c r="O56">
+        <f>AVERAGE(I$21:I$22)</f>
+        <v>2.2204713856538582E-14</v>
+      </c>
+    </row>
+    <row r="57" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <f>STDEV(I$1:I$3)/SQRT(COUNT(I$1:I$3))</f>
+        <v>4.7043281897702433E-2</v>
+      </c>
+      <c r="K57">
+        <f>STDEV(I$4:I$6)/SQRT(COUNT(I$4:I$6))</f>
+        <v>6.3772773096146374E-15</v>
+      </c>
+      <c r="L57">
+        <f>STDEV(I$7:I$12,I$17:I$19)/SQRT(COUNT(I$7:I$12,I$17:I$19))</f>
+        <v>7.4617681527279955E-4</v>
+      </c>
+      <c r="M57">
+        <f>STDEV(I$13:I$16)/SQRT(COUNT(I$13:I$16))</f>
+        <v>4.0529326997889823E-6</v>
+      </c>
+      <c r="O57">
+        <f>STDEV(I$21:I$22)/SQRT(COUNT(I$21:I$22))</f>
+        <v>2.2978287727198393E-19</v>
+      </c>
+    </row>
+    <row r="59" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>0</v>
+      </c>
+      <c r="L59" t="s">
+        <v>1</v>
+      </c>
+      <c r="M59" t="s">
+        <v>2</v>
+      </c>
+      <c r="N59" t="s">
+        <v>3</v>
+      </c>
+      <c r="O59" t="s">
+        <v>4</v>
+      </c>
+      <c r="P59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>21</v>
+      </c>
+      <c r="K60">
+        <f>AVERAGE(J$1:J$3)</f>
+        <v>3.6073751761273023</v>
+      </c>
+      <c r="L60">
+        <f>AVERAGE(J$4:J$6)</f>
+        <v>4.5811578254944498</v>
+      </c>
+      <c r="M60">
+        <f>AVERAGE(J$7:J$12,J$17:J$19)</f>
+        <v>3.51692207739478</v>
+      </c>
+      <c r="N60">
+        <f>AVERAGE(J$13:J$16)</f>
+        <v>4.4114283716836216</v>
+      </c>
+      <c r="O60">
+        <f>J$20</f>
+        <v>2.4328816932437634</v>
+      </c>
+      <c r="P60">
+        <f>AVERAGE(J$21:J$22)</f>
+        <v>3.3952480713996169</v>
+      </c>
+    </row>
+    <row r="61" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <f>STDEV(J$1:J$3)/SQRT(COUNT(J$1:J$3))</f>
+        <v>1.0122908364969967</v>
+      </c>
+      <c r="L61">
+        <f>STDEV(J$4:J$6)/SQRT(COUNT(J$4:J$6))</f>
+        <v>0.74102585341338212</v>
+      </c>
+      <c r="M61">
+        <f>STDEV(J$7:J$12,J$17:J$19)/SQRT(COUNT(J$7:J$12,J$17:J$19))</f>
+        <v>0.38597012567114813</v>
+      </c>
+      <c r="N61">
+        <f>STDEV(J$13:J$16)/SQRT(COUNT(J$13:J$16))</f>
+        <v>0.66382289260777116</v>
+      </c>
+      <c r="P61">
+        <f>STDEV(J$21:J$22)/SQRT(COUNT(J$21:J$22))</f>
+        <v>0.42113282835845389</v>
+      </c>
+    </row>
+    <row r="63" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
+        <v>0</v>
+      </c>
+      <c r="M63" t="s">
+        <v>1</v>
+      </c>
+      <c r="N63" t="s">
+        <v>2</v>
+      </c>
+      <c r="O63" t="s">
+        <v>3</v>
+      </c>
+      <c r="P63" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>22</v>
+      </c>
+      <c r="L64">
+        <f>AVERAGE(K$1:K$3)</f>
+        <v>18.818233196202602</v>
+      </c>
+      <c r="M64">
+        <f>AVERAGE(K$4:K$6)</f>
+        <v>14.884031830230191</v>
+      </c>
+      <c r="N64">
+        <f>AVERAGE(K$7:K$12,K$17:K$19)</f>
+        <v>17.654540033650139</v>
+      </c>
+      <c r="O64">
+        <f>AVERAGE(K$13:K$16)</f>
+        <v>15.511444233694277</v>
+      </c>
+      <c r="P64">
+        <f>K$20</f>
+        <v>21.999999999997559</v>
+      </c>
+      <c r="Q64">
+        <f>AVERAGE(K$21:K$22)</f>
+        <v>20.073933739916427</v>
+      </c>
+    </row>
+    <row r="65" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <f>STDEV(K$1:K$3)/SQRT(COUNT(K$1:K$3))</f>
+        <v>2.749667108525184</v>
+      </c>
+      <c r="M65">
+        <f>STDEV(K$4:K$6)/SQRT(COUNT(K$4:K$6))</f>
+        <v>2.7073905114872208</v>
+      </c>
+      <c r="N65">
+        <f>STDEV(K$7:K$12,K$17:K$19)/SQRT(COUNT(K$7:K$12,K$17:K$19))</f>
+        <v>1.3292941062026584</v>
+      </c>
+      <c r="O65">
+        <f>STDEV(K$13:K$16)/SQRT(COUNT(K$13:K$16))</f>
+        <v>1.694872077696727</v>
+      </c>
+      <c r="Q65">
+        <f>STDEV(K$21:K$22)/SQRT(COUNT(K$21:K$22))</f>
+        <v>0.877136811613207</v>
+      </c>
+    </row>
+    <row r="67" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="M67" t="s">
+        <v>0</v>
+      </c>
+      <c r="N67" t="s">
+        <v>1</v>
+      </c>
+      <c r="O67" t="s">
+        <v>2</v>
+      </c>
+      <c r="P67" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>4</v>
+      </c>
+      <c r="R67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
+        <v>23</v>
+      </c>
+      <c r="M68">
+        <f>AVERAGE(L$1:L$3)</f>
+        <v>302386980.01654357</v>
+      </c>
+      <c r="N68">
+        <f>AVERAGE(L$4:L$6)</f>
+        <v>307023757.75154978</v>
+      </c>
+      <c r="O68">
+        <f>AVERAGE(L$7:L$12,L$17:L$19)</f>
+        <v>455668700.79304117</v>
+      </c>
+      <c r="P68">
+        <f>AVERAGE(L$13:L$16)</f>
+        <v>589413319.65210319</v>
+      </c>
+      <c r="Q68">
+        <f>L$20</f>
+        <v>898068381.93210459</v>
+      </c>
+      <c r="R68">
+        <f>AVERAGE(L$21:L$22)</f>
+        <v>1240491715.0529809</v>
+      </c>
+    </row>
+    <row r="69" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="M69">
+        <f>STDEV(L$1:L$3)/SQRT(COUNT(L$1:L$3))</f>
+        <v>98309638.616056696</v>
+      </c>
+      <c r="N69">
+        <f>STDEV(L$4:L$6)/SQRT(COUNT(L$4:L$6))</f>
+        <v>161012746.78001404</v>
+      </c>
+      <c r="O69">
+        <f>STDEV(L$7:L$12,L$17:L$19)/SQRT(COUNT(L$7:L$12,L$17:L$19))</f>
+        <v>171677736.19797912</v>
+      </c>
+      <c r="P69">
+        <f>STDEV(L$13:L$16)/SQRT(COUNT(L$13:L$16))</f>
+        <v>96090682.504834935</v>
+      </c>
+      <c r="R69">
+        <f>STDEV(L$21:L$22)/SQRT(COUNT(L$21:L$22))</f>
+        <v>328743761.02513415</v>
+      </c>
+    </row>
+    <row r="71" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="N71" t="s">
+        <v>0</v>
+      </c>
+      <c r="O71" t="s">
+        <v>1</v>
+      </c>
+      <c r="P71" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>3</v>
+      </c>
+      <c r="R71" t="s">
+        <v>4</v>
+      </c>
+      <c r="S71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="M72" t="s">
+        <v>11</v>
+      </c>
+      <c r="N72">
+        <f>AVERAGE(M$1:M$3)</f>
+        <v>0.99662997411815801</v>
+      </c>
+      <c r="O72">
+        <f>AVERAGE(M$4:M$6)</f>
+        <v>0.99678502774392774</v>
+      </c>
+      <c r="P72">
+        <f>AVERAGE(M$7:M$12,M$17:M$19)</f>
+        <v>0.9946243241560917</v>
+      </c>
+      <c r="Q72">
+        <f>AVERAGE(M$13:M$16)</f>
+        <v>0.99613211356786546</v>
+      </c>
+      <c r="R72">
+        <f>M$20</f>
+        <v>0.99345692483643755</v>
+      </c>
+      <c r="S72">
+        <f>AVERAGE(M$21:M$22)</f>
+        <v>0.99082673534324806</v>
+      </c>
+    </row>
+    <row r="73" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <f>STDEV(M$1:M$3)/SQRT(COUNT(M$1:M$3))</f>
+        <v>4.9336913887755639E-4</v>
+      </c>
+      <c r="O73">
+        <f>STDEV(M$4:M$6)/SQRT(COUNT(M$4:M$6))</f>
+        <v>3.486949347042988E-4</v>
+      </c>
+      <c r="P73">
+        <f>STDEV(M$7:M$12,M$17:M$19)/SQRT(COUNT(M$7:M$12,M$17:M$19))</f>
+        <v>1.9810102119476331E-3</v>
+      </c>
+      <c r="Q73">
+        <f>STDEV(M$13:M$16)/SQRT(COUNT(M$13:M$16))</f>
+        <v>1.6834148194512729E-3</v>
+      </c>
+      <c r="S73">
+        <f>STDEV(M$21:M$22)/SQRT(COUNT(M$21:M$22))</f>
+        <v>3.5454264834695604E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="O75" t="s">
+        <v>0</v>
+      </c>
+      <c r="P75" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>2</v>
+      </c>
+      <c r="R75" t="s">
+        <v>3</v>
+      </c>
+      <c r="S75" t="s">
+        <v>4</v>
+      </c>
+      <c r="T75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="N76" t="s">
+        <v>12</v>
+      </c>
+      <c r="O76">
+        <f>AVERAGE(N$1:N$3)</f>
+        <v>0.99199938412162059</v>
+      </c>
+      <c r="P76">
+        <f>AVERAGE(N$4:N$6)</f>
+        <v>0.97541479470508063</v>
+      </c>
+      <c r="Q76">
+        <f>AVERAGE(N$7:N$12,N$17:N$19)</f>
+        <v>0.96965084484165076</v>
+      </c>
+      <c r="R76">
+        <f>AVERAGE(N$13:N$16)</f>
+        <v>0.99258746444793977</v>
+      </c>
+      <c r="S76">
+        <f>N$20</f>
+        <v>0.98644924290192071</v>
+      </c>
+      <c r="T76">
+        <f>AVERAGE(N$21:N$22)</f>
+        <v>0.97245198416071776</v>
+      </c>
+    </row>
+    <row r="77" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="O77">
+        <f>STDEV(N$1:N$3)/SQRT(COUNT(N$1:N$3))</f>
+        <v>3.3666505227571966E-3</v>
+      </c>
+      <c r="P77">
+        <f>STDEV(N$4:N$6)/SQRT(COUNT(N$4:N$6))</f>
+        <v>1.0654580102394942E-2</v>
+      </c>
+      <c r="Q77">
+        <f>STDEV(N$7:N$12,N$17:N$19)/SQRT(COUNT(N$7:N$12,N$17:N$19))</f>
+        <v>1.1875659785251722E-2</v>
+      </c>
+      <c r="R77">
+        <f>STDEV(N$13:N$16)/SQRT(COUNT(N$13:N$16))</f>
+        <v>2.5055085561655724E-3</v>
+      </c>
+      <c r="T77">
+        <f>STDEV(N$21:N$22)/SQRT(COUNT(N$21:N$22))</f>
+        <v>1.2023160573295222E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="P79" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>1</v>
+      </c>
+      <c r="R79" t="s">
+        <v>2</v>
+      </c>
+      <c r="S79" t="s">
+        <v>3</v>
+      </c>
+      <c r="T79" t="s">
+        <v>4</v>
+      </c>
+      <c r="U79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="O80" t="s">
+        <v>13</v>
+      </c>
+      <c r="P80">
+        <f>AVERAGE(O$1:O$3)</f>
+        <v>0.99642630127703191</v>
+      </c>
+      <c r="Q80">
+        <f>AVERAGE(O$4:O$6)</f>
+        <v>0.98562172652789837</v>
+      </c>
+      <c r="R80">
+        <f>AVERAGE(O$7:O$12,O$17:O$19)</f>
+        <v>0.97622736868249915</v>
+      </c>
+      <c r="S80">
+        <f>AVERAGE(O$13:O$16)</f>
+        <v>0.96792446357023321</v>
+      </c>
+      <c r="T80">
+        <f>O$20</f>
+        <v>0.99602689796079291</v>
+      </c>
+      <c r="U80">
+        <f>AVERAGE(O$21:O$22)</f>
+        <v>0.9939440085543001</v>
+      </c>
+    </row>
+    <row r="81" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P81">
+        <f>STDEV(O$1:O$3)/SQRT(COUNT(O$1:O$3))</f>
+        <v>7.903214212686805E-4</v>
+      </c>
+      <c r="Q81">
+        <f>STDEV(O$4:O$6)/SQRT(COUNT(O$4:O$6))</f>
+        <v>9.0723300721945472E-3</v>
+      </c>
+      <c r="R81">
+        <f>STDEV(O$7:O$12,O$17:O$19)/SQRT(COUNT(O$7:O$12,O$17:O$19))</f>
+        <v>1.2129818847755281E-2</v>
+      </c>
+      <c r="S81">
+        <f>STDEV(O$13:O$16)/SQRT(COUNT(O$13:O$16))</f>
+        <v>9.1385974951318887E-3</v>
+      </c>
+      <c r="U81">
+        <f>STDEV(O$21:O$22)/SQRT(COUNT(O$21:O$22))</f>
+        <v>1.5092714424497777E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="Q83" t="s">
+        <v>0</v>
+      </c>
+      <c r="R83" t="s">
+        <v>1</v>
+      </c>
+      <c r="S83" t="s">
+        <v>2</v>
+      </c>
+      <c r="T83" t="s">
+        <v>3</v>
+      </c>
+      <c r="U83" t="s">
+        <v>4</v>
+      </c>
+      <c r="V83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P84" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q84">
+        <f>AVERAGE(P$1:P$3)</f>
+        <v>8.2769960386286354E-2</v>
+      </c>
+      <c r="R84">
+        <f>AVERAGE(P$4:P$6)</f>
+        <v>8.1747176174903999E-2</v>
+      </c>
+      <c r="S84">
+        <f>AVERAGE(P$7:P$12,P$17:P$19)</f>
+        <v>9.6618096060557532E-2</v>
+      </c>
+      <c r="T84">
+        <f>AVERAGE(P$13:P$16)</f>
+        <v>8.0488259007867796E-2</v>
+      </c>
+      <c r="U84">
+        <f>P$20</f>
+        <v>0.11612890077785666</v>
+      </c>
+      <c r="V84">
+        <f>AVERAGE(P$21:P$22)</f>
+        <v>0.13277519443340902</v>
+      </c>
+    </row>
+    <row r="85" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="Q85">
+        <f>STDEV(P$1:P$3)/SQRT(COUNT(P$1:P$3))</f>
+        <v>6.1728202303740097E-3</v>
+      </c>
+      <c r="R85">
+        <f>STDEV(P$4:P$6)/SQRT(COUNT(P$4:P$6))</f>
+        <v>4.7620664425895532E-3</v>
+      </c>
+      <c r="S85">
+        <f>STDEV(P$7:P$12,P$17:P$19)/SQRT(COUNT(P$7:P$12,P$17:P$19))</f>
+        <v>1.5214270543208034E-2</v>
+      </c>
+      <c r="T85">
+        <f>STDEV(P$13:P$16)/SQRT(COUNT(P$13:P$16))</f>
+        <v>2.014243603928605E-2</v>
+      </c>
+      <c r="V85">
+        <f>STDEV(P$21:P$22)/SQRT(COUNT(P$21:P$22))</f>
+        <v>2.6130878673853903E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="R87" t="s">
+        <v>0</v>
+      </c>
+      <c r="S87" t="s">
+        <v>1</v>
+      </c>
+      <c r="T87" t="s">
+        <v>2</v>
+      </c>
+      <c r="U87" t="s">
+        <v>3</v>
+      </c>
+      <c r="V87" t="s">
+        <v>4</v>
+      </c>
+      <c r="W87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="Q88" t="s">
+        <v>15</v>
+      </c>
+      <c r="R88">
+        <f>AVERAGE(Q$1:Q$3)</f>
+        <v>0.12003209288401152</v>
+      </c>
+      <c r="S88">
+        <f>AVERAGE(Q$4:Q$6)</f>
+        <v>0.21343844914888963</v>
+      </c>
+      <c r="T88">
+        <f>AVERAGE(Q$7:Q$12,Q$17:Q$19)</f>
+        <v>0.21495956670453156</v>
+      </c>
+      <c r="U88">
+        <f>AVERAGE(Q$13:Q$16)</f>
+        <v>0.12579060832283959</v>
+      </c>
+      <c r="V88">
+        <f>Q$20</f>
+        <v>0.16359252591784523</v>
+      </c>
+      <c r="W88">
+        <f>AVERAGE(Q$21:Q$22)</f>
+        <v>0.22933142053717082</v>
+      </c>
+    </row>
+    <row r="89" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="R89">
+        <f>STDEV(Q$1:Q$3)/SQRT(COUNT(Q$1:Q$3))</f>
+        <v>2.9915209911607666E-2</v>
+      </c>
+      <c r="S89">
+        <f>STDEV(Q$4:Q$6)/SQRT(COUNT(Q$4:Q$6))</f>
+        <v>4.3580024502883882E-2</v>
+      </c>
+      <c r="T89">
+        <f>STDEV(Q$7:Q$12,Q$17:Q$19)/SQRT(COUNT(Q$7:Q$12,Q$17:Q$19))</f>
+        <v>4.9563045357193969E-2</v>
+      </c>
+      <c r="U89">
+        <f>STDEV(Q$13:Q$16)/SQRT(COUNT(Q$13:Q$16))</f>
+        <v>2.5182325466262E-2</v>
+      </c>
+      <c r="W89">
+        <f>STDEV(Q$21:Q$22)/SQRT(COUNT(Q$21:Q$22))</f>
+        <v>5.2445112898152908E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="S91" t="s">
+        <v>0</v>
+      </c>
+      <c r="T91" t="s">
+        <v>1</v>
+      </c>
+      <c r="U91" t="s">
+        <v>2</v>
+      </c>
+      <c r="V91" t="s">
+        <v>3</v>
+      </c>
+      <c r="W91" t="s">
+        <v>4</v>
+      </c>
+      <c r="X91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="R92" t="s">
+        <v>16</v>
+      </c>
+      <c r="S92">
+        <f>AVERAGE(R$1:R$3)</f>
+        <v>9.8876526846989221E-2</v>
+      </c>
+      <c r="T92">
+        <f>AVERAGE(R$4:R$6)</f>
+        <v>0.15989821775497828</v>
+      </c>
+      <c r="U92">
+        <f>AVERAGE(R$7:R$12,R$17:R$19)</f>
+        <v>0.1863577766352795</v>
+      </c>
+      <c r="V92">
+        <f>AVERAGE(R$13:R$16)</f>
+        <v>0.24531984414001679</v>
+      </c>
+      <c r="W92">
+        <f>R$20</f>
+        <v>0.10046394420079181</v>
+      </c>
+      <c r="X92">
+        <f>AVERAGE(R$21:R$22)</f>
+        <v>0.1111235379234371</v>
+      </c>
+    </row>
+    <row r="93" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="S93">
+        <f>STDEV(R$1:R$3)/SQRT(COUNT(R$1:R$3))</f>
+        <v>1.6225282641834871E-2</v>
+      </c>
+      <c r="T93">
+        <f>STDEV(R$4:R$6)/SQRT(COUNT(R$4:R$6))</f>
+        <v>4.7075848425480959E-2</v>
+      </c>
+      <c r="U93">
+        <f>STDEV(R$7:R$12,R$17:R$19)/SQRT(COUNT(R$7:R$12,R$17:R$19))</f>
+        <v>4.367031583618889E-2</v>
+      </c>
+      <c r="V93">
+        <f>STDEV(R$13:R$16)/SQRT(COUNT(R$13:R$16))</f>
+        <v>4.2744543922925191E-2</v>
+      </c>
+      <c r="X93">
+        <f>STDEV(R$21:R$22)/SQRT(COUNT(R$21:R$22))</f>
+        <v>1.5358734968358647E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="N23:W44">
+    <cfRule type="notContainsText" dxfId="1" priority="2" operator="notContains" text="Ok">
+      <formula>ISERROR(SEARCH("Ok",N23))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD23:AE44">
+    <cfRule type="notContainsText" dxfId="0" priority="1" operator="notContains" text="Ok">
+      <formula>ISERROR(SEARCH("Ok",AD23))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resetting repo results back to what they were before changing FL bounds to 0.01-0.5
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation_moredata.xlsx
+++ b/Lacex_summary_FinalConfirmation_moredata.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2325D539-0029-4FF1-85FF-B120A890ACDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BFFAC9-89A5-4BD0-825D-75787A35DFA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B075899B-8E8B-4489-B096-777C4BA97E2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="24">
   <si>
     <t>HK-2</t>
   </si>
@@ -104,90 +106,6 @@
   </si>
   <si>
     <t>Gamma</t>
-  </si>
-  <si>
-    <t>0.02 ± 0</t>
-  </si>
-  <si>
-    <t>0 ± 0</t>
-  </si>
-  <si>
-    <t>0.01 ± 0</t>
-  </si>
-  <si>
-    <t>0.03 ± 0.01</t>
-  </si>
-  <si>
-    <t>0.19 ± 0.03</t>
-  </si>
-  <si>
-    <t>0.11 ± 0.11</t>
-  </si>
-  <si>
-    <t>0.32 ± 0.22</t>
-  </si>
-  <si>
-    <t>0.14 ± 0.08</t>
-  </si>
-  <si>
-    <t>0.06 ± 0.02</t>
-  </si>
-  <si>
-    <t>0.05 ± 0.01</t>
-  </si>
-  <si>
-    <t>0.07 ± 0.02</t>
-  </si>
-  <si>
-    <t>1.71E-13 ± 1.49E-13</t>
-  </si>
-  <si>
-    <t>0.03 ± 0.03</t>
-  </si>
-  <si>
-    <t>0.02 ± 0.01</t>
-  </si>
-  <si>
-    <t>0.01 ± 0.01</t>
-  </si>
-  <si>
-    <t>0.15 ± 0.04</t>
-  </si>
-  <si>
-    <t>0.53 ± 0.07</t>
-  </si>
-  <si>
-    <t>0.24 ± 0.07</t>
-  </si>
-  <si>
-    <t>0.09 ± 0.03</t>
-  </si>
-  <si>
-    <t>0.03 ± 0</t>
-  </si>
-  <si>
-    <t>0.08 ± 0.02</t>
-  </si>
-  <si>
-    <t>0.4 ± 0.1</t>
-  </si>
-  <si>
-    <t>0.27 ± 0.07</t>
-  </si>
-  <si>
-    <t>0.26 ± 0.14</t>
-  </si>
-  <si>
-    <t>0.05 ± 0.05</t>
-  </si>
-  <si>
-    <t>9.33E-08 ± 9.33E-08</t>
-  </si>
-  <si>
-    <t>1.24E-06 ± 1.24E-06</t>
-  </si>
-  <si>
-    <t>8.19E-06 ± 8.19E-06</t>
   </si>
 </sst>
 </file>
@@ -347,16 +265,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.3632607711826903E-4</c:v>
+                    <c:v>1.3632467423976377E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.2769661600346282E-3</c:v>
+                    <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0184696395931343E-2</c:v>
+                    <c:v>1.0181144930654133E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.4460017690863679E-3</c:v>
+                    <c:v>9.1957167148318739E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -368,16 +286,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.3632607711826903E-4</c:v>
+                    <c:v>1.3632467423976377E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.2769661600346282E-3</c:v>
+                    <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0184696395931343E-2</c:v>
+                    <c:v>1.0181144930654133E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.4460017690863679E-3</c:v>
+                    <c:v>9.1957167148318739E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -423,16 +341,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.6597133043012298E-3</c:v>
+                  <c:v>3.6597166972760207E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3300064731281707E-2</c:v>
+                  <c:v>1.2969578710698102E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0904225837136496E-2</c:v>
+                  <c:v>3.9850373025406699E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7758110867901771E-3</c:v>
+                  <c:v>1.7436370403402304E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -701,16 +619,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>3.7887328106141906E-2</c:v>
+                    <c:v>3.7887236211488991E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.6912787197246887E-2</c:v>
+                    <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.984101299788778E-2</c:v>
+                    <c:v>0.34452837581693579</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.8964194893118057E-2</c:v>
+                    <c:v>0.44401386483779698</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -722,16 +640,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>3.7887328106141906E-2</c:v>
+                    <c:v>3.7887236211488991E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.6912787197246887E-2</c:v>
+                    <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.984101299788778E-2</c:v>
+                    <c:v>0.34452837581693579</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.8964194893118057E-2</c:v>
+                    <c:v>0.44401386483779698</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -777,16 +695,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.14700879061061764</c:v>
+                  <c:v>0.14700895503484715</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53211377816446115</c:v>
+                  <c:v>0.51874426073426694</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23593587790019413</c:v>
+                  <c:v>0.67733097633142481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.8135960815575995E-2</c:v>
+                  <c:v>0.55341627633490109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2134,6 +2052,114 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="27">
+          <cell r="C27" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="E27" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>kMCT4</v>
+          </cell>
+          <cell r="C28">
+            <v>9.2535545750464687E-2</v>
+          </cell>
+          <cell r="D28">
+            <v>0.3541415185008206</v>
+          </cell>
+          <cell r="E28">
+            <v>0.75444268232926348</v>
+          </cell>
+          <cell r="F28">
+            <v>0.16916415025152015</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>1.2057455739979463E-2</v>
+          </cell>
+          <cell r="D29">
+            <v>5.7309495294150879E-2</v>
+          </cell>
+          <cell r="E29">
+            <v>0.39928208436858398</v>
+          </cell>
+          <cell r="F29">
+            <v>0.13741088889033834</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="D31" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="E31" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="F31" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="G31" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32" t="str">
+            <v>R1L</v>
+          </cell>
+          <cell r="D32">
+            <v>7.384890314233869E-2</v>
+          </cell>
+          <cell r="E32">
+            <v>5.0263555960985945E-2</v>
+          </cell>
+          <cell r="F32">
+            <v>6.3109847044927683E-2</v>
+          </cell>
+          <cell r="G32">
+            <v>8.0357873156810505E-2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="D33">
+            <v>2.3803754511435734E-2</v>
+          </cell>
+          <cell r="E33">
+            <v>2.3947765296666392E-2</v>
+          </cell>
+          <cell r="F33">
+            <v>1.0466686942143609E-2</v>
+          </cell>
+          <cell r="G33">
+            <v>1.4625933793160245E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2431,11 +2457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5426EC7D-B74E-4953-AA3A-EC81D60A2FE4}">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57:M57"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,10 +2470,10 @@
         <v>2.0781114759556379E-2</v>
       </c>
       <c r="B1">
-        <v>3.4795160765735142E-3</v>
+        <v>3.4795161265732725E-3</v>
       </c>
       <c r="C1">
-        <v>0.12115537052459717</v>
+        <v>0.12115537047460399</v>
       </c>
       <c r="D1">
         <v>3.5353019394421974E-2</v>
@@ -2457,16 +2482,16 @@
         <v>2.2204460492503131E-14</v>
       </c>
       <c r="F1">
-        <v>0.22199754974964128</v>
+        <v>0.22199757443326015</v>
       </c>
       <c r="G1">
-        <v>2.6690613833378639E-2</v>
+        <v>2.670202489455735E-2</v>
       </c>
       <c r="H1">
-        <v>0.1193284328924214</v>
+        <v>0.1193170263614496</v>
       </c>
       <c r="I1">
-        <v>0.14112981277088579</v>
+        <v>0.1411298456931295</v>
       </c>
       <c r="J1">
         <v>2.356211808499348</v>
@@ -2478,22 +2503,22 @@
         <v>254686091.39268142</v>
       </c>
       <c r="M1">
-        <v>0.99715195462511397</v>
+        <v>0.99715195462511363</v>
       </c>
       <c r="N1">
-        <v>0.99785346972164479</v>
+        <v>0.99785346972528499</v>
       </c>
       <c r="O1">
-        <v>0.99488532530889628</v>
+        <v>0.99488532535510454</v>
       </c>
       <c r="P1">
-        <v>7.6353436469702857E-2</v>
+        <v>7.6353436469702843E-2</v>
       </c>
       <c r="Q1">
-        <v>6.5139118627818918E-2</v>
+        <v>6.5139118584084318E-2</v>
       </c>
       <c r="R1">
-        <v>0.13102591924998203</v>
+        <v>0.13102591930261462</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -2501,28 +2526,28 @@
         <v>1.9731495213395425E-2</v>
       </c>
       <c r="B2">
-        <v>3.9270155220979732E-3</v>
+        <v>3.9270147990883662E-3</v>
       </c>
       <c r="C2">
-        <v>0.21794698510467292</v>
+        <v>0.21794698582814859</v>
       </c>
       <c r="D2">
         <v>0.10099996196568557</v>
       </c>
       <c r="E2">
-        <v>4.7034496087961561E-13</v>
+        <v>2.2205996670362198E-14</v>
       </c>
       <c r="F2">
-        <v>0.11894114935080123</v>
+        <v>0.11894110934795486</v>
       </c>
       <c r="G2">
-        <v>2.664110113072218E-2</v>
+        <v>2.6561340578606808E-2</v>
       </c>
       <c r="H2">
-        <v>4.8217942224329242E-2</v>
+        <v>4.8297651990673832E-2</v>
       </c>
       <c r="I2">
-        <v>2.220559544695324E-14</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="J2">
         <v>5.6114128380547523</v>
@@ -2534,22 +2559,22 @@
         <v>161047158.1115168</v>
       </c>
       <c r="M2">
-        <v>0.99709416769265724</v>
+        <v>0.99709416769265702</v>
       </c>
       <c r="N2">
-        <v>0.98619132463554471</v>
+        <v>0.98619132265690701</v>
       </c>
       <c r="O2">
-        <v>0.996892042958339</v>
+        <v>0.99689204548862798</v>
       </c>
       <c r="P2">
-        <v>7.6844094339646438E-2</v>
+        <v>7.6844094339646424E-2</v>
       </c>
       <c r="Q2">
-        <v>0.1680899816948194</v>
+        <v>0.16808999389977516</v>
       </c>
       <c r="R2">
-        <v>7.8981935377848367E-2</v>
+        <v>7.8981907325062134E-2</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -2557,28 +2582,28 @@
         <v>2.0365465865092722E-2</v>
       </c>
       <c r="B3">
-        <v>3.5726083142322011E-3</v>
+        <v>3.5726191661664243E-3</v>
       </c>
       <c r="C3">
-        <v>0.23160371771812638</v>
+        <v>0.23160370685789064</v>
       </c>
       <c r="D3">
         <v>4.2510089797902627E-2</v>
       </c>
       <c r="E3">
-        <v>2.2215821287872737E-14</v>
+        <v>2.2219642502235133E-14</v>
       </c>
       <c r="F3">
-        <v>0.10008767273141045</v>
+        <v>0.10008818132332642</v>
       </c>
       <c r="G3">
-        <v>2.6672811045030269E-2</v>
+        <v>2.6572920741034615E-2</v>
       </c>
       <c r="H3">
-        <v>6.003748527936624E-2</v>
+        <v>6.0138209620568157E-2</v>
       </c>
       <c r="I3">
-        <v>2.2223963563717064E-14</v>
+        <v>2.2230487406924265E-14</v>
       </c>
       <c r="J3">
         <v>2.8545008818278075</v>
@@ -2590,22 +2615,22 @@
         <v>491427690.54543257</v>
       </c>
       <c r="M3">
-        <v>0.99564380003669684</v>
+        <v>0.99564380003670339</v>
       </c>
       <c r="N3">
-        <v>0.99195331473946191</v>
+        <v>0.99195335998266976</v>
       </c>
       <c r="O3">
-        <v>0.99750161606307208</v>
+        <v>0.9975015329873631</v>
       </c>
       <c r="P3">
-        <v>9.5112350349510072E-2</v>
+        <v>9.5112350349509781E-2</v>
       </c>
       <c r="Q3">
-        <v>0.12686753230657891</v>
+        <v>0.12686716616817512</v>
       </c>
       <c r="R3">
-        <v>8.662068991569144E-2</v>
+        <v>8.6621753913290897E-2</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -2613,28 +2638,28 @@
         <v>1.9994972552697242E-2</v>
       </c>
       <c r="B4">
-        <v>1.1428957242739431E-2</v>
+        <v>8.2261049334318315E-3</v>
       </c>
       <c r="C4">
-        <v>4.6201953210387075E-3</v>
+        <v>7.8238786162331871E-3</v>
       </c>
       <c r="D4">
-        <v>4.1710389111108179E-2</v>
+        <v>4.1448382824856529E-2</v>
       </c>
       <c r="E4">
-        <v>4.3470861867194528E-6</v>
+        <v>8.4517983628408446E-7</v>
       </c>
       <c r="F4">
-        <v>0.57037919412157423</v>
+        <v>0.38417933083549277</v>
       </c>
       <c r="G4">
-        <v>2.8011204464739852E-2</v>
+        <v>2.801117129673817E-2</v>
       </c>
       <c r="H4">
-        <v>0.49999996831517102</v>
+        <v>0.30888130275024206</v>
       </c>
       <c r="I4">
-        <v>3.4402918055781228E-14</v>
+        <v>4.1254209297634721E-14</v>
       </c>
       <c r="J4">
         <v>5.740537779224173</v>
@@ -2646,22 +2671,22 @@
         <v>142097848.58194768</v>
       </c>
       <c r="M4">
-        <v>0.99706209855722094</v>
+        <v>0.99706208406329411</v>
       </c>
       <c r="N4">
-        <v>0.95883234223505442</v>
+        <v>0.95451182918462252</v>
       </c>
       <c r="O4">
-        <v>0.97779071715475974</v>
+        <v>0.96755342148890255</v>
       </c>
       <c r="P4">
-        <v>7.846580057922635E-2</v>
+        <v>7.8465803659368477E-2</v>
       </c>
       <c r="Q4">
-        <v>0.28475806421751526</v>
+        <v>0.29835113413949227</v>
       </c>
       <c r="R4">
-        <v>0.21412326557080974</v>
+        <v>0.25391303933089066</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
@@ -2696,28 +2721,28 @@
         <v>2.023647882476649E-2</v>
       </c>
       <c r="B5">
-        <v>1.574099062102436E-2</v>
+        <v>1.7952384844695909E-2</v>
       </c>
       <c r="C5">
-        <v>0.32892928351956346</v>
+        <v>0.32513897643519724</v>
       </c>
       <c r="D5">
-        <v>9.2481989463721506E-2</v>
+        <v>9.267293693911316E-2</v>
       </c>
       <c r="E5">
-        <v>7.6041037030782729E-2</v>
+        <v>3.37910782375764E-14</v>
       </c>
       <c r="F5">
-        <v>0.62403863061172127</v>
+        <v>0.77012992110925338</v>
       </c>
       <c r="G5">
-        <v>2.7998968097937872E-2</v>
+        <v>2.6757739839081779E-2</v>
       </c>
       <c r="H5">
-        <v>0.49607216299812229</v>
+        <v>0.67099227523245808</v>
       </c>
       <c r="I5">
-        <v>2.799251060401586E-7</v>
+        <v>4.1482880168662724E-14</v>
       </c>
       <c r="J5">
         <v>3.2019451544874276</v>
@@ -2729,22 +2754,22 @@
         <v>629017289.17440271</v>
       </c>
       <c r="M5">
-        <v>0.99609218906723862</v>
+        <v>0.99609224845038047</v>
       </c>
       <c r="N5">
-        <v>0.9819920857404878</v>
+        <v>0.98228022729653697</v>
       </c>
       <c r="O5">
-        <v>0.99365010508655915</v>
+        <v>0.99321581530579128</v>
       </c>
       <c r="P5">
-        <v>9.1133685204087059E-2</v>
+        <v>9.1131006252957447E-2</v>
       </c>
       <c r="Q5">
-        <v>0.19404583817298404</v>
+        <v>0.18801244877525125</v>
       </c>
       <c r="R5">
-        <v>0.11610503576133344</v>
+        <v>0.11728586191248075</v>
       </c>
       <c r="T5" s="1">
         <f>1/51</f>
@@ -2785,28 +2810,28 @@
         <v>2.0231218059161282E-2</v>
       </c>
       <c r="B6">
-        <v>1.2730246330081329E-2</v>
+        <v>1.2730246353966567E-2</v>
       </c>
       <c r="C6">
-        <v>1.0000022204460493E-8</v>
+        <v>1.0000022208952447E-8</v>
       </c>
       <c r="D6">
-        <v>4.1159362977100808E-2</v>
+        <v>4.1159362974046244E-2</v>
       </c>
       <c r="E6">
-        <v>2.2204908402536481E-14</v>
+        <v>2.2215914010445092E-14</v>
       </c>
       <c r="F6">
-        <v>0.401923509760088</v>
+        <v>0.40192353025805466</v>
       </c>
       <c r="G6">
-        <v>2.7068787848909991E-2</v>
+        <v>2.7650327011609629E-2</v>
       </c>
       <c r="H6">
-        <v>0.19426552401571529</v>
+        <v>0.19368398855284627</v>
       </c>
       <c r="I6">
-        <v>2.220465849625446E-14</v>
+        <v>2.2237737766946569E-14</v>
       </c>
       <c r="J6">
         <v>4.8009905427717481</v>
@@ -2818,22 +2843,22 @@
         <v>149956135.49829885</v>
       </c>
       <c r="M6">
-        <v>0.99720075071843151</v>
+        <v>0.99720075071810876</v>
       </c>
       <c r="N6">
-        <v>0.98945232733318678</v>
+        <v>0.98945232763408242</v>
       </c>
       <c r="O6">
-        <v>0.99609594268036072</v>
+        <v>0.99609594278900127</v>
       </c>
       <c r="P6">
-        <v>7.5644718612184608E-2</v>
+        <v>7.5644718612386044E-2</v>
       </c>
       <c r="Q6">
-        <v>0.15395176347094605</v>
+        <v>0.1539517645319253</v>
       </c>
       <c r="R6">
-        <v>0.108495752828278</v>
+        <v>0.10849575202156349</v>
       </c>
       <c r="T6" s="1">
         <f>1/47</f>
@@ -2871,10 +2896,10 @@
         <v>2.0352218032308276E-2</v>
       </c>
       <c r="B7">
-        <v>1.133638073871621E-2</v>
+        <v>1.1336378651585302E-2</v>
       </c>
       <c r="C7">
-        <v>1.6568059747632265E-2</v>
+        <v>1.6568061839038396E-2</v>
       </c>
       <c r="D7">
         <v>4.5873244781070611E-2</v>
@@ -2883,16 +2908,16 @@
         <v>2.2204460492503131E-14</v>
       </c>
       <c r="F7">
-        <v>7.6265666547093658E-2</v>
+        <v>7.6265635306323493E-2</v>
       </c>
       <c r="G7">
-        <v>2.7725091771904645E-2</v>
+        <v>2.7659978894551168E-2</v>
       </c>
       <c r="H7">
-        <v>9.8468216971801567E-2</v>
+        <v>9.8533251240757375E-2</v>
       </c>
       <c r="I7">
-        <v>2.2204725434828872E-14</v>
+        <v>2.2204979238374094E-14</v>
       </c>
       <c r="J7">
         <v>1.952898836424503</v>
@@ -2904,22 +2929,22 @@
         <v>132744891.08503906</v>
       </c>
       <c r="M7">
-        <v>0.99900216768483063</v>
+        <v>0.99900216768483463</v>
       </c>
       <c r="N7">
-        <v>0.99812720801648736</v>
+        <v>0.99812720704547231</v>
       </c>
       <c r="O7">
-        <v>0.99659961836433864</v>
+        <v>0.9965996225501188</v>
       </c>
       <c r="P7">
-        <v>4.4448064950345249E-2</v>
+        <v>4.4448064950350752E-2</v>
       </c>
       <c r="Q7">
-        <v>6.3844913090838437E-2</v>
+        <v>6.3844926603594698E-2</v>
       </c>
       <c r="R7">
-        <v>9.123190692841987E-2</v>
+        <v>9.123185443573037E-2</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -2927,28 +2952,28 @@
         <v>2.0420572162940933E-2</v>
       </c>
       <c r="B8">
-        <v>2.2011934508948738E-2</v>
+        <v>2.8455085625926618E-2</v>
       </c>
       <c r="C8">
-        <v>0.20827938762371043</v>
+        <v>0.19463910134944526</v>
       </c>
       <c r="D8">
-        <v>6.5007089336341681E-2</v>
+        <v>6.5007089083382458E-2</v>
       </c>
       <c r="E8">
-        <v>8.9208067474833064E-2</v>
+        <v>2.4898037270932147E-3</v>
       </c>
       <c r="F8">
-        <v>7.660170543363902E-2</v>
+        <v>0.23965150048870829</v>
       </c>
       <c r="G8">
-        <v>2.6872161981565137E-2</v>
+        <v>2.7079786776221599E-2</v>
       </c>
       <c r="H8">
-        <v>0.12440865192396866</v>
+        <v>0.57170256654956031</v>
       </c>
       <c r="I8">
-        <v>2.2204570531824728E-14</v>
+        <v>9.941866654942422E-7</v>
       </c>
       <c r="J8">
         <v>2.4430206679346318</v>
@@ -2960,22 +2985,22 @@
         <v>457955160.74923623</v>
       </c>
       <c r="M8">
-        <v>0.99838221935488858</v>
+        <v>0.99837928576034285</v>
       </c>
       <c r="N8">
-        <v>0.9973488546160052</v>
+        <v>0.99840550035107978</v>
       </c>
       <c r="O8">
-        <v>0.99710079863989232</v>
+        <v>0.97812854760325485</v>
       </c>
       <c r="P8">
-        <v>5.7537209678967305E-2</v>
+        <v>5.751194069035951E-2</v>
       </c>
       <c r="Q8">
-        <v>7.2381879490547474E-2</v>
+        <v>5.6148136508280842E-2</v>
       </c>
       <c r="R8">
-        <v>7.7702565550152647E-2</v>
+        <v>0.21109361441809982</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -2983,28 +3008,28 @@
         <v>1.9856607624304978E-2</v>
       </c>
       <c r="B9">
-        <v>5.5954517550855804E-3</v>
+        <v>6.9060525830266173E-2</v>
       </c>
       <c r="C9">
-        <v>0.3229822326411822</v>
+        <v>0.25801108459089117</v>
       </c>
       <c r="D9">
-        <v>7.4905465924434506E-2</v>
+        <v>7.4230058620422631E-2</v>
       </c>
       <c r="E9">
-        <v>9.9999999999977801E-2</v>
+        <v>2.9250814687839763E-14</v>
       </c>
       <c r="F9">
-        <v>0.18965559004345928</v>
+        <v>3.2253352307515293</v>
       </c>
       <c r="G9">
-        <v>2.801120448177051E-2</v>
+        <v>2.8011204478663298E-2</v>
       </c>
       <c r="H9">
-        <v>0.4999999999999778</v>
+        <v>9.750654659613712</v>
       </c>
       <c r="I9">
-        <v>2.2204844847856116E-14</v>
+        <v>8.9507003447047568E-9</v>
       </c>
       <c r="J9">
         <v>4.3363113643580764</v>
@@ -3016,22 +3041,22 @@
         <v>1205583684.8478703</v>
       </c>
       <c r="M9">
-        <v>0.99455790128187005</v>
+        <v>0.99455792352757189</v>
       </c>
       <c r="N9">
-        <v>0.94817760365235948</v>
+        <v>0.95888050748856335</v>
       </c>
       <c r="O9">
-        <v>0.96634777842910735</v>
+        <v>0.98176164041495118</v>
       </c>
       <c r="P9">
-        <v>0.10398825524888045</v>
+        <v>0.10398649260370561</v>
       </c>
       <c r="Q9">
-        <v>0.32856276942112639</v>
+        <v>0.29760772423271709</v>
       </c>
       <c r="R9">
-        <v>0.27231147818537682</v>
+        <v>0.19874222923660653</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -3039,28 +3064,28 @@
         <v>1.9607843138025917E-2</v>
       </c>
       <c r="B10">
-        <v>5.3909028768448679E-3</v>
+        <v>1.2323139929023586E-2</v>
       </c>
       <c r="C10">
-        <v>2.2521113960106455E-2</v>
+        <v>1.5598276110641449E-2</v>
       </c>
       <c r="D10">
-        <v>6.2210612234105268E-2</v>
+        <v>6.230835978644024E-2</v>
       </c>
       <c r="E10">
-        <v>4.4302630861675838E-14</v>
+        <v>1.0730907695642397E-3</v>
       </c>
       <c r="F10">
-        <v>0.53522268695722675</v>
+        <v>1.2599420336012488</v>
       </c>
       <c r="G10">
-        <v>2.8011204481765768E-2</v>
+        <v>2.7334357934778661E-2</v>
       </c>
       <c r="H10">
-        <v>0.49999999999997308</v>
+        <v>1.4553538898315348</v>
       </c>
       <c r="I10">
-        <v>1.120653752485981E-5</v>
+        <v>4.0807233768722193E-14</v>
       </c>
       <c r="J10">
         <v>3.6193816110419976</v>
@@ -3072,22 +3097,22 @@
         <v>83209857.156356871</v>
       </c>
       <c r="M10">
-        <v>0.9966826809852054</v>
+        <v>0.99668267063118265</v>
       </c>
       <c r="N10">
-        <v>0.98688246658357237</v>
+        <v>0.98967172348163557</v>
       </c>
       <c r="O10">
-        <v>0.99481961344349834</v>
+        <v>0.99072332294345355</v>
       </c>
       <c r="P10">
-        <v>8.1022431760208027E-2</v>
+        <v>8.1022592759074114E-2</v>
       </c>
       <c r="Q10">
-        <v>0.16855659356558364</v>
+        <v>0.1457665294218416</v>
       </c>
       <c r="R10">
-        <v>0.13298570171434937</v>
+        <v>0.13578312841773169</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -3095,28 +3120,28 @@
         <v>1.9607868588388273E-2</v>
       </c>
       <c r="B11">
-        <v>1.7638601406568435E-2</v>
+        <v>1.601888853618769E-2</v>
       </c>
       <c r="C11">
-        <v>0.16260666761405404</v>
+        <v>0.1641584912521373</v>
       </c>
       <c r="D11">
-        <v>4.4242338708686456E-2</v>
+        <v>4.5283825219602628E-2</v>
       </c>
       <c r="E11">
-        <v>8.7429511035403882E-4</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F11">
-        <v>0.13249062043267457</v>
+        <v>0.11219420894660005</v>
       </c>
       <c r="G11">
-        <v>2.7212493461733569E-2</v>
+        <v>2.6739389223432025E-2</v>
       </c>
       <c r="H11">
-        <v>0.24297878803639783</v>
+        <v>0.19245141659030984</v>
       </c>
       <c r="I11">
-        <v>1.4590149912989482E-8</v>
+        <v>2.2206781588809361E-14</v>
       </c>
       <c r="J11">
         <v>2.8612100103634148</v>
@@ -3128,22 +3153,22 @@
         <v>44059879.020455331</v>
       </c>
       <c r="M11">
-        <v>0.99213811697012155</v>
+        <v>0.99213822043396482</v>
       </c>
       <c r="N11">
-        <v>0.99429763683120853</v>
+        <v>0.99410838184506134</v>
       </c>
       <c r="O11">
-        <v>0.99178266419674876</v>
+        <v>0.99319548348425291</v>
       </c>
       <c r="P11">
-        <v>0.12447004841661347</v>
+        <v>0.12446931357457527</v>
       </c>
       <c r="Q11">
-        <v>0.11612419352381233</v>
+        <v>0.11716632920010855</v>
       </c>
       <c r="R11">
-        <v>0.1575783799105851</v>
+        <v>0.14608669072309458</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -3151,28 +3176,28 @@
         <v>1.9955136692618142E-2</v>
       </c>
       <c r="B12">
-        <v>7.9999999999960353E-2</v>
+        <v>7.9999999969555299E-2</v>
       </c>
       <c r="C12">
-        <v>2.0255250917328227</v>
+        <v>2.025498154431006</v>
       </c>
       <c r="D12">
-        <v>3.7430807982119514E-2</v>
+        <v>3.7430807982120715E-2</v>
       </c>
       <c r="E12">
-        <v>1.7089976663320057E-11</v>
+        <v>4.813190262085224E-11</v>
       </c>
       <c r="F12">
-        <v>0.17802177286522836</v>
+        <v>0.17802513032889813</v>
       </c>
       <c r="G12">
-        <v>2.7590873656651516E-2</v>
+        <v>2.6557682885802104E-2</v>
       </c>
       <c r="H12">
-        <v>0.37264777222187589</v>
+        <v>0.37369127504783234</v>
       </c>
       <c r="I12">
-        <v>4.1323741019457654E-14</v>
+        <v>4.2438187820793242E-14</v>
       </c>
       <c r="J12">
         <v>5.3408895358905601</v>
@@ -3184,22 +3209,22 @@
         <v>1300249383.1199305</v>
       </c>
       <c r="M12">
-        <v>0.97974716394439265</v>
+        <v>0.97974716357598268</v>
       </c>
       <c r="N12">
-        <v>0.92111121563310538</v>
+        <v>0.92111167361335022</v>
       </c>
       <c r="O12">
-        <v>0.9665480468369112</v>
+        <v>0.96654862729160018</v>
       </c>
       <c r="P12">
-        <v>0.20055742380615996</v>
+        <v>0.20055742706207924</v>
       </c>
       <c r="Q12">
-        <v>0.38893081733581075</v>
+        <v>0.38892998015242602</v>
       </c>
       <c r="R12">
-        <v>0.25542133591577271</v>
+        <v>0.25541943931821498</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -3207,28 +3232,28 @@
         <v>1.9932134010064936E-2</v>
       </c>
       <c r="B13">
-        <v>8.8663051236494411E-3</v>
+        <v>8.6403546782031753E-3</v>
       </c>
       <c r="C13">
-        <v>6.9789982564623335E-2</v>
+        <v>6.9996504707704105E-2</v>
       </c>
       <c r="D13">
-        <v>4.1899008128684898E-2</v>
+        <v>4.117029077902333E-2</v>
       </c>
       <c r="E13">
-        <v>5.3283819570849964E-4</v>
+        <v>5.5774294888870558E-10</v>
       </c>
       <c r="F13">
-        <v>0.15196902534763565</v>
+        <v>0.14710121465685502</v>
       </c>
       <c r="G13">
-        <v>2.801120448177051E-2</v>
+        <v>2.7606148348276426E-2</v>
       </c>
       <c r="H13">
-        <v>0.4999999999999778</v>
+        <v>0.48172107020411004</v>
       </c>
       <c r="I13">
-        <v>2.2204676522351301E-14</v>
+        <v>3.1310055328609909E-14</v>
       </c>
       <c r="J13">
         <v>4.079138265678818</v>
@@ -3240,22 +3265,22 @@
         <v>566450101.24093688</v>
       </c>
       <c r="M13">
-        <v>0.99898531956302528</v>
+        <v>0.99898533074451068</v>
       </c>
       <c r="N13">
-        <v>0.99719326369820838</v>
+        <v>0.99701139548014506</v>
       </c>
       <c r="O13">
-        <v>0.94788871172308053</v>
+        <v>0.949541110127199</v>
       </c>
       <c r="P13">
-        <v>4.4816025560176276E-2</v>
+        <v>4.4815903611969979E-2</v>
       </c>
       <c r="Q13">
-        <v>8.0275869056076282E-2</v>
+        <v>8.2400008207427697E-2</v>
       </c>
       <c r="R13">
-        <v>0.33032427339876697</v>
+        <v>0.32512088803992523</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -3263,28 +3288,28 @@
         <v>1.9701617767527744E-2</v>
       </c>
       <c r="B14">
-        <v>4.735933099338758E-3</v>
+        <v>4.8323620306448935E-3</v>
       </c>
       <c r="C14">
-        <v>5.5526300970527151E-3</v>
+        <v>5.4563962150907331E-3</v>
       </c>
       <c r="D14">
-        <v>4.0167045159102244E-2</v>
+        <v>4.0812904702452656E-2</v>
       </c>
       <c r="E14">
-        <v>6.7413238629853802E-6</v>
+        <v>1.7651220104339856E-5</v>
       </c>
       <c r="F14">
-        <v>2.9837576852025954E-2</v>
+        <v>3.1617351973594027E-2</v>
       </c>
       <c r="G14">
-        <v>2.7276452469382397E-2</v>
+        <v>2.725000798928098E-2</v>
       </c>
       <c r="H14">
-        <v>3.82087883020314E-2</v>
+        <v>4.7124138988605048E-2</v>
       </c>
       <c r="I14">
-        <v>3.279043328633545E-5</v>
+        <v>1.6211893547391038E-5</v>
       </c>
       <c r="J14">
         <v>4.5658015908569123</v>
@@ -3296,22 +3321,22 @@
         <v>350999697.1980691</v>
       </c>
       <c r="M14">
-        <v>0.99208182662321498</v>
+        <v>0.99208181807768536</v>
       </c>
       <c r="N14">
-        <v>0.99496241651027384</v>
+        <v>0.99508377256621872</v>
       </c>
       <c r="O14">
-        <v>0.99332667787179918</v>
+        <v>0.99253225813286505</v>
       </c>
       <c r="P14">
-        <v>0.12573156715291495</v>
+        <v>0.12573170714751689</v>
       </c>
       <c r="Q14">
-        <v>0.10334460087098453</v>
+        <v>0.10237015179103715</v>
       </c>
       <c r="R14">
-        <v>0.12382743988360392</v>
+        <v>0.12637696756741412</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -3319,28 +3344,28 @@
         <v>1.9647451233942632E-2</v>
       </c>
       <c r="B15">
-        <v>9.627872075642651E-3</v>
+        <v>1.1560450572118007E-2</v>
       </c>
       <c r="C15">
-        <v>8.904700151440266E-2</v>
+        <v>8.4848356183085338E-2</v>
       </c>
       <c r="D15">
-        <v>8.8738460064248847E-2</v>
+        <v>8.8738451615117273E-2</v>
       </c>
       <c r="E15">
-        <v>5.6390836241633498E-2</v>
+        <v>2.407360763413255E-14</v>
       </c>
       <c r="F15">
-        <v>4.9463070926385501E-2</v>
+        <v>0.15210747569666191</v>
       </c>
       <c r="G15">
-        <v>2.6548648767190847E-2</v>
+        <v>2.6611480178405034E-2</v>
       </c>
       <c r="H15">
-        <v>1.7732417872616674E-2</v>
+        <v>0.22793467277447976</v>
       </c>
       <c r="I15">
-        <v>2.2204465470219053E-14</v>
+        <v>3.8305931461935391E-14</v>
       </c>
       <c r="J15">
         <v>6.1031742274447058</v>
@@ -3352,22 +3377,22 @@
         <v>621934179.43162954</v>
       </c>
       <c r="M15">
-        <v>0.99881950192927693</v>
+        <v>0.99882163160938198</v>
       </c>
       <c r="N15">
-        <v>0.99064358089077498</v>
+        <v>0.99270388667667397</v>
       </c>
       <c r="O15">
-        <v>0.99551992042118576</v>
+        <v>0.96037915720805644</v>
       </c>
       <c r="P15">
-        <v>4.8333595573126678E-2</v>
+        <v>4.8286264033468369E-2</v>
       </c>
       <c r="Q15">
-        <v>0.13658324492493817</v>
+        <v>0.12081206714507217</v>
       </c>
       <c r="R15">
-        <v>9.4634390024914791E-2</v>
+        <v>0.28282810134363656</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -3375,28 +3400,28 @@
         <v>2.0254106371624593E-2</v>
       </c>
       <c r="B16">
-        <v>3.8731340485298588E-3</v>
+        <v>4.4712314332643145E-2</v>
       </c>
       <c r="C16">
-        <v>0.37949424762133072</v>
+        <v>0.33865466146936779</v>
       </c>
       <c r="D16">
-        <v>0.10027579446100324</v>
+        <v>0.10027579446083579</v>
       </c>
       <c r="E16">
         <v>2.2204460492503131E-14</v>
       </c>
       <c r="F16">
-        <v>0.12127417013625687</v>
+        <v>1.8828390630124936</v>
       </c>
       <c r="G16">
-        <v>2.801120448177051E-2</v>
+        <v>2.8011204481770472E-2</v>
       </c>
       <c r="H16">
-        <v>0.4999999999999778</v>
+        <v>9.9999999999999787</v>
       </c>
       <c r="I16">
-        <v>2.2205263256223658E-14</v>
+        <v>4.8819468832966442E-10</v>
       </c>
       <c r="J16">
         <v>2.8975994027540488</v>
@@ -3408,22 +3433,22 @@
         <v>818269300.73777747</v>
       </c>
       <c r="M16">
-        <v>0.99463967391501673</v>
+        <v>0.99463967383988361</v>
       </c>
       <c r="N16">
-        <v>0.97424382005487198</v>
+        <v>0.985550803068721</v>
       </c>
       <c r="O16">
-        <v>0.98436713326261316</v>
+        <v>0.96924532881281233</v>
       </c>
       <c r="P16">
-        <v>0.1031191612427458</v>
+        <v>0.10311916123851592</v>
       </c>
       <c r="Q16">
-        <v>0.24610388964834184</v>
+        <v>0.19758020614782132</v>
       </c>
       <c r="R16">
-        <v>0.25587347166347341</v>
+        <v>0.24695341960909117</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -3431,28 +3456,28 @@
         <v>2.0450312385911232E-2</v>
       </c>
       <c r="B17">
-        <v>9.3435261466663418E-3</v>
+        <v>8.923362709430319E-3</v>
       </c>
       <c r="C17">
-        <v>1.1050788296480039E-3</v>
+        <v>1.5268678764787176E-3</v>
       </c>
       <c r="D17">
-        <v>4.2219008518471456E-2</v>
+        <v>4.1485128594566129E-2</v>
       </c>
       <c r="E17">
-        <v>2.2204588180832684E-14</v>
+        <v>5.0322381980571912E-5</v>
       </c>
       <c r="F17">
-        <v>0.21221492107704915</v>
+        <v>0.20035088574662624</v>
       </c>
       <c r="G17">
-        <v>2.6760248590911362E-2</v>
+        <v>2.8011204470866559E-2</v>
       </c>
       <c r="H17">
-        <v>8.9677025204365712E-2</v>
+        <v>7.8836529817834081E-2</v>
       </c>
       <c r="I17">
-        <v>2.22054794874069E-14</v>
+        <v>4.4177389542715639E-14</v>
       </c>
       <c r="J17">
         <v>4.9944093087717132</v>
@@ -3464,22 +3489,22 @@
         <v>87097810.529802099</v>
       </c>
       <c r="M17">
-        <v>0.99683911484762233</v>
+        <v>0.99683910813226995</v>
       </c>
       <c r="N17">
-        <v>0.98740154063546326</v>
+        <v>0.9867659528053907</v>
       </c>
       <c r="O17">
-        <v>0.99844606998034513</v>
+        <v>0.99860625939314263</v>
       </c>
       <c r="P17">
-        <v>8.2129029009649773E-2</v>
+        <v>8.2129228260778453E-2</v>
       </c>
       <c r="Q17">
-        <v>0.16423504579605921</v>
+        <v>0.16814307852940949</v>
       </c>
       <c r="R17">
-        <v>7.187643535224883E-2</v>
+        <v>6.8346251598520716E-2</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -3487,28 +3512,28 @@
         <v>1.9778014887334602E-2</v>
       </c>
       <c r="B18">
-        <v>4.6821235101460149E-2</v>
+        <v>5.2535975976707519E-2</v>
       </c>
       <c r="C18">
-        <v>0.12780437785006987</v>
+        <v>0.12208854799275491</v>
       </c>
       <c r="D18">
         <v>7.614398766366591E-2</v>
       </c>
       <c r="E18">
-        <v>2.3680712807817982E-14</v>
+        <v>2.2204554673015353E-14</v>
       </c>
       <c r="F18">
-        <v>0.64648816291184541</v>
+        <v>0.72928382779249157</v>
       </c>
       <c r="G18">
-        <v>2.8011204481770465E-2</v>
+        <v>2.7631055008154236E-2</v>
       </c>
       <c r="H18">
-        <v>0.49999999999997041</v>
+        <v>0.57990303234465335</v>
       </c>
       <c r="I18">
-        <v>2.2204460492503131E-14</v>
+        <v>2.2204460492503134E-14</v>
       </c>
       <c r="J18">
         <v>3.2428732950368784</v>
@@ -3520,22 +3545,22 @@
         <v>776346501.63544285</v>
       </c>
       <c r="M18">
-        <v>0.99704775638282817</v>
+        <v>0.99704775731930395</v>
       </c>
       <c r="N18">
-        <v>0.97804795074433337</v>
+        <v>0.97850365971070608</v>
       </c>
       <c r="O18">
-        <v>0.99732824936063724</v>
+        <v>0.99708218383603886</v>
       </c>
       <c r="P18">
-        <v>7.8493394029665139E-2</v>
+        <v>7.8493392353228289E-2</v>
       </c>
       <c r="Q18">
-        <v>0.21006903537952973</v>
+        <v>0.20798423390640772</v>
       </c>
       <c r="R18">
-        <v>7.6059156886082557E-2</v>
+        <v>7.9032400824502233E-2</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -3546,25 +3571,25 @@
         <v>7.9999999999977797E-2</v>
       </c>
       <c r="C19">
-        <v>6.0470131252492688E-3</v>
+        <v>8.4733543146847997E-3</v>
       </c>
       <c r="D19">
         <v>3.8974783538952548E-2</v>
       </c>
       <c r="E19">
-        <v>2.2204460492503131E-14</v>
+        <v>2.2204473777882011E-14</v>
       </c>
       <c r="F19">
-        <v>7.6461774833530699E-2</v>
+        <v>7.4930334020398101E-2</v>
       </c>
       <c r="G19">
         <v>2.6525198939014245E-2</v>
       </c>
       <c r="H19">
-        <v>1.0000000000022205E-2</v>
+        <v>1.0000022204521512E-8</v>
       </c>
       <c r="I19">
-        <v>2.2204532691315942E-14</v>
+        <v>6.715716657390027E-3</v>
       </c>
       <c r="J19">
         <v>2.8613040667312468</v>
@@ -3576,22 +3601,22 @@
         <v>13771138.993237138</v>
       </c>
       <c r="M19">
-        <v>0.99716513163134535</v>
+        <v>0.99722462033937131</v>
       </c>
       <c r="N19">
-        <v>0.90794537169988088</v>
+        <v>0.90128299723359717</v>
       </c>
       <c r="O19">
-        <v>0.89491751628455818</v>
+        <v>0.8834006306256792</v>
       </c>
       <c r="P19">
-        <v>0.10823188741399233</v>
+        <v>9.6944412290866436E-2</v>
       </c>
       <c r="Q19">
-        <v>0.49249245351170307</v>
+        <v>0.48904516178599816</v>
       </c>
       <c r="R19">
-        <v>0.49034598202871504</v>
+        <v>0.49148438074501466</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -3599,10 +3624,10 @@
         <v>2.025226724750458E-2</v>
       </c>
       <c r="B20">
-        <v>3.6610390547511515E-2</v>
+        <v>3.661038817423995E-2</v>
       </c>
       <c r="C20">
-        <v>0.5853033897148392</v>
+        <v>0.58530339194918313</v>
       </c>
       <c r="D20">
         <v>4.2860723219890554E-2</v>
@@ -3611,16 +3636,16 @@
         <v>9.9999999999977801E-2</v>
       </c>
       <c r="F20">
-        <v>0.13494301354701782</v>
+        <v>0.13494299556910744</v>
       </c>
       <c r="G20">
-        <v>2.7115786906026642E-2</v>
+        <v>2.6595818555612983E-2</v>
       </c>
       <c r="H20">
-        <v>0.20534211709335104</v>
+        <v>0.20586204465426139</v>
       </c>
       <c r="I20">
-        <v>2.2204509967596189E-14</v>
+        <v>2.2204503459977956E-14</v>
       </c>
       <c r="J20">
         <v>2.4328816932437634</v>
@@ -3632,22 +3657,22 @@
         <v>898068381.93210459</v>
       </c>
       <c r="M20">
-        <v>0.9934569248362799</v>
+        <v>0.99345692483643755</v>
       </c>
       <c r="N20">
-        <v>0.98644924365814857</v>
+        <v>0.98644924290192071</v>
       </c>
       <c r="O20">
-        <v>0.99602689623857521</v>
+        <v>0.99602689796079291</v>
       </c>
       <c r="P20">
-        <v>0.1161289007810055</v>
+        <v>0.11612890077785666</v>
       </c>
       <c r="Q20">
-        <v>0.16359252139818381</v>
+        <v>0.16359252591784523</v>
       </c>
       <c r="R20">
-        <v>0.10046396257918214</v>
+        <v>0.10046394420079181</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -3658,25 +3683,25 @@
         <v>7.9999999999977797E-2</v>
       </c>
       <c r="C21">
-        <v>2.4870588046489526</v>
+        <v>2.4870592214691891</v>
       </c>
       <c r="D21">
         <v>4.3368027883496717E-2</v>
       </c>
       <c r="E21">
-        <v>2.2204867724035772E-14</v>
+        <v>2.2205191754949247E-14</v>
       </c>
       <c r="F21">
-        <v>0.2172093137196848</v>
+        <v>0.21720927390656489</v>
       </c>
       <c r="G21">
-        <v>2.7318550695947286E-2</v>
+        <v>2.6542277456997741E-2</v>
       </c>
       <c r="H21">
-        <v>0.27892530084188294</v>
+        <v>0.27970150312629444</v>
       </c>
       <c r="I21">
-        <v>2.2204460492503137E-14</v>
+        <v>2.220448407366131E-14</v>
       </c>
       <c r="J21">
         <v>2.9741152430411644</v>
@@ -3688,22 +3713,22 @@
         <v>1569235476.0781155</v>
       </c>
       <c r="M21">
-        <v>0.98728130885960819</v>
+        <v>0.98728130885977849</v>
       </c>
       <c r="N21">
-        <v>0.98447514688737792</v>
+        <v>0.98447514473401299</v>
       </c>
       <c r="O21">
-        <v>0.99243473531977422</v>
+        <v>0.99243473711185037</v>
       </c>
       <c r="P21">
-        <v>0.15890607311015181</v>
+        <v>0.15890607310726296</v>
       </c>
       <c r="Q21">
-        <v>0.17688629596336616</v>
+        <v>0.17688630763901789</v>
       </c>
       <c r="R21">
-        <v>0.12648228614488313</v>
+        <v>0.12648227289179581</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -3711,28 +3736,28 @@
         <v>1.9998083024111244E-2</v>
       </c>
       <c r="B22">
-        <v>7.9999999999962199E-2</v>
+        <v>7.9999999999977797E-2</v>
       </c>
       <c r="C22">
-        <v>2.4607137940382193</v>
+        <v>2.4607134617885431</v>
       </c>
       <c r="D22">
-        <v>4.4657955198497093E-2</v>
+        <v>4.4657955198512699E-2</v>
       </c>
       <c r="E22">
-        <v>3.780698624177397E-14</v>
+        <v>2.220960075234407E-14</v>
       </c>
       <c r="F22">
-        <v>0.26729348110179429</v>
+        <v>0.26729351310643173</v>
       </c>
       <c r="G22">
-        <v>2.759856641401728E-2</v>
+        <v>2.655305918638852E-2</v>
       </c>
       <c r="H22">
-        <v>0.37177147491607176</v>
+        <v>0.37281704729437759</v>
       </c>
       <c r="I22">
-        <v>3.7805012280679368E-14</v>
+        <v>2.2204943639415854E-14</v>
       </c>
       <c r="J22">
         <v>3.8163808997580695</v>
@@ -3744,22 +3769,22 @@
         <v>911747954.02784622</v>
       </c>
       <c r="M22">
-        <v>0.99437216182673116</v>
+        <v>0.99437216182671762</v>
       </c>
       <c r="N22">
-        <v>0.96042882203253122</v>
+        <v>0.96042882358742254</v>
       </c>
       <c r="O22">
-        <v>0.9954532812165402</v>
+        <v>0.99545327999674993</v>
       </c>
       <c r="P22">
-        <v>0.10664431575679494</v>
+        <v>0.10664431575955506</v>
       </c>
       <c r="Q22">
-        <v>0.28177653898350413</v>
+        <v>0.28177653343532372</v>
       </c>
       <c r="R22">
-        <v>9.5764790000760769E-2</v>
+        <v>9.5764802955078374E-2</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -4072,7 +4097,7 @@
       </c>
       <c r="T27" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Lower</v>
       </c>
       <c r="U27" t="str">
         <f t="shared" si="0"/>
@@ -4101,27 +4126,27 @@
       </c>
       <c r="C28">
         <f>AVERAGE(B$1:B$3)</f>
-        <v>3.6597133043012298E-3</v>
+        <v>3.6597166972760207E-3</v>
       </c>
       <c r="D28">
         <f>AVERAGE(B$4:B$6)</f>
-        <v>1.3300064731281707E-2</v>
+        <v>1.2969578710698102E-2</v>
       </c>
       <c r="E28">
         <f>AVERAGE(B$7:B$12,B$17:B$19)</f>
-        <v>3.0904225837136496E-2</v>
+        <v>3.9850373025406699E-2</v>
       </c>
       <c r="F28">
         <f>AVERAGE(B$13:B$16)</f>
-        <v>6.7758110867901771E-3</v>
+        <v>1.7436370403402304E-2</v>
       </c>
       <c r="G28">
         <f>B$20</f>
-        <v>3.6610390547511515E-2</v>
+        <v>3.661038817423995E-2</v>
       </c>
       <c r="H28">
         <f>AVERAGE(B$21:B$22)</f>
-        <v>7.9999999999969998E-2</v>
+        <v>7.9999999999977797E-2</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="2"/>
@@ -4175,23 +4200,23 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>STDEV(B$1:B$3)/SQRT(COUNT(B$1:B$3))</f>
-        <v>1.3632607711826903E-4</v>
+        <v>1.3632467423976377E-4</v>
       </c>
       <c r="D29">
         <f>STDEV(B$4:B$6)/SQRT(COUNT(B$4:B$6))</f>
-        <v>1.2769661600346282E-3</v>
+        <v>2.8102841025300172E-3</v>
       </c>
       <c r="E29">
         <f>STDEV(B$7:B$12,B$17:B$19)/SQRT(COUNT(B$7:B$12,B$17:B$19))</f>
-        <v>1.0184696395931343E-2</v>
+        <v>1.0181144930654133E-2</v>
       </c>
       <c r="F29">
         <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
-        <v>1.4460017690863679E-3</v>
+        <v>9.1957167148318739E-3</v>
       </c>
       <c r="H29">
         <f>STDEV(B$21:B$22)/SQRT(COUNT(B$21:B$22))</f>
-        <v>7.7993167479917247E-15</v>
+        <v>0</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="2"/>
@@ -4329,7 +4354,7 @@
       </c>
       <c r="R31" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="0"/>
@@ -4366,27 +4391,27 @@
       </c>
       <c r="D32">
         <f>AVERAGE(C$1:C$3)</f>
-        <v>0.1902353577824655</v>
+        <v>0.19023535438688108</v>
       </c>
       <c r="E32">
         <f>AVERAGE(C$4:C$6)</f>
-        <v>0.11118316294687479</v>
+        <v>0.11098762168381754</v>
       </c>
       <c r="F32">
         <f>AVERAGE(C$7:C$12,C$17:C$19)</f>
-        <v>0.32149322479160841</v>
+        <v>0.31184021552856422</v>
       </c>
       <c r="G32">
         <f>AVERAGE(C$13:C$16)</f>
-        <v>0.13597096544935236</v>
+        <v>0.12473897964381199</v>
       </c>
       <c r="H32">
         <f>C$20</f>
-        <v>0.5853033897148392</v>
+        <v>0.58530339194918313</v>
       </c>
       <c r="I32">
         <f>AVERAGE(C$21:C$22)</f>
-        <v>2.4738862993435857</v>
+        <v>2.4738863416288659</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="2"/>
@@ -4414,7 +4439,7 @@
       </c>
       <c r="T32" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="0"/>
@@ -4440,23 +4465,23 @@
     <row r="33" spans="4:31" x14ac:dyDescent="0.25">
       <c r="D33">
         <f>STDEV(C$1:C$3)/SQRT(COUNT(C$1:C$3))</f>
-        <v>3.4764253988252884E-2</v>
+        <v>3.4764251947037965E-2</v>
       </c>
       <c r="E33">
         <f>STDEV(C$4:C$6)/SQRT(COUNT(C$4:C$6))</f>
-        <v>0.10888122932266156</v>
+        <v>0.10709949468666879</v>
       </c>
       <c r="F33">
         <f>STDEV(C$7:C$12,C$17:C$19)/SQRT(COUNT(C$7:C$12,C$17:C$19))</f>
-        <v>0.21614755302810942</v>
+        <v>0.21648529436558617</v>
       </c>
       <c r="G33">
         <f>STDEV(C$13:C$16)/SQRT(COUNT(C$13:C$16))</f>
-        <v>8.3113532814475699E-2</v>
+        <v>7.3357716046404037E-2</v>
       </c>
       <c r="I33">
         <f>STDEV(C$21:C$22)/SQRT(COUNT(C$21:C$22))</f>
-        <v>1.317250530536662E-2</v>
+        <v>1.3172879840323004E-2</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="2"/>
@@ -4484,7 +4509,7 @@
       </c>
       <c r="T33" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U33" t="str">
         <f t="shared" si="0"/>
@@ -4534,7 +4559,7 @@
       </c>
       <c r="T34" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U34" t="str">
         <f t="shared" si="0"/>
@@ -4602,7 +4627,7 @@
       </c>
       <c r="T35" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U35" t="str">
         <f t="shared" si="0"/>
@@ -4635,15 +4660,15 @@
       </c>
       <c r="F36">
         <f>AVERAGE(D$4:D$6)</f>
-        <v>5.8450580517310169E-2</v>
+        <v>5.8426894246005306E-2</v>
       </c>
       <c r="G36">
         <f>AVERAGE(D$7:D$12,D$17:D$19)</f>
-        <v>5.4111926520871996E-2</v>
+        <v>5.408192058558043E-2</v>
       </c>
       <c r="H36">
         <f>AVERAGE(D$13:D$16)</f>
-        <v>6.7770076953259817E-2</v>
+        <v>6.7749360389357263E-2</v>
       </c>
       <c r="I36">
         <f>D$20</f>
@@ -4651,7 +4676,7 @@
       </c>
       <c r="J36">
         <f>AVERAGE(D$21:D$22)</f>
-        <v>4.4012991540996901E-2</v>
+        <v>4.4012991541004708E-2</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="2"/>
@@ -4709,19 +4734,19 @@
       </c>
       <c r="F37">
         <f>STDEV(D$4:D$6)/SQRT(COUNT(D$4:D$6))</f>
-        <v>1.7016447960806473E-2</v>
+        <v>1.7123224610862724E-2</v>
       </c>
       <c r="G37">
         <f>STDEV(D$7:D$12,D$17:D$19)/SQRT(COUNT(D$7:D$12,D$17:D$19))</f>
-        <v>5.1588586627325109E-3</v>
+        <v>5.1216710439505198E-3</v>
       </c>
       <c r="H37">
         <f>STDEV(D$13:D$16)/SQRT(COUNT(D$13:D$16))</f>
-        <v>1.5619257150863446E-2</v>
+        <v>1.5627247705565079E-2</v>
       </c>
       <c r="J37">
         <f>STDEV(D$21:D$22)/SQRT(COUNT(D$21:D$22))</f>
-        <v>6.4496365750018811E-4</v>
+        <v>6.4496365750799079E-4</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="2"/>
@@ -4803,7 +4828,7 @@
       </c>
       <c r="U38" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="0"/>
@@ -4867,7 +4892,7 @@
       </c>
       <c r="T39" t="str">
         <f t="shared" si="2"/>
-        <v>Lower</v>
+        <v>Upper</v>
       </c>
       <c r="U39" t="str">
         <f t="shared" si="2"/>
@@ -4896,19 +4921,19 @@
       </c>
       <c r="F40">
         <f>AVERAGE(E$1:E$3)</f>
-        <v>1.7158841421999715E-13</v>
+        <v>2.2210033221700154E-14</v>
       </c>
       <c r="G40">
         <f>AVERAGE(E$4:E$6)</f>
-        <v>2.5348461372330554E-2</v>
+        <v>2.8172663076369224E-7</v>
       </c>
       <c r="H40">
         <f>AVERAGE(E$7:E$12,E$17:E$19)</f>
-        <v>2.1120262511376605E-2</v>
+        <v>4.0146854743199973E-4</v>
       </c>
       <c r="I40">
         <f>AVERAGE(E$13:E$16)</f>
-        <v>1.4232603940306798E-2</v>
+        <v>4.4129444733917032E-6</v>
       </c>
       <c r="J40">
         <f>E$20</f>
@@ -4916,7 +4941,7 @@
       </c>
       <c r="K40">
         <f>AVERAGE(E$21:E$22)</f>
-        <v>3.0005926982904871E-14</v>
+        <v>2.2207396253646659E-14</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="2"/>
@@ -4944,7 +4969,7 @@
       </c>
       <c r="T40" t="str">
         <f t="shared" si="2"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U40" t="str">
         <f t="shared" si="2"/>
@@ -4970,23 +4995,23 @@
     <row r="41" spans="4:31" x14ac:dyDescent="0.25">
       <c r="F41">
         <f>STDEV(E$1:E$3)/SQRT(COUNT(E$1:E$3))</f>
-        <v>1.493782733658106E-13</v>
+        <v>4.8250618270174104E-18</v>
       </c>
       <c r="G41">
         <f>STDEV(E$4:E$6)/SQRT(COUNT(E$4:E$6))</f>
-        <v>2.5346287860291056E-2</v>
+        <v>2.8172660276019622E-7</v>
       </c>
       <c r="H41">
         <f>STDEV(E$7:E$12,E$17:E$19)/SQRT(COUNT(E$7:E$12,E$17:E$19))</f>
-        <v>1.3916544060130964E-2</v>
+        <v>2.8632212313389749E-4</v>
       </c>
       <c r="I41">
         <f>STDEV(E$13:E$16)/SQRT(COUNT(E$13:E$16))</f>
-        <v>1.4053298291185456E-2</v>
+        <v>4.4127585456074152E-6</v>
       </c>
       <c r="K41">
         <f>STDEV(E$21:E$22)/SQRT(COUNT(E$21:E$22))</f>
-        <v>7.8010592588690992E-15</v>
+        <v>2.2044986974114701E-18</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="2"/>
@@ -5018,7 +5043,7 @@
       </c>
       <c r="U41" t="str">
         <f t="shared" si="2"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="2"/>
@@ -5064,7 +5089,7 @@
       </c>
       <c r="T42" t="str">
         <f t="shared" si="2"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U42" t="str">
         <f t="shared" si="2"/>
@@ -5132,7 +5157,7 @@
       </c>
       <c r="T43" t="str">
         <f t="shared" si="2"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U43" t="str">
         <f t="shared" si="2"/>
@@ -5161,27 +5186,27 @@
       </c>
       <c r="G44">
         <f>AVERAGE(F$1:F$3)</f>
-        <v>0.14700879061061764</v>
+        <v>0.14700895503484715</v>
       </c>
       <c r="H44">
         <f>AVERAGE(F$4:F$6)</f>
-        <v>0.53211377816446115</v>
+        <v>0.51874426073426694</v>
       </c>
       <c r="I44">
         <f>AVERAGE(F$7:F$12,F$17:F$19)</f>
-        <v>0.23593587790019413</v>
+        <v>0.67733097633142481</v>
       </c>
       <c r="J44">
         <f>AVERAGE(F$13:F$16)</f>
-        <v>8.8135960815575995E-2</v>
+        <v>0.55341627633490109</v>
       </c>
       <c r="K44">
         <f>F$20</f>
-        <v>0.13494301354701782</v>
+        <v>0.13494299556910744</v>
       </c>
       <c r="L44">
         <f>AVERAGE(F$21:F$22)</f>
-        <v>0.24225139741073953</v>
+        <v>0.24225139350649832</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="2"/>
@@ -5209,7 +5234,7 @@
       </c>
       <c r="T44" t="str">
         <f t="shared" si="2"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U44" t="str">
         <f t="shared" si="2"/>
@@ -5235,23 +5260,23 @@
     <row r="45" spans="4:31" x14ac:dyDescent="0.25">
       <c r="G45">
         <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
-        <v>3.7887328106141906E-2</v>
+        <v>3.7887236211488991E-2</v>
       </c>
       <c r="H45">
         <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
-        <v>6.6912787197246887E-2</v>
+        <v>0.12579716058654763</v>
       </c>
       <c r="I45">
         <f>STDEV(F$7:F$12,F$17:F$19)/SQRT(COUNT(F$7:F$12,F$17:F$19))</f>
-        <v>6.984101299788778E-2</v>
+        <v>0.34452837581693579</v>
       </c>
       <c r="J45">
         <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
-        <v>2.8964194893118057E-2</v>
+        <v>0.44401386483779698</v>
       </c>
       <c r="L45">
         <f>STDEV(F$21:F$22)/SQRT(COUNT(F$21:F$22))</f>
-        <v>2.5042083691054894E-2</v>
+        <v>2.5042119599933226E-2</v>
       </c>
       <c r="N45" t="s">
         <v>17</v>
@@ -5334,49 +5359,49 @@
       </c>
       <c r="H48">
         <f>AVERAGE(G$1:G$3)</f>
-        <v>2.6668175336377026E-2</v>
+        <v>2.6612095404732927E-2</v>
       </c>
       <c r="I48">
         <f>AVERAGE(G$4:G$6)</f>
-        <v>2.7692986803862573E-2</v>
+        <v>2.7473079382476524E-2</v>
       </c>
       <c r="J48">
         <f>AVERAGE(G$7:G$12,G$17:G$19)</f>
-        <v>2.7413297983009691E-2</v>
+        <v>2.7283317623498213E-2</v>
       </c>
       <c r="K48">
         <f>AVERAGE(G$13:G$16)</f>
-        <v>2.7461877550028567E-2</v>
+        <v>2.7369710249433226E-2</v>
       </c>
       <c r="L48">
         <f>G$20</f>
-        <v>2.7115786906026642E-2</v>
+        <v>2.6595818555612983E-2</v>
       </c>
       <c r="M48">
         <f>AVERAGE(G$21:G$22)</f>
-        <v>2.7458558554982283E-2</v>
+        <v>2.654766832169313E-2</v>
       </c>
     </row>
     <row r="49" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H49">
         <f>STDEV(G$1:G$3)/SQRT(COUNT(G$1:G$3))</f>
-        <v>1.4479805214217238E-5</v>
+        <v>4.5088837848277105E-5</v>
       </c>
       <c r="I49">
         <f>STDEV(G$4:G$6)/SQRT(COUNT(G$4:G$6))</f>
-        <v>3.121194662790988E-4</v>
+        <v>3.7252970632583378E-4</v>
       </c>
       <c r="J49">
         <f>STDEV(G$7:G$12,G$17:G$19)/SQRT(COUNT(G$7:G$12,G$17:G$19))</f>
-        <v>1.9541867727211271E-4</v>
+        <v>1.9591704856672309E-4</v>
       </c>
       <c r="K49">
         <f>STDEV(G$13:G$16)/SQRT(COUNT(G$13:G$16))</f>
-        <v>3.5022485946054928E-4</v>
+        <v>2.9674052868955972E-4</v>
       </c>
       <c r="M49">
         <f>STDEV(G$21:G$22)/SQRT(COUNT(G$21:G$22))</f>
-        <v>1.4000785903499693E-4</v>
+        <v>5.3908646953891581E-6</v>
       </c>
     </row>
     <row r="51" spans="8:17" x14ac:dyDescent="0.25">
@@ -5405,49 +5430,49 @@
       </c>
       <c r="I52">
         <f>AVERAGE(H$1:H$3)</f>
-        <v>7.5861286798705629E-2</v>
+        <v>7.5917629324230532E-2</v>
       </c>
       <c r="J52">
         <f>AVERAGE(H$4:H$6)</f>
-        <v>0.39677921844300285</v>
+        <v>0.39118585551184881</v>
       </c>
       <c r="K52">
         <f>AVERAGE(H$7:H$12,H$17:H$19)</f>
-        <v>0.27090893937315036</v>
+        <v>1.4556807367818019</v>
       </c>
       <c r="L52">
         <f>AVERAGE(H$13:H$16)</f>
-        <v>0.26398530154365096</v>
+        <v>2.6891949704917932</v>
       </c>
       <c r="M52">
         <f>H$20</f>
-        <v>0.20534211709335104</v>
+        <v>0.20586204465426139</v>
       </c>
       <c r="N52">
         <f>AVERAGE(H$21:H$22)</f>
-        <v>0.32534838787897735</v>
+        <v>0.32625927521033604</v>
       </c>
     </row>
     <row r="53" spans="8:17" x14ac:dyDescent="0.25">
       <c r="I53">
         <f>STDEV(H$1:H$3)/SQRT(COUNT(H$1:H$3))</f>
-        <v>2.1999772662891989E-2</v>
+        <v>2.1967251752266336E-2</v>
       </c>
       <c r="J53">
         <f>STDEV(H$4:H$6)/SQRT(COUNT(H$4:H$6))</f>
-        <v>0.10126319541438172</v>
+        <v>0.14380117024004904</v>
       </c>
       <c r="K53">
         <f>STDEV(H$7:H$12,H$17:H$19)/SQRT(COUNT(H$7:H$12,H$17:H$19))</f>
-        <v>6.6739090240732699E-2</v>
+        <v>1.0473379060285419</v>
       </c>
       <c r="L53">
         <f>STDEV(H$13:H$16)/SQRT(COUNT(H$13:H$16))</f>
-        <v>0.13632723878677147</v>
+        <v>2.4385643271491557</v>
       </c>
       <c r="N53">
         <f>STDEV(H$21:H$22)/SQRT(COUNT(H$21:H$22))</f>
-        <v>4.642308703709442E-2</v>
+        <v>4.6557772084041354E-2</v>
       </c>
     </row>
     <row r="55" spans="8:17" x14ac:dyDescent="0.25">
@@ -5476,49 +5501,49 @@
       </c>
       <c r="J56">
         <f>AVERAGE(I$1:I$3)</f>
-        <v>4.704327092364341E-2</v>
+        <v>4.7043281897724644E-2</v>
       </c>
       <c r="K56">
         <f>AVERAGE(I$4:I$6)</f>
-        <v>9.330838754924506E-8</v>
+        <v>3.4991609077748002E-14</v>
       </c>
       <c r="L56">
         <f>AVERAGE(I$7:I$12,I$17:I$19)</f>
-        <v>1.2467919832583505E-6</v>
+        <v>7.4630219943887829E-4</v>
       </c>
       <c r="M56">
         <f>AVERAGE(I$13:I$16)</f>
-        <v>8.1976083382374636E-6</v>
+        <v>4.0530954529238379E-6</v>
       </c>
       <c r="N56">
         <f>I$20</f>
-        <v>2.2204509967596189E-14</v>
+        <v>2.2204503459977956E-14</v>
       </c>
       <c r="O56">
         <f>AVERAGE(I$21:I$22)</f>
-        <v>3.0004736386591249E-14</v>
+        <v>2.2204713856538582E-14</v>
       </c>
     </row>
     <row r="57" spans="8:17" x14ac:dyDescent="0.25">
       <c r="J57">
         <f>STDEV(I$1:I$3)/SQRT(COUNT(I$1:I$3))</f>
-        <v>4.7043270923621192E-2</v>
+        <v>4.7043281897702433E-2</v>
       </c>
       <c r="K57">
         <f>STDEV(I$4:I$6)/SQRT(COUNT(I$4:I$6))</f>
-        <v>9.3308359245456856E-8</v>
+        <v>6.3772773096146374E-15</v>
       </c>
       <c r="L57">
         <f>STDEV(I$7:I$12,I$17:I$19)/SQRT(COUNT(I$7:I$12,I$17:I$19))</f>
-        <v>1.2449692316753025E-6</v>
+        <v>7.4617681527279955E-4</v>
       </c>
       <c r="M57">
         <f>STDEV(I$13:I$16)/SQRT(COUNT(I$13:I$16))</f>
-        <v>8.1976083160326609E-6</v>
+        <v>4.0529326997889823E-6</v>
       </c>
       <c r="O57">
         <f>STDEV(I$21:I$22)/SQRT(COUNT(I$21:I$22))</f>
-        <v>7.8002758940881152E-15</v>
+        <v>2.2978287727198393E-19</v>
       </c>
     </row>
     <row r="59" spans="8:17" x14ac:dyDescent="0.25">
@@ -5760,49 +5785,49 @@
       </c>
       <c r="N72">
         <f>AVERAGE(M$1:M$3)</f>
-        <v>0.99662997411815601</v>
+        <v>0.99662997411815801</v>
       </c>
       <c r="O72">
         <f>AVERAGE(M$4:M$6)</f>
-        <v>0.99678501278096354</v>
+        <v>0.99678502774392774</v>
       </c>
       <c r="P72">
         <f>AVERAGE(M$7:M$12,M$17:M$19)</f>
-        <v>0.99461802812034483</v>
+        <v>0.9946243241560917</v>
       </c>
       <c r="Q72">
         <f>AVERAGE(M$13:M$16)</f>
-        <v>0.9961315805076334</v>
+        <v>0.99613211356786546</v>
       </c>
       <c r="R72">
         <f>M$20</f>
-        <v>0.9934569248362799</v>
+        <v>0.99345692483643755</v>
       </c>
       <c r="S72">
         <f>AVERAGE(M$21:M$22)</f>
-        <v>0.99082673534316967</v>
+        <v>0.99082673534324806</v>
       </c>
     </row>
     <row r="73" spans="12:21" x14ac:dyDescent="0.25">
       <c r="N73">
         <f>STDEV(M$1:M$3)/SQRT(COUNT(M$1:M$3))</f>
-        <v>4.9336913887983213E-4</v>
+        <v>4.9336913887755639E-4</v>
       </c>
       <c r="O73">
         <f>STDEV(M$4:M$6)/SQRT(COUNT(M$4:M$6))</f>
-        <v>3.4871651771266294E-4</v>
+        <v>3.486949347042988E-4</v>
       </c>
       <c r="P73">
         <f>STDEV(M$7:M$12,M$17:M$19)/SQRT(COUNT(M$7:M$12,M$17:M$19))</f>
-        <v>1.9800158693533414E-3</v>
+        <v>1.9810102119476331E-3</v>
       </c>
       <c r="Q73">
         <f>STDEV(M$13:M$16)/SQRT(COUNT(M$13:M$16))</f>
-        <v>1.6831280395604258E-3</v>
+        <v>1.6834148194512729E-3</v>
       </c>
       <c r="S73">
         <f>STDEV(M$21:M$22)/SQRT(COUNT(M$21:M$22))</f>
-        <v>3.5454264835614868E-3</v>
+        <v>3.5454264834695604E-3</v>
       </c>
     </row>
     <row r="75" spans="12:21" x14ac:dyDescent="0.25">
@@ -5831,49 +5856,49 @@
       </c>
       <c r="O76">
         <f>AVERAGE(N$1:N$3)</f>
-        <v>0.9919993696988838</v>
+        <v>0.99199938412162059</v>
       </c>
       <c r="P76">
         <f>AVERAGE(N$4:N$6)</f>
-        <v>0.97675891843624296</v>
+        <v>0.97541479470508063</v>
       </c>
       <c r="Q76">
         <f>AVERAGE(N$7:N$12,N$17:N$19)</f>
-        <v>0.9688155387124906</v>
+        <v>0.96965084484165076</v>
       </c>
       <c r="R76">
         <f>AVERAGE(N$13:N$16)</f>
-        <v>0.98926077028853232</v>
+        <v>0.99258746444793977</v>
       </c>
       <c r="S76">
         <f>N$20</f>
-        <v>0.98644924365814857</v>
+        <v>0.98644924290192071</v>
       </c>
       <c r="T76">
         <f>AVERAGE(N$21:N$22)</f>
-        <v>0.97245198445995462</v>
+        <v>0.97245198416071776</v>
       </c>
     </row>
     <row r="77" spans="12:21" x14ac:dyDescent="0.25">
       <c r="O77">
         <f>STDEV(N$1:N$3)/SQRT(COUNT(N$1:N$3))</f>
-        <v>3.3666500559051083E-3</v>
+        <v>3.3666505227571966E-3</v>
       </c>
       <c r="P77">
         <f>STDEV(N$4:N$6)/SQRT(COUNT(N$4:N$6))</f>
-        <v>9.2183766083138597E-3</v>
+        <v>1.0654580102394942E-2</v>
       </c>
       <c r="Q77">
         <f>STDEV(N$7:N$12,N$17:N$19)/SQRT(COUNT(N$7:N$12,N$17:N$19))</f>
-        <v>1.1478576794660104E-2</v>
+        <v>1.1875659785251722E-2</v>
       </c>
       <c r="R77">
         <f>STDEV(N$13:N$16)/SQRT(COUNT(N$13:N$16))</f>
-        <v>5.1869562431028169E-3</v>
+        <v>2.5055085561655724E-3</v>
       </c>
       <c r="T77">
         <f>STDEV(N$21:N$22)/SQRT(COUNT(N$21:N$22))</f>
-        <v>1.2023162427423351E-2</v>
+        <v>1.2023160573295222E-2</v>
       </c>
     </row>
     <row r="79" spans="12:21" x14ac:dyDescent="0.25">
@@ -5902,49 +5927,49 @@
       </c>
       <c r="P80">
         <f>AVERAGE(O$1:O$3)</f>
-        <v>0.99642632811010257</v>
+        <v>0.99642630127703191</v>
       </c>
       <c r="Q80">
         <f>AVERAGE(O$4:O$6)</f>
-        <v>0.98917892164055987</v>
+        <v>0.98562172652789837</v>
       </c>
       <c r="R80">
         <f>AVERAGE(O$7:O$12,O$17:O$19)</f>
-        <v>0.97821003950400409</v>
+        <v>0.97622736868249915</v>
       </c>
       <c r="S80">
         <f>AVERAGE(O$13:O$16)</f>
-        <v>0.98027561081966963</v>
+        <v>0.96792446357023321</v>
       </c>
       <c r="T80">
         <f>O$20</f>
-        <v>0.99602689623857521</v>
+        <v>0.99602689796079291</v>
       </c>
       <c r="U80">
         <f>AVERAGE(O$21:O$22)</f>
-        <v>0.99394400826815721</v>
+        <v>0.9939440085543001</v>
       </c>
     </row>
     <row r="81" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P81">
         <f>STDEV(O$1:O$3)/SQRT(COUNT(O$1:O$3))</f>
-        <v>7.9034002545263853E-4</v>
+        <v>7.903214212686805E-4</v>
       </c>
       <c r="Q81">
         <f>STDEV(O$4:O$6)/SQRT(COUNT(O$4:O$6))</f>
-        <v>5.7377095151756631E-3</v>
+        <v>9.0723300721945472E-3</v>
       </c>
       <c r="R81">
         <f>STDEV(O$7:O$12,O$17:O$19)/SQRT(COUNT(O$7:O$12,O$17:O$19))</f>
-        <v>1.1269732134431406E-2</v>
+        <v>1.2129818847755281E-2</v>
       </c>
       <c r="S81">
         <f>STDEV(O$13:O$16)/SQRT(COUNT(O$13:O$16))</f>
-        <v>1.1061837985539188E-2</v>
+        <v>9.1385974951318887E-3</v>
       </c>
       <c r="U81">
         <f>STDEV(O$21:O$22)/SQRT(COUNT(O$21:O$22))</f>
-        <v>1.509272948382989E-3</v>
+        <v>1.5092714424497777E-3</v>
       </c>
     </row>
     <row r="83" spans="16:24" x14ac:dyDescent="0.25">
@@ -5973,49 +5998,49 @@
       </c>
       <c r="Q84">
         <f>AVERAGE(P$1:P$3)</f>
-        <v>8.2769960386286451E-2</v>
+        <v>8.2769960386286354E-2</v>
       </c>
       <c r="R84">
         <f>AVERAGE(P$4:P$6)</f>
-        <v>8.1748068131832677E-2</v>
+        <v>8.1747176174903999E-2</v>
       </c>
       <c r="S84">
         <f>AVERAGE(P$7:P$12,P$17:P$19)</f>
-        <v>9.7875304923831299E-2</v>
+        <v>9.6618096060557532E-2</v>
       </c>
       <c r="T84">
         <f>AVERAGE(P$13:P$16)</f>
-        <v>8.0500087382240917E-2</v>
+        <v>8.0488259007867796E-2</v>
       </c>
       <c r="U84">
         <f>P$20</f>
-        <v>0.1161289007810055</v>
+        <v>0.11612890077785666</v>
       </c>
       <c r="V84">
         <f>AVERAGE(P$21:P$22)</f>
-        <v>0.13277519443347338</v>
+        <v>0.13277519443340902</v>
       </c>
     </row>
     <row r="85" spans="16:24" x14ac:dyDescent="0.25">
       <c r="Q85">
         <f>STDEV(P$1:P$3)/SQRT(COUNT(P$1:P$3))</f>
-        <v>6.1728202303741025E-3</v>
+        <v>6.1728202303740097E-3</v>
       </c>
       <c r="R85">
         <f>STDEV(P$4:P$6)/SQRT(COUNT(P$4:P$6))</f>
-        <v>4.7629466277518016E-3</v>
+        <v>4.7620664425895532E-3</v>
       </c>
       <c r="S85">
         <f>STDEV(P$7:P$12,P$17:P$19)/SQRT(COUNT(P$7:P$12,P$17:P$19))</f>
-        <v>1.5268331327673275E-2</v>
+        <v>1.5214270543208034E-2</v>
       </c>
       <c r="T85">
         <f>STDEV(P$13:P$16)/SQRT(COUNT(P$13:P$16))</f>
-        <v>2.0136088514527462E-2</v>
+        <v>2.014243603928605E-2</v>
       </c>
       <c r="V85">
         <f>STDEV(P$21:P$22)/SQRT(COUNT(P$21:P$22))</f>
-        <v>2.6130878676678425E-2</v>
+        <v>2.6130878673853903E-2</v>
       </c>
     </row>
     <row r="87" spans="16:24" x14ac:dyDescent="0.25">
@@ -6044,49 +6069,49 @@
       </c>
       <c r="R88">
         <f>AVERAGE(Q$1:Q$3)</f>
-        <v>0.12003221087640574</v>
+        <v>0.12003209288401152</v>
       </c>
       <c r="S88">
         <f>AVERAGE(Q$4:Q$6)</f>
-        <v>0.21091855528714845</v>
+        <v>0.21343844914888963</v>
       </c>
       <c r="T88">
         <f>AVERAGE(Q$7:Q$12,Q$17:Q$19)</f>
-        <v>0.2227997445683346</v>
+        <v>0.21495956670453156</v>
       </c>
       <c r="U88">
         <f>AVERAGE(Q$13:Q$16)</f>
-        <v>0.1415769011250852</v>
+        <v>0.12579060832283959</v>
       </c>
       <c r="V88">
         <f>Q$20</f>
-        <v>0.16359252139818381</v>
+        <v>0.16359252591784523</v>
       </c>
       <c r="W88">
         <f>AVERAGE(Q$21:Q$22)</f>
-        <v>0.22933141747343516</v>
+        <v>0.22933142053717082</v>
       </c>
     </row>
     <row r="89" spans="16:24" x14ac:dyDescent="0.25">
       <c r="R89">
         <f>STDEV(Q$1:Q$3)/SQRT(COUNT(Q$1:Q$3))</f>
-        <v>2.9915220573315807E-2</v>
+        <v>2.9915209911607666E-2</v>
       </c>
       <c r="S89">
         <f>STDEV(Q$4:Q$6)/SQRT(COUNT(Q$4:Q$6))</f>
-        <v>3.8691465535530538E-2</v>
+        <v>4.3580024502883882E-2</v>
       </c>
       <c r="T89">
         <f>STDEV(Q$7:Q$12,Q$17:Q$19)/SQRT(COUNT(Q$7:Q$12,Q$17:Q$19))</f>
-        <v>4.9627161039818901E-2</v>
+        <v>4.9563045357193969E-2</v>
       </c>
       <c r="U89">
         <f>STDEV(Q$13:Q$16)/SQRT(COUNT(Q$13:Q$16))</f>
-        <v>3.6708710645921253E-2</v>
+        <v>2.5182325466262E-2</v>
       </c>
       <c r="W89">
         <f>STDEV(Q$21:Q$22)/SQRT(COUNT(Q$21:Q$22))</f>
-        <v>5.2445121510068915E-2</v>
+        <v>5.2445112898152908E-2</v>
       </c>
     </row>
     <row r="91" spans="16:24" x14ac:dyDescent="0.25">
@@ -6115,49 +6140,49 @@
       </c>
       <c r="S92">
         <f>AVERAGE(R$1:R$3)</f>
-        <v>9.8876181514507278E-2</v>
+        <v>9.8876526846989221E-2</v>
       </c>
       <c r="T92">
         <f>AVERAGE(R$4:R$6)</f>
-        <v>0.14624135138680708</v>
+        <v>0.15989821775497828</v>
       </c>
       <c r="U92">
         <f>AVERAGE(R$7:R$12,R$17:R$19)</f>
-        <v>0.18061254916352254</v>
+        <v>0.1863577766352795</v>
       </c>
       <c r="V92">
         <f>AVERAGE(R$13:R$16)</f>
-        <v>0.20116489374268978</v>
+        <v>0.24531984414001679</v>
       </c>
       <c r="W92">
         <f>R$20</f>
-        <v>0.10046396257918214</v>
+        <v>0.10046394420079181</v>
       </c>
       <c r="X92">
         <f>AVERAGE(R$21:R$22)</f>
-        <v>0.11112353807282195</v>
+        <v>0.1111235379234371</v>
       </c>
     </row>
     <row r="93" spans="16:24" x14ac:dyDescent="0.25">
       <c r="S93">
         <f>STDEV(R$1:R$3)/SQRT(COUNT(R$1:R$3))</f>
-        <v>1.6225410832674477E-2</v>
+        <v>1.6225282641834871E-2</v>
       </c>
       <c r="T93">
         <f>STDEV(R$4:R$6)/SQRT(COUNT(R$4:R$6))</f>
-        <v>3.4011963589556958E-2</v>
+        <v>4.7075848425480959E-2</v>
       </c>
       <c r="U93">
         <f>STDEV(R$7:R$12,R$17:R$19)/SQRT(COUNT(R$7:R$12,R$17:R$19))</f>
-        <v>4.6259091503100064E-2</v>
+        <v>4.367031583618889E-2</v>
       </c>
       <c r="V93">
         <f>STDEV(R$13:R$16)/SQRT(COUNT(R$13:R$16))</f>
-        <v>5.553152546303932E-2</v>
+        <v>4.2744543922925191E-2</v>
       </c>
       <c r="X93">
         <f>STDEV(R$21:R$22)/SQRT(COUNT(R$21:R$22))</f>
-        <v>1.5358748072061203E-2</v>
+        <v>1.5358734968358647E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6174,674 +6199,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5469456-525F-43EE-A89C-F45469404D5B}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:W15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:W11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2.0292691946014841E-2</v>
-      </c>
-      <c r="C2">
-        <v>3.6597133043012298E-3</v>
-      </c>
-      <c r="D2">
-        <v>0.1902353577824655</v>
-      </c>
-      <c r="E2">
-        <v>5.9621023719336724E-2</v>
-      </c>
-      <c r="F2">
-        <v>1.7158841421999715E-13</v>
-      </c>
-      <c r="G2">
-        <v>0.14700879061061764</v>
-      </c>
-      <c r="H2">
-        <v>2.6668175336377026E-2</v>
-      </c>
-      <c r="I2">
-        <v>7.5861286798705629E-2</v>
-      </c>
-      <c r="J2">
-        <v>4.704327092364341E-2</v>
-      </c>
-      <c r="T2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2.0154223145541671E-2</v>
-      </c>
-      <c r="C3">
-        <v>1.3300064731281707E-2</v>
-      </c>
-      <c r="D3">
-        <v>0.11118316294687479</v>
-      </c>
-      <c r="E3">
-        <v>5.8450580517310169E-2</v>
-      </c>
-      <c r="F3">
-        <v>2.5348461372330554E-2</v>
-      </c>
-      <c r="G3">
-        <v>0.53211377816446115</v>
-      </c>
-      <c r="H3">
-        <v>2.7692986803862573E-2</v>
-      </c>
-      <c r="I3">
-        <v>0.39677921844300285</v>
-      </c>
-      <c r="J3">
-        <v>9.330838754924506E-8</v>
-      </c>
-      <c r="S3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1.9977688407619744E-2</v>
-      </c>
-      <c r="C4">
-        <v>3.0904225837136496E-2</v>
-      </c>
-      <c r="D4">
-        <v>0.32149322479160841</v>
-      </c>
-      <c r="E4">
-        <v>5.4111926520871996E-2</v>
-      </c>
-      <c r="F4">
-        <v>2.1120262511376605E-2</v>
-      </c>
-      <c r="G4">
-        <v>0.23593587790019413</v>
-      </c>
-      <c r="H4">
-        <v>2.7413297983009691E-2</v>
-      </c>
-      <c r="I4">
-        <v>0.27090893937315036</v>
-      </c>
-      <c r="J4">
-        <v>1.2467919832583505E-6</v>
-      </c>
-      <c r="S4" t="s">
-        <v>6</v>
-      </c>
-      <c r="T4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1.9883827345789976E-2</v>
-      </c>
-      <c r="C5">
-        <v>6.7758110867901771E-3</v>
-      </c>
-      <c r="D5">
-        <v>0.13597096544935236</v>
-      </c>
-      <c r="E5">
-        <v>6.7770076953259817E-2</v>
-      </c>
-      <c r="F5">
-        <v>1.4232603940306798E-2</v>
-      </c>
-      <c r="G5">
-        <v>8.8135960815575995E-2</v>
-      </c>
-      <c r="H5">
-        <v>2.7461877550028567E-2</v>
-      </c>
-      <c r="I5">
-        <v>0.26398530154365096</v>
-      </c>
-      <c r="J5">
-        <v>8.1976083382374636E-6</v>
-      </c>
-      <c r="S5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T5" t="s">
-        <v>28</v>
-      </c>
-      <c r="U5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V5" t="s">
-        <v>30</v>
-      </c>
-      <c r="W5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="S6" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" t="s">
-        <v>32</v>
-      </c>
-      <c r="U6" t="s">
-        <v>32</v>
-      </c>
-      <c r="V6" t="s">
-        <v>33</v>
-      </c>
-      <c r="W6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>3.0517608599749297E-4</v>
-      </c>
-      <c r="C7">
-        <v>1.3632607711826903E-4</v>
-      </c>
-      <c r="D7">
-        <v>3.4764253988252884E-2</v>
-      </c>
-      <c r="E7">
-        <v>2.0792372896380848E-2</v>
-      </c>
-      <c r="F7">
-        <v>1.493782733658106E-13</v>
-      </c>
-      <c r="G7">
-        <v>3.7887328106141906E-2</v>
-      </c>
-      <c r="H7">
-        <v>1.4479805214217238E-5</v>
-      </c>
-      <c r="I7">
-        <v>2.1999772662891989E-2</v>
-      </c>
-      <c r="J7">
-        <v>4.7043270923621192E-2</v>
-      </c>
-      <c r="S7" t="s">
-        <v>10</v>
-      </c>
-      <c r="T7" t="s">
-        <v>35</v>
-      </c>
-      <c r="U7" t="s">
-        <v>36</v>
-      </c>
-      <c r="V7" t="s">
-        <v>37</v>
-      </c>
-      <c r="W7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>7.9639777340775558E-5</v>
-      </c>
-      <c r="C8">
-        <v>1.2769661600346282E-3</v>
-      </c>
-      <c r="D8">
-        <v>0.10888122932266156</v>
-      </c>
-      <c r="E8">
-        <v>1.7016447960806473E-2</v>
-      </c>
-      <c r="F8">
-        <v>2.5346287860291056E-2</v>
-      </c>
-      <c r="G8">
-        <v>6.6912787197246887E-2</v>
-      </c>
-      <c r="H8">
-        <v>3.121194662790988E-4</v>
-      </c>
-      <c r="I8">
-        <v>0.10126319541438172</v>
-      </c>
-      <c r="J8">
-        <v>9.3308359245456856E-8</v>
-      </c>
-      <c r="S8" t="s">
-        <v>7</v>
-      </c>
-      <c r="T8" t="s">
-        <v>39</v>
-      </c>
-      <c r="U8" t="s">
-        <v>40</v>
-      </c>
-      <c r="V8" t="s">
-        <v>41</v>
-      </c>
-      <c r="W8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>1.1372842838082459E-4</v>
-      </c>
-      <c r="C9">
-        <v>1.0184696395931343E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.21614755302810942</v>
-      </c>
-      <c r="E9">
-        <v>5.1588586627325109E-3</v>
-      </c>
-      <c r="F9">
-        <v>1.3916544060130964E-2</v>
-      </c>
-      <c r="G9">
-        <v>6.984101299788778E-2</v>
-      </c>
-      <c r="H9">
-        <v>1.9541867727211271E-4</v>
-      </c>
-      <c r="I9">
-        <v>6.6739090240732699E-2</v>
-      </c>
-      <c r="J9">
-        <v>1.2449692316753025E-6</v>
-      </c>
-      <c r="S9" t="s">
-        <v>18</v>
-      </c>
-      <c r="T9" t="s">
-        <v>43</v>
-      </c>
-      <c r="U9" t="s">
-        <v>43</v>
-      </c>
-      <c r="V9" t="s">
-        <v>43</v>
-      </c>
-      <c r="W9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>1.379957992866012E-4</v>
-      </c>
-      <c r="C10">
-        <v>1.4460017690863679E-3</v>
-      </c>
-      <c r="D10">
-        <v>8.3113532814475699E-2</v>
-      </c>
-      <c r="E10">
-        <v>1.5619257150863446E-2</v>
-      </c>
-      <c r="F10">
-        <v>1.4053298291185456E-2</v>
-      </c>
-      <c r="G10">
-        <v>2.8964194893118057E-2</v>
-      </c>
-      <c r="H10">
-        <v>3.5022485946054928E-4</v>
-      </c>
-      <c r="I10">
-        <v>0.13632723878677147</v>
-      </c>
-      <c r="J10">
-        <v>8.1976083160326609E-6</v>
-      </c>
-      <c r="S10" t="s">
-        <v>9</v>
-      </c>
-      <c r="T10" t="s">
-        <v>44</v>
-      </c>
-      <c r="U10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V10" t="s">
-        <v>46</v>
-      </c>
-      <c r="W10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" t="s">
-        <v>20</v>
-      </c>
-      <c r="S11" t="s">
-        <v>20</v>
-      </c>
-      <c r="T11" t="s">
-        <v>48</v>
-      </c>
-      <c r="U11" t="s">
-        <v>49</v>
-      </c>
-      <c r="V11" t="s">
-        <v>50</v>
-      </c>
-      <c r="W11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="str">
-        <f>IF(NOT(ISNUMBER(FIND("E",B2))),_xlfn.CONCAT(ROUND(B2,2), " ± ", ROUND(B7,2)),_xlfn.CONCAT(LEFT(B2,4),RIGHT(B2,4), " ± ",LEFT(B7,4),RIGHT(B7,4)))</f>
-        <v>0.02 ± 0</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" ref="C12:J12" si="0">IF(NOT(ISNUMBER(FIND("E",C2))),_xlfn.CONCAT(ROUND(C2,2), " ± ", ROUND(C7,2)),_xlfn.CONCAT(LEFT(C2,4),RIGHT(C2,4), " ± ",LEFT(C7,4),RIGHT(C7,4)))</f>
-        <v>0 ± 0</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>0.19 ± 0.03</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>0.06 ± 0.02</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>1.71E-13 ± 1.49E-13</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>0.15 ± 0.04</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>0.03 ± 0</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>0.08 ± 0.02</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>0.05 ± 0.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" ref="B13:J15" si="1">IF(NOT(ISNUMBER(FIND("E",B3))),_xlfn.CONCAT(ROUND(B3,2), " ± ", ROUND(B8,2)),_xlfn.CONCAT(LEFT(B3,4),RIGHT(B3,4), " ± ",LEFT(B8,4),RIGHT(B8,4)))</f>
-        <v>0.02 ± 0</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>0.01 ± 0</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="1"/>
-        <v>0.11 ± 0.11</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="1"/>
-        <v>0.06 ± 0.02</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="1"/>
-        <v>0.03 ± 0.03</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="1"/>
-        <v>0.53 ± 0.07</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="1"/>
-        <v>0.03 ± 0</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="1"/>
-        <v>0.4 ± 0.1</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="1"/>
-        <v>9.33E-08 ± 9.33E-08</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.02 ± 0</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.03 ± 0.01</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.32 ± 0.22</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.05 ± 0.01</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.02 ± 0.01</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.24 ± 0.07</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.03 ± 0</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>0.27 ± 0.07</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="1"/>
-        <v>1.24E-06 ± 1.24E-06</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.02 ± 0</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.01 ± 0</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.14 ± 0.08</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.07 ± 0.02</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.01 ± 0.01</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.09 ± 0.03</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.03 ± 0</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="1"/>
-        <v>0.26 ± 0.14</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="1"/>
-        <v>8.19E-06 ± 8.19E-06</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Resetting repo back to original results with FL from 1E-8 to 10 and initial condition
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation_moredata.xlsx
+++ b/Lacex_summary_FinalConfirmation_moredata.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B101A59-E5A4-49E6-854E-4FB7E5FFC3D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BFFAC9-89A5-4BD0-825D-75787A35DFA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B075899B-8E8B-4489-B096-777C4BA97E2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -262,16 +265,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>4.0251366925833192E-3</c:v>
+                    <c:v>1.3632467423976377E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7125592049724646E-3</c:v>
+                    <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.020338152597138E-2</c:v>
+                    <c:v>1.0181144930654133E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.2628005908930579E-3</c:v>
+                    <c:v>9.1957167148318739E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -283,16 +286,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>4.0251366925833192E-3</c:v>
+                    <c:v>1.3632467423976377E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7125592049724646E-3</c:v>
+                    <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.020338152597138E-2</c:v>
+                    <c:v>1.0181144930654133E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.2628005908930579E-3</c:v>
+                    <c:v>9.1957167148318739E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -338,16 +341,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.7628151949548294E-3</c:v>
+                  <c:v>3.6597166972760207E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5652619320196723E-2</c:v>
+                  <c:v>1.2969578710698102E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1877715078838673E-2</c:v>
+                  <c:v>3.9850373025406699E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1800442735511141E-3</c:v>
+                  <c:v>1.7436370403402304E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,16 +619,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.20417348892883633</c:v>
+                    <c:v>3.7887236211488991E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.14430652595370547</c:v>
+                    <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.7833579515523295E-2</c:v>
+                    <c:v>0.34452837581693579</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.2790536732440492E-2</c:v>
+                    <c:v>0.44401386483779698</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -637,16 +640,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>0.20417348892883633</c:v>
+                    <c:v>3.7887236211488991E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.14430652595370547</c:v>
+                    <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.7833579515523295E-2</c:v>
+                    <c:v>0.34452837581693579</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.2790536732440492E-2</c:v>
+                    <c:v>0.44401386483779698</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -692,16 +695,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.34970880651974651</c:v>
+                  <c:v>0.14700895503484715</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65427814759042635</c:v>
+                  <c:v>0.51874426073426694</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29264641929465679</c:v>
+                  <c:v>0.67733097633142481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12137635598704148</c:v>
+                  <c:v>0.55341627633490109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2049,6 +2052,114 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="27">
+          <cell r="C27" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="E27" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>kMCT4</v>
+          </cell>
+          <cell r="C28">
+            <v>9.2535545750464687E-2</v>
+          </cell>
+          <cell r="D28">
+            <v>0.3541415185008206</v>
+          </cell>
+          <cell r="E28">
+            <v>0.75444268232926348</v>
+          </cell>
+          <cell r="F28">
+            <v>0.16916415025152015</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>1.2057455739979463E-2</v>
+          </cell>
+          <cell r="D29">
+            <v>5.7309495294150879E-2</v>
+          </cell>
+          <cell r="E29">
+            <v>0.39928208436858398</v>
+          </cell>
+          <cell r="F29">
+            <v>0.13741088889033834</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="D31" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="E31" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="F31" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="G31" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32" t="str">
+            <v>R1L</v>
+          </cell>
+          <cell r="D32">
+            <v>7.384890314233869E-2</v>
+          </cell>
+          <cell r="E32">
+            <v>5.0263555960985945E-2</v>
+          </cell>
+          <cell r="F32">
+            <v>6.3109847044927683E-2</v>
+          </cell>
+          <cell r="G32">
+            <v>8.0357873156810505E-2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="D33">
+            <v>2.3803754511435734E-2</v>
+          </cell>
+          <cell r="E33">
+            <v>2.3947765296666392E-2</v>
+          </cell>
+          <cell r="F33">
+            <v>1.0466686942143609E-2</v>
+          </cell>
+          <cell r="G33">
+            <v>1.4625933793160245E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2348,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5426EC7D-B74E-4953-AA3A-EC81D60A2FE4}">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,28 +2470,28 @@
         <v>2.0781114759556379E-2</v>
       </c>
       <c r="B1">
-        <v>3.3859492422262656E-3</v>
+        <v>3.4795161265732725E-3</v>
       </c>
       <c r="C1">
-        <v>0.12124917011238057</v>
+        <v>0.12115537047460399</v>
       </c>
       <c r="D1">
-        <v>3.5353019422967744E-2</v>
+        <v>3.5353019394421974E-2</v>
       </c>
       <c r="E1">
-        <v>4.065532119208215E-14</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F1">
-        <v>0.16526756951397378</v>
+        <v>0.22199757443326015</v>
       </c>
       <c r="G1">
-        <v>2.7441798126395123E-2</v>
+        <v>2.670202489455735E-2</v>
       </c>
       <c r="H1">
-        <v>0.11029092486311136</v>
+        <v>0.1193170263614496</v>
       </c>
       <c r="I1">
-        <v>6.3939051334378397E-2</v>
+        <v>0.1411298456931295</v>
       </c>
       <c r="J1">
         <v>2.356211808499348</v>
@@ -2392,22 +2503,22 @@
         <v>254686091.39268142</v>
       </c>
       <c r="M1">
-        <v>0.99715195420116631</v>
+        <v>0.99715195462511363</v>
       </c>
       <c r="N1">
-        <v>0.99781034114910905</v>
+        <v>0.99785346972528499</v>
       </c>
       <c r="O1">
-        <v>0.9944468637356233</v>
+        <v>0.99488532535510454</v>
       </c>
       <c r="P1">
-        <v>7.635343647626909E-2</v>
+        <v>7.6353436469702843E-2</v>
       </c>
       <c r="Q1">
-        <v>6.5831452608878835E-2</v>
+        <v>6.5139118584084318E-2</v>
       </c>
       <c r="R1">
-        <v>0.13365862371476647</v>
+        <v>0.13102591930261462</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -2415,28 +2526,28 @@
         <v>1.9731495213395425E-2</v>
       </c>
       <c r="B2">
-        <v>1.5802526621865268E-2</v>
+        <v>3.9270147990883662E-3</v>
       </c>
       <c r="C2">
-        <v>0.20701534191361032</v>
+        <v>0.21794698582814859</v>
       </c>
       <c r="D2">
-        <v>0.10057109997556396</v>
+        <v>0.10099996196568557</v>
       </c>
       <c r="E2">
-        <v>5.4649200648486607E-2</v>
+        <v>2.2205996670362198E-14</v>
       </c>
       <c r="F2">
-        <v>0.75743935087751979</v>
+        <v>0.11894110934795486</v>
       </c>
       <c r="G2">
-        <v>2.8011204481763162E-2</v>
+        <v>2.6561340578606808E-2</v>
       </c>
       <c r="H2">
-        <v>0.79999999999997051</v>
+        <v>4.8297651990673832E-2</v>
       </c>
       <c r="I2">
-        <v>5.6566723585759117E-8</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="J2">
         <v>5.6114128380547523</v>
@@ -2448,22 +2559,22 @@
         <v>161047158.1115168</v>
       </c>
       <c r="M2">
-        <v>0.99709416881346757</v>
+        <v>0.99709416769265702</v>
       </c>
       <c r="N2">
-        <v>0.99186795922175552</v>
+        <v>0.98619132265690701</v>
       </c>
       <c r="O2">
-        <v>0.94844785627890316</v>
+        <v>0.99689204548862798</v>
       </c>
       <c r="P2">
-        <v>7.6845094655211735E-2</v>
+        <v>7.6844094339646424E-2</v>
       </c>
       <c r="Q2">
-        <v>0.13352085399215621</v>
+        <v>0.16808999389977516</v>
       </c>
       <c r="R2">
-        <v>0.31898953671287356</v>
+        <v>7.8981907325062134E-2</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -2471,28 +2582,28 @@
         <v>2.0365465865092722E-2</v>
       </c>
       <c r="B3">
-        <v>4.0999697207729554E-3</v>
+        <v>3.5726191661664243E-3</v>
       </c>
       <c r="C3">
-        <v>0.23107594141950297</v>
+        <v>0.23160370685789064</v>
       </c>
       <c r="D3">
         <v>4.2510089797902627E-2</v>
       </c>
       <c r="E3">
-        <v>2.2204460492503131E-14</v>
+        <v>2.2219642502235133E-14</v>
       </c>
       <c r="F3">
-        <v>0.12641949916774603</v>
+        <v>0.10008818132332642</v>
       </c>
       <c r="G3">
-        <v>2.6525198939014415E-2</v>
+        <v>2.6572920741034615E-2</v>
       </c>
       <c r="H3">
-        <v>0.10000000000004027</v>
+        <v>6.0138209620568157E-2</v>
       </c>
       <c r="I3">
-        <v>2.2204553829255399E-14</v>
+        <v>2.2230487406924265E-14</v>
       </c>
       <c r="J3">
         <v>2.8545008818278075</v>
@@ -2504,22 +2615,22 @@
         <v>491427690.54543257</v>
       </c>
       <c r="M3">
-        <v>0.99564380029001576</v>
+        <v>0.99564380003670339</v>
       </c>
       <c r="N3">
-        <v>0.99377861626078023</v>
+        <v>0.99195335998266976</v>
       </c>
       <c r="O3">
-        <v>0.99157136517751154</v>
+        <v>0.9975015329873631</v>
       </c>
       <c r="P3">
-        <v>9.5112350342101901E-2</v>
+        <v>9.5112350349509781E-2</v>
       </c>
       <c r="Q3">
-        <v>0.11160789958693174</v>
+        <v>0.12686716616817512</v>
       </c>
       <c r="R3">
-        <v>0.14354756617798475</v>
+        <v>8.6621753913290897E-2</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -2527,28 +2638,28 @@
         <v>1.9994972552697242E-2</v>
       </c>
       <c r="B4">
-        <v>1.3159473866827963E-2</v>
+        <v>8.2261049334318315E-3</v>
       </c>
       <c r="C4">
-        <v>2.8908280002256674E-3</v>
+        <v>7.8238786162331871E-3</v>
       </c>
       <c r="D4">
-        <v>4.1791285747858259E-2</v>
+        <v>4.1448382824856529E-2</v>
       </c>
       <c r="E4">
-        <v>8.5606397144019304E-6</v>
+        <v>8.4517983628408446E-7</v>
       </c>
       <c r="F4">
-        <v>0.65964308762133117</v>
+        <v>0.38417933083549277</v>
       </c>
       <c r="G4">
-        <v>2.8011204416402567E-2</v>
+        <v>2.801117129673817E-2</v>
       </c>
       <c r="H4">
-        <v>0.59301604818926135</v>
+        <v>0.30888130275024206</v>
       </c>
       <c r="I4">
-        <v>2.9367147966718029E-14</v>
+        <v>4.1254209297634721E-14</v>
       </c>
       <c r="J4">
         <v>5.740537779224173</v>
@@ -2560,22 +2671,22 @@
         <v>142097848.58194768</v>
       </c>
       <c r="M4">
-        <v>0.99706208132712515</v>
+        <v>0.99706208406329411</v>
       </c>
       <c r="N4">
-        <v>0.95994945688506395</v>
+        <v>0.95451182918462252</v>
       </c>
       <c r="O4">
-        <v>0.98029025839829376</v>
+        <v>0.96755342148890255</v>
       </c>
       <c r="P4">
-        <v>7.8465805069870512E-2</v>
+        <v>7.8465803659368477E-2</v>
       </c>
       <c r="Q4">
-        <v>0.28043680746057709</v>
+        <v>0.29835113413949227</v>
       </c>
       <c r="R4">
-        <v>0.2008770089338153</v>
+        <v>0.25391303933089066</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
@@ -2610,28 +2721,28 @@
         <v>2.023647882476649E-2</v>
       </c>
       <c r="B5">
-        <v>2.1071973089867007E-2</v>
+        <v>1.7952384844695909E-2</v>
       </c>
       <c r="C5">
-        <v>0.32201921887946955</v>
+        <v>0.32513897643519724</v>
       </c>
       <c r="D5">
-        <v>9.2382191685178208E-2</v>
+        <v>9.267293693911316E-2</v>
       </c>
       <c r="E5">
-        <v>4.427518080653284E-14</v>
+        <v>3.37910782375764E-14</v>
       </c>
       <c r="F5">
-        <v>0.90149872550022647</v>
+        <v>0.77012992110925338</v>
       </c>
       <c r="G5">
-        <v>2.8011204481748556E-2</v>
+        <v>2.6757739839081779E-2</v>
       </c>
       <c r="H5">
-        <v>0.79999999999995575</v>
+        <v>0.67099227523245808</v>
       </c>
       <c r="I5">
-        <v>4.6974891390117743E-8</v>
+        <v>4.1482880168662724E-14</v>
       </c>
       <c r="J5">
         <v>3.2019451544874276</v>
@@ -2643,22 +2754,22 @@
         <v>629017289.17440271</v>
       </c>
       <c r="M5">
-        <v>0.99609224849316724</v>
+        <v>0.99609224845038047</v>
       </c>
       <c r="N5">
-        <v>0.98263465500878289</v>
+        <v>0.98228022729653697</v>
       </c>
       <c r="O5">
-        <v>0.99282153781040217</v>
+        <v>0.99321581530579128</v>
       </c>
       <c r="P5">
-        <v>9.1131006250945182E-2</v>
+        <v>9.1131006252957447E-2</v>
       </c>
       <c r="Q5">
-        <v>0.18634991218103297</v>
+        <v>0.18801244877525125</v>
       </c>
       <c r="R5">
-        <v>0.12052345033468065</v>
+        <v>0.11728586191248075</v>
       </c>
       <c r="T5" s="1">
         <f>1/51</f>
@@ -2699,28 +2810,28 @@
         <v>2.0231218059161282E-2</v>
       </c>
       <c r="B6">
-        <v>1.2726411003895198E-2</v>
+        <v>1.2730246353966567E-2</v>
       </c>
       <c r="C6">
-        <v>7.9607376073030608E-7</v>
+        <v>1.0000022208952447E-8</v>
       </c>
       <c r="D6">
-        <v>4.174095416704348E-2</v>
+        <v>4.1159362974046244E-2</v>
       </c>
       <c r="E6">
-        <v>4.2069139845619385E-14</v>
+        <v>2.2215914010445092E-14</v>
       </c>
       <c r="F6">
-        <v>0.40169262964972152</v>
+        <v>0.40192353025805466</v>
       </c>
       <c r="G6">
-        <v>2.8011146278234388E-2</v>
+        <v>2.7650327011609629E-2</v>
       </c>
       <c r="H6">
-        <v>0.19312507094591191</v>
+        <v>0.19368398855284627</v>
       </c>
       <c r="I6">
-        <v>3.161376008960995E-14</v>
+        <v>2.2237737766946569E-14</v>
       </c>
       <c r="J6">
         <v>4.8009905427717481</v>
@@ -2732,22 +2843,22 @@
         <v>149956135.49829885</v>
       </c>
       <c r="M6">
-        <v>0.99720079181976096</v>
+        <v>0.99720075071810876</v>
       </c>
       <c r="N6">
-        <v>0.98945602456020088</v>
+        <v>0.98945232763408242</v>
       </c>
       <c r="O6">
-        <v>0.99609505995529535</v>
+        <v>0.99609594278900127</v>
       </c>
       <c r="P6">
-        <v>7.5644702930155239E-2</v>
+        <v>7.5644718612386044E-2</v>
       </c>
       <c r="Q6">
-        <v>0.15400438425648463</v>
+        <v>0.1539517645319253</v>
       </c>
       <c r="R6">
-        <v>0.10852155997897234</v>
+        <v>0.10849575202156349</v>
       </c>
       <c r="T6" s="1">
         <f>1/47</f>
@@ -2785,28 +2896,28 @@
         <v>2.0352218032308276E-2</v>
       </c>
       <c r="B7">
-        <v>1.1340575606028381E-2</v>
+        <v>1.1336378651585302E-2</v>
       </c>
       <c r="C7">
-        <v>1.6564456468285828E-2</v>
+        <v>1.6568061839038396E-2</v>
       </c>
       <c r="D7">
-        <v>4.5051654933822564E-2</v>
+        <v>4.5873244781070611E-2</v>
       </c>
       <c r="E7">
-        <v>3.9890355474612253E-6</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F7">
-        <v>7.7089388890080088E-2</v>
+        <v>7.6265635306323493E-2</v>
       </c>
       <c r="G7">
-        <v>2.7685421155182077E-2</v>
+        <v>2.7659978894551168E-2</v>
       </c>
       <c r="H7">
-        <v>0.1000000085379574</v>
+        <v>9.8533251240757375E-2</v>
       </c>
       <c r="I7">
-        <v>4.0699336460787677E-14</v>
+        <v>2.2204979238374094E-14</v>
       </c>
       <c r="J7">
         <v>1.952898836424503</v>
@@ -2818,22 +2929,22 @@
         <v>132744891.08503906</v>
       </c>
       <c r="M7">
-        <v>0.99900216781254869</v>
+        <v>0.99900216768483463</v>
       </c>
       <c r="N7">
-        <v>0.99812741596588161</v>
+        <v>0.99812720704547231</v>
       </c>
       <c r="O7">
-        <v>0.99654244162299332</v>
+        <v>0.9965996225501188</v>
       </c>
       <c r="P7">
-        <v>4.4448078348034686E-2</v>
+        <v>4.4448064950350752E-2</v>
       </c>
       <c r="Q7">
-        <v>6.3835921086169298E-2</v>
+        <v>6.3844926603594698E-2</v>
       </c>
       <c r="R7">
-        <v>9.2284127875690986E-2</v>
+        <v>9.123185443573037E-2</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -2841,28 +2952,28 @@
         <v>2.0420572162940933E-2</v>
       </c>
       <c r="B8">
-        <v>2.2011934502524991E-2</v>
+        <v>2.8455085625926618E-2</v>
       </c>
       <c r="C8">
-        <v>0.20827938796859147</v>
+        <v>0.19463910134944526</v>
       </c>
       <c r="D8">
-        <v>6.5007089336341681E-2</v>
+        <v>6.5007089083382458E-2</v>
       </c>
       <c r="E8">
-        <v>8.9208071557410562E-2</v>
+        <v>2.4898037270932147E-3</v>
       </c>
       <c r="F8">
-        <v>7.6601701277703785E-2</v>
+        <v>0.23965150048870829</v>
       </c>
       <c r="G8">
-        <v>2.662943691424717E-2</v>
+        <v>2.7079786776221599E-2</v>
       </c>
       <c r="H8">
-        <v>0.12465136592002039</v>
+        <v>0.57170256654956031</v>
       </c>
       <c r="I8">
-        <v>2.2204565693651495E-14</v>
+        <v>9.941866654942422E-7</v>
       </c>
       <c r="J8">
         <v>2.4430206679346318</v>
@@ -2874,22 +2985,22 @@
         <v>457955160.74923623</v>
       </c>
       <c r="M8">
-        <v>0.99838221935495342</v>
+        <v>0.99837928576034285</v>
       </c>
       <c r="N8">
-        <v>0.99734885460777134</v>
+        <v>0.99840550035107978</v>
       </c>
       <c r="O8">
-        <v>0.99710079907135296</v>
+        <v>0.97812854760325485</v>
       </c>
       <c r="P8">
-        <v>5.7537209681503235E-2</v>
+        <v>5.751194069035951E-2</v>
       </c>
       <c r="Q8">
-        <v>7.2381879606454258E-2</v>
+        <v>5.6148136508280842E-2</v>
       </c>
       <c r="R8">
-        <v>7.7702559747089103E-2</v>
+        <v>0.21109361441809982</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -2897,28 +3008,28 @@
         <v>1.9856607624304978E-2</v>
       </c>
       <c r="B9">
-        <v>7.071676434255149E-3</v>
+        <v>6.9060525830266173E-2</v>
       </c>
       <c r="C9">
-        <v>0.32154985009364861</v>
+        <v>0.25801108459089117</v>
       </c>
       <c r="D9">
-        <v>7.4905465924434506E-2</v>
+        <v>7.4230058620422631E-2</v>
       </c>
       <c r="E9">
-        <v>9.9999999999977801E-2</v>
+        <v>2.9250814687839763E-14</v>
       </c>
       <c r="F9">
-        <v>0.28309933055226932</v>
+        <v>3.2253352307515293</v>
       </c>
       <c r="G9">
-        <v>2.801120448177051E-2</v>
+        <v>2.8011204478663298E-2</v>
       </c>
       <c r="H9">
-        <v>0.79999999999997784</v>
+        <v>9.750654659613712</v>
       </c>
       <c r="I9">
-        <v>2.2204917090344473E-14</v>
+        <v>8.9507003447047568E-9</v>
       </c>
       <c r="J9">
         <v>4.3363113643580764</v>
@@ -2930,22 +3041,22 @@
         <v>1205583684.8478703</v>
       </c>
       <c r="M9">
-        <v>0.99455790233076147</v>
+        <v>0.99455792352757189</v>
       </c>
       <c r="N9">
-        <v>0.95173244711098659</v>
+        <v>0.95888050748856335</v>
       </c>
       <c r="O9">
-        <v>0.97321577031869899</v>
+        <v>0.98176164041495118</v>
       </c>
       <c r="P9">
-        <v>0.10398786762200615</v>
+        <v>0.10398649260370561</v>
       </c>
       <c r="Q9">
-        <v>0.31864354729954852</v>
+        <v>0.29760772423271709</v>
       </c>
       <c r="R9">
-        <v>0.24525259099802013</v>
+        <v>0.19874222923660653</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -2953,28 +3064,28 @@
         <v>1.9607843138025917E-2</v>
       </c>
       <c r="B10">
-        <v>8.1859985050619956E-3</v>
+        <v>1.2323139929023586E-2</v>
       </c>
       <c r="C10">
-        <v>1.9944039440557171E-2</v>
+        <v>1.5598276110641449E-2</v>
       </c>
       <c r="D10">
-        <v>6.2002426913260425E-2</v>
+        <v>6.230835978644024E-2</v>
       </c>
       <c r="E10">
-        <v>2.6273039513340247E-2</v>
+        <v>1.0730907695642397E-3</v>
       </c>
       <c r="F10">
-        <v>0.85557210696149466</v>
+        <v>1.2599420336012488</v>
       </c>
       <c r="G10">
-        <v>2.8011204481770337E-2</v>
+        <v>2.7334357934778661E-2</v>
       </c>
       <c r="H10">
-        <v>0.79999999999997762</v>
+        <v>1.4553538898315348</v>
       </c>
       <c r="I10">
-        <v>1.9251948922425374E-5</v>
+        <v>4.0807233768722193E-14</v>
       </c>
       <c r="J10">
         <v>3.6193816110419976</v>
@@ -2986,22 +3097,22 @@
         <v>83209857.156356871</v>
       </c>
       <c r="M10">
-        <v>0.99668230762726062</v>
+        <v>0.99668267063118265</v>
       </c>
       <c r="N10">
-        <v>0.98901753412808713</v>
+        <v>0.98967172348163557</v>
       </c>
       <c r="O10">
-        <v>0.99266222127078774</v>
+        <v>0.99072332294345355</v>
       </c>
       <c r="P10">
-        <v>8.1027876361946971E-2</v>
+        <v>8.1022592759074114E-2</v>
       </c>
       <c r="Q10">
-        <v>0.16848414188151448</v>
+        <v>0.1457665294218416</v>
       </c>
       <c r="R10">
-        <v>0.17628609246706237</v>
+        <v>0.13578312841773169</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -3009,10 +3120,10 @@
         <v>1.9607868588388273E-2</v>
       </c>
       <c r="B11">
-        <v>1.6018889310917536E-2</v>
+        <v>1.601888853618769E-2</v>
       </c>
       <c r="C11">
-        <v>0.16415849047657283</v>
+        <v>0.1641584912521373</v>
       </c>
       <c r="D11">
         <v>4.5283825219602628E-2</v>
@@ -3021,16 +3132,16 @@
         <v>2.2204460492503131E-14</v>
       </c>
       <c r="F11">
-        <v>0.11219421846189438</v>
+        <v>0.11219420894660005</v>
       </c>
       <c r="G11">
-        <v>2.8009227956620524E-2</v>
+        <v>2.6739389223432025E-2</v>
       </c>
       <c r="H11">
-        <v>0.19118160273525966</v>
+        <v>0.19245141659030984</v>
       </c>
       <c r="I11">
-        <v>2.2206821263400803E-14</v>
+        <v>2.2206781588809361E-14</v>
       </c>
       <c r="J11">
         <v>2.8612100103634148</v>
@@ -3042,22 +3153,22 @@
         <v>44059879.020455331</v>
       </c>
       <c r="M11">
-        <v>0.99213822043396427</v>
+        <v>0.99213822043396482</v>
       </c>
       <c r="N11">
-        <v>0.99410838199577845</v>
+        <v>0.99410838184506134</v>
       </c>
       <c r="O11">
-        <v>0.99319548298489735</v>
+        <v>0.99319548348425291</v>
       </c>
       <c r="P11">
-        <v>0.12446931357457514</v>
+        <v>0.12446931357457527</v>
       </c>
       <c r="Q11">
-        <v>0.11716632821090975</v>
+        <v>0.11716632920010855</v>
       </c>
       <c r="R11">
-        <v>0.14608669522659817</v>
+        <v>0.14608669072309458</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -3065,28 +3176,28 @@
         <v>1.9955136692618142E-2</v>
       </c>
       <c r="B12">
-        <v>7.9999999999973412E-2</v>
+        <v>7.9999999969555299E-2</v>
       </c>
       <c r="C12">
-        <v>2.0256046140424044</v>
+        <v>2.025498154431006</v>
       </c>
       <c r="D12">
-        <v>3.7430807982107454E-2</v>
+        <v>3.7430807982120715E-2</v>
       </c>
       <c r="E12">
-        <v>2.774528106152081E-14</v>
+        <v>4.813190262085224E-11</v>
       </c>
       <c r="F12">
-        <v>0.17801410729971484</v>
+        <v>0.17802513032889813</v>
       </c>
       <c r="G12">
-        <v>2.7545144210098283E-2</v>
+        <v>2.6557682885802104E-2</v>
       </c>
       <c r="H12">
-        <v>0.37267132757820554</v>
+        <v>0.37369127504783234</v>
       </c>
       <c r="I12">
-        <v>2.8277363175229545E-14</v>
+        <v>4.2438187820793242E-14</v>
       </c>
       <c r="J12">
         <v>5.3408895358905601</v>
@@ -3098,22 +3209,22 @@
         <v>1300249383.1199305</v>
       </c>
       <c r="M12">
-        <v>0.97974716503179859</v>
+        <v>0.97974716357598268</v>
       </c>
       <c r="N12">
-        <v>0.92111017235374715</v>
+        <v>0.92111167361335022</v>
       </c>
       <c r="O12">
-        <v>0.96654677642923925</v>
+        <v>0.96654862729160018</v>
       </c>
       <c r="P12">
-        <v>0.20055741419657805</v>
+        <v>0.20055742706207924</v>
       </c>
       <c r="Q12">
-        <v>0.38893342491619531</v>
+        <v>0.38892998015242602</v>
       </c>
       <c r="R12">
-        <v>0.25542601154025274</v>
+        <v>0.25541943931821498</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -3121,28 +3232,28 @@
         <v>1.9932134010064936E-2</v>
       </c>
       <c r="B13">
-        <v>9.6264518394332411E-3</v>
+        <v>8.6403546782031753E-3</v>
       </c>
       <c r="C13">
-        <v>6.9009978894920887E-2</v>
+        <v>6.9996504707704105E-2</v>
       </c>
       <c r="D13">
-        <v>4.1899008128684898E-2</v>
+        <v>4.117029077902333E-2</v>
       </c>
       <c r="E13">
-        <v>2.2204460492503131E-14</v>
+        <v>5.5774294888870558E-10</v>
       </c>
       <c r="F13">
-        <v>0.17272057466079108</v>
+        <v>0.14710121465685502</v>
       </c>
       <c r="G13">
-        <v>2.7951825513667101E-2</v>
+        <v>2.7606148348276426E-2</v>
       </c>
       <c r="H13">
-        <v>0.58800531838989667</v>
+        <v>0.48172107020411004</v>
       </c>
       <c r="I13">
-        <v>2.220470571366802E-14</v>
+        <v>3.1310055328609909E-14</v>
       </c>
       <c r="J13">
         <v>4.079138265678818</v>
@@ -3154,22 +3265,22 @@
         <v>566450101.24093688</v>
       </c>
       <c r="M13">
-        <v>0.99898533054488681</v>
+        <v>0.99898533074451068</v>
       </c>
       <c r="N13">
-        <v>0.99766732036658889</v>
+        <v>0.99701139548014506</v>
       </c>
       <c r="O13">
-        <v>0.94220867602833114</v>
+        <v>0.949541110127199</v>
       </c>
       <c r="P13">
-        <v>4.4815903396743927E-2</v>
+        <v>4.4815903611969979E-2</v>
       </c>
       <c r="Q13">
-        <v>7.4461539814194844E-2</v>
+        <v>8.2400008207427697E-2</v>
       </c>
       <c r="R13">
-        <v>0.34675203053639719</v>
+        <v>0.32512088803992523</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -3177,28 +3288,28 @@
         <v>1.9701617767527744E-2</v>
       </c>
       <c r="B14">
-        <v>5.2196428401127112E-3</v>
+        <v>4.8323620306448935E-3</v>
       </c>
       <c r="C14">
-        <v>5.0678581346943127E-3</v>
+        <v>5.4563962150907331E-3</v>
       </c>
       <c r="D14">
-        <v>3.8812904714334524E-2</v>
+        <v>4.0812904702452656E-2</v>
       </c>
       <c r="E14">
-        <v>2.2204460492503131E-14</v>
+        <v>1.7651220104339856E-5</v>
       </c>
       <c r="F14">
-        <v>4.3233912111200291E-2</v>
+        <v>3.1617351973594027E-2</v>
       </c>
       <c r="G14">
-        <v>2.6525198939014252E-2</v>
+        <v>2.725000798928098E-2</v>
       </c>
       <c r="H14">
-        <v>0.10000000000002221</v>
+        <v>4.7124138988605048E-2</v>
       </c>
       <c r="I14">
-        <v>2.2204663392748155E-14</v>
+        <v>1.6211893547391038E-5</v>
       </c>
       <c r="J14">
         <v>4.5658015908569123</v>
@@ -3210,22 +3321,22 @@
         <v>350999697.1980691</v>
       </c>
       <c r="M14">
-        <v>0.9920818465232899</v>
+        <v>0.99208181807768536</v>
       </c>
       <c r="N14">
-        <v>0.99532048210912372</v>
+        <v>0.99508377256621872</v>
       </c>
       <c r="O14">
-        <v>0.98395376288691061</v>
+        <v>0.99253225813286505</v>
       </c>
       <c r="P14">
-        <v>0.12573147815758959</v>
+        <v>0.12573170714751689</v>
       </c>
       <c r="Q14">
-        <v>0.10080560098090117</v>
+        <v>0.10237015179103715</v>
       </c>
       <c r="R14">
-        <v>0.18327511028642562</v>
+        <v>0.12637696756741412</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -3233,28 +3344,28 @@
         <v>1.9647451233942632E-2</v>
       </c>
       <c r="B15">
-        <v>9.080612905371932E-3</v>
+        <v>1.1560450572118007E-2</v>
       </c>
       <c r="C15">
-        <v>8.7365180710462828E-2</v>
+        <v>8.4848356183085338E-2</v>
       </c>
       <c r="D15">
-        <v>8.8738460064248847E-2</v>
+        <v>8.8738451615117273E-2</v>
       </c>
       <c r="E15">
-        <v>8.9183453825783033E-4</v>
+        <v>2.407360763413255E-14</v>
       </c>
       <c r="F15">
-        <v>9.1180234746986472E-2</v>
+        <v>0.15210747569666191</v>
       </c>
       <c r="G15">
-        <v>2.6525198939014245E-2</v>
+        <v>2.6611480178405034E-2</v>
       </c>
       <c r="H15">
-        <v>0.10000000000002221</v>
+        <v>0.22793467277447976</v>
       </c>
       <c r="I15">
-        <v>2.2204670740703577E-14</v>
+        <v>3.8305931461935391E-14</v>
       </c>
       <c r="J15">
         <v>6.1031742274447058</v>
@@ -3266,22 +3377,22 @@
         <v>621934179.43162954</v>
       </c>
       <c r="M15">
-        <v>0.99882160641446005</v>
+        <v>0.99882163160938198</v>
       </c>
       <c r="N15">
-        <v>0.9900136555432858</v>
+        <v>0.99270388667667397</v>
       </c>
       <c r="O15">
-        <v>0.98174408296885385</v>
+        <v>0.96037915720805644</v>
       </c>
       <c r="P15">
-        <v>4.8286825124937288E-2</v>
+        <v>4.8286264033468369E-2</v>
       </c>
       <c r="Q15">
-        <v>0.14097755866553399</v>
+        <v>0.12081206714507217</v>
       </c>
       <c r="R15">
-        <v>0.19257911283467274</v>
+        <v>0.28282810134363656</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -3289,28 +3400,28 @@
         <v>2.0254106371624593E-2</v>
       </c>
       <c r="B16">
-        <v>4.7934695092865711E-3</v>
+        <v>4.4712314332643145E-2</v>
       </c>
       <c r="C16">
-        <v>0.3785738050665487</v>
+        <v>0.33865466146936779</v>
       </c>
       <c r="D16">
-        <v>0.1002757944610032</v>
+        <v>0.10027579446083579</v>
       </c>
       <c r="E16">
         <v>2.2204460492503131E-14</v>
       </c>
       <c r="F16">
-        <v>0.17837070242918812</v>
+        <v>1.8828390630124936</v>
       </c>
       <c r="G16">
-        <v>2.8011204481770496E-2</v>
+        <v>2.8011204481770472E-2</v>
       </c>
       <c r="H16">
-        <v>0.79999999999997784</v>
+        <v>9.9999999999999787</v>
       </c>
       <c r="I16">
-        <v>2.2278702887509174E-14</v>
+        <v>4.8819468832966442E-10</v>
       </c>
       <c r="J16">
         <v>2.8975994027540488</v>
@@ -3322,22 +3433,22 @@
         <v>818269300.73777747</v>
       </c>
       <c r="M16">
-        <v>0.99463967389519259</v>
+        <v>0.99463967383988361</v>
       </c>
       <c r="N16">
-        <v>0.9779234311986813</v>
+        <v>0.985550803068721</v>
       </c>
       <c r="O16">
-        <v>0.98190372641679557</v>
+        <v>0.96924532881281233</v>
       </c>
       <c r="P16">
-        <v>0.1031191612413374</v>
+        <v>0.10311916123851592</v>
       </c>
       <c r="Q16">
-        <v>0.23149875741370632</v>
+        <v>0.19758020614782132</v>
       </c>
       <c r="R16">
-        <v>0.24659754344648577</v>
+        <v>0.24695341960909117</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -3345,28 +3456,28 @@
         <v>2.0450312385911232E-2</v>
       </c>
       <c r="B17">
-        <v>9.7343720970810531E-3</v>
+        <v>8.923362709430319E-3</v>
       </c>
       <c r="C17">
-        <v>7.1379381093056033E-4</v>
+        <v>1.5268678764787176E-3</v>
       </c>
       <c r="D17">
-        <v>4.2219008518467098E-2</v>
+        <v>4.1485128594566129E-2</v>
       </c>
       <c r="E17">
-        <v>2.6561025200262177E-14</v>
+        <v>5.0322381980571912E-5</v>
       </c>
       <c r="F17">
-        <v>0.22421730909372353</v>
+        <v>0.20035088574662624</v>
       </c>
       <c r="G17">
-        <v>2.6525198939018609E-2</v>
+        <v>2.8011204470866559E-2</v>
       </c>
       <c r="H17">
-        <v>0.10000000000002657</v>
+        <v>7.8836529817834081E-2</v>
       </c>
       <c r="I17">
-        <v>2.656376954120298E-14</v>
+        <v>4.4177389542715639E-14</v>
       </c>
       <c r="J17">
         <v>4.9944093087717132</v>
@@ -3378,22 +3489,22 @@
         <v>87097810.529802099</v>
       </c>
       <c r="M17">
-        <v>0.9968391250237093</v>
+        <v>0.99683910813226995</v>
       </c>
       <c r="N17">
-        <v>0.98794566989083576</v>
+        <v>0.9867659528053907</v>
       </c>
       <c r="O17">
-        <v>0.99807141390182319</v>
+        <v>0.99860625939314263</v>
       </c>
       <c r="P17">
-        <v>8.2129028156743722E-2</v>
+        <v>8.2129228260778453E-2</v>
       </c>
       <c r="Q17">
-        <v>0.16090459930902531</v>
+        <v>0.16814307852940949</v>
       </c>
       <c r="R17">
-        <v>7.7891100393209761E-2</v>
+        <v>6.8346251598520716E-2</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -3401,28 +3512,28 @@
         <v>1.9778014887334602E-2</v>
       </c>
       <c r="B18">
-        <v>5.2535989253727731E-2</v>
+        <v>5.2535975976707519E-2</v>
       </c>
       <c r="C18">
-        <v>0.12208853471445501</v>
+        <v>0.12208854799275491</v>
       </c>
       <c r="D18">
         <v>7.614398766366591E-2</v>
       </c>
       <c r="E18">
-        <v>2.2204460492503131E-14</v>
+        <v>2.2204554673015353E-14</v>
       </c>
       <c r="F18">
-        <v>0.72928402309098084</v>
+        <v>0.72928382779249157</v>
       </c>
       <c r="G18">
-        <v>2.7772524804142718E-2</v>
+        <v>2.7631055008154236E-2</v>
       </c>
       <c r="H18">
-        <v>0.57976174400218183</v>
+        <v>0.57990303234465335</v>
       </c>
       <c r="I18">
-        <v>2.22045022460376E-14</v>
+        <v>2.2204460492503134E-14</v>
       </c>
       <c r="J18">
         <v>3.2428732950368784</v>
@@ -3434,22 +3545,22 @@
         <v>776346501.63544285</v>
       </c>
       <c r="M18">
-        <v>0.99704775731930573</v>
+        <v>0.99704775731930395</v>
       </c>
       <c r="N18">
-        <v>0.97850366062719285</v>
+        <v>0.97850365971070608</v>
       </c>
       <c r="O18">
-        <v>0.99708218322815889</v>
+        <v>0.99708218383603886</v>
       </c>
       <c r="P18">
-        <v>7.8493392353226402E-2</v>
+        <v>7.8493392353228289E-2</v>
       </c>
       <c r="Q18">
-        <v>0.20798422974981115</v>
+        <v>0.20798423390640772</v>
       </c>
       <c r="R18">
-        <v>7.9032408155446793E-2</v>
+        <v>7.9032400824502233E-2</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -3460,25 +3571,25 @@
         <v>7.9999999999977797E-2</v>
       </c>
       <c r="C19">
-        <v>1.0000022204957719E-8</v>
+        <v>8.4733543146847997E-3</v>
       </c>
       <c r="D19">
         <v>3.8974783538952548E-2</v>
       </c>
       <c r="E19">
-        <v>2.2204460807475865E-14</v>
+        <v>2.2204473777882011E-14</v>
       </c>
       <c r="F19">
-        <v>9.7745588024049479E-2</v>
+        <v>7.4930334020398101E-2</v>
       </c>
       <c r="G19">
         <v>2.6525198939014245E-2</v>
       </c>
       <c r="H19">
-        <v>0.10000000000002221</v>
+        <v>1.0000022204521512E-8</v>
       </c>
       <c r="I19">
-        <v>2.2204555356114175E-14</v>
+        <v>6.715716657390027E-3</v>
       </c>
       <c r="J19">
         <v>2.8613040667312468</v>
@@ -3490,22 +3601,22 @@
         <v>13771138.993237138</v>
       </c>
       <c r="M19">
-        <v>0.99695207360049998</v>
+        <v>0.99722462033937131</v>
       </c>
       <c r="N19">
-        <v>0.91369621682872326</v>
+        <v>0.90128299723359717</v>
       </c>
       <c r="O19">
-        <v>0.95847563980812811</v>
+        <v>0.8834006306256792</v>
       </c>
       <c r="P19">
-        <v>0.14265588967869366</v>
+        <v>9.6944412290866436E-2</v>
       </c>
       <c r="Q19">
-        <v>0.52736600662597077</v>
+        <v>0.48904516178599816</v>
       </c>
       <c r="R19">
-        <v>0.73136744293789402</v>
+        <v>0.49148438074501466</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -3513,10 +3624,10 @@
         <v>2.025226724750458E-2</v>
       </c>
       <c r="B20">
-        <v>3.6610391490975655E-2</v>
+        <v>3.661038817423995E-2</v>
       </c>
       <c r="C20">
-        <v>0.58530338882665311</v>
+        <v>0.58530339194918313</v>
       </c>
       <c r="D20">
         <v>4.2860723219890554E-2</v>
@@ -3525,16 +3636,16 @@
         <v>9.9999999999977801E-2</v>
       </c>
       <c r="F20">
-        <v>0.13494302069264516</v>
+        <v>0.13494299556910744</v>
       </c>
       <c r="G20">
-        <v>2.6749603680624949E-2</v>
+        <v>2.6595818555612983E-2</v>
       </c>
       <c r="H20">
-        <v>0.20570831653393457</v>
+        <v>0.20586204465426139</v>
       </c>
       <c r="I20">
-        <v>2.2204512590459397E-14</v>
+        <v>2.2204503459977956E-14</v>
       </c>
       <c r="J20">
         <v>2.4328816932437634</v>
@@ -3546,22 +3657,22 @@
         <v>898068381.93210459</v>
       </c>
       <c r="M20">
-        <v>0.99345692483621739</v>
+        <v>0.99345692483643755</v>
       </c>
       <c r="N20">
-        <v>0.98644924395872025</v>
+        <v>0.98644924290192071</v>
       </c>
       <c r="O20">
-        <v>0.99602689555396506</v>
+        <v>0.99602689796079291</v>
       </c>
       <c r="P20">
-        <v>0.11612890078225724</v>
+        <v>0.11612890077785666</v>
       </c>
       <c r="Q20">
-        <v>0.16359251960162435</v>
+        <v>0.16359252591784523</v>
       </c>
       <c r="R20">
-        <v>0.10046396988442108</v>
+        <v>0.10046394420079181</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -3569,28 +3680,28 @@
         <v>1.9645457395348342E-2</v>
       </c>
       <c r="B21">
-        <v>7.9999999999955759E-2</v>
+        <v>7.9999999999977797E-2</v>
       </c>
       <c r="C21">
-        <v>2.4878310327833182</v>
+        <v>2.4870592214691891</v>
       </c>
       <c r="D21">
-        <v>4.3368027883474623E-2</v>
+        <v>4.3368027883496717E-2</v>
       </c>
       <c r="E21">
-        <v>2.2345198295408543E-14</v>
+        <v>2.2205191754949247E-14</v>
       </c>
       <c r="F21">
-        <v>0.2171379979147679</v>
+        <v>0.21720927390656489</v>
       </c>
       <c r="G21">
-        <v>2.8011204396358586E-2</v>
+        <v>2.6542277456997741E-2</v>
       </c>
       <c r="H21">
-        <v>0.27810077379309728</v>
+        <v>0.27970150312629444</v>
       </c>
       <c r="I21">
-        <v>4.4272338651206418E-14</v>
+        <v>2.220448407366131E-14</v>
       </c>
       <c r="J21">
         <v>2.9741152430411644</v>
@@ -3602,22 +3713,22 @@
         <v>1569235476.0781155</v>
       </c>
       <c r="M21">
-        <v>0.98728130917477275</v>
+        <v>0.98728130885977849</v>
       </c>
       <c r="N21">
-        <v>0.98447128884658253</v>
+        <v>0.98447514473401299</v>
       </c>
       <c r="O21">
-        <v>0.99243801268993947</v>
+        <v>0.99243473711185037</v>
       </c>
       <c r="P21">
-        <v>0.15890606776799515</v>
+        <v>0.15890607310726296</v>
       </c>
       <c r="Q21">
-        <v>0.17690769259613348</v>
+        <v>0.17688630763901789</v>
       </c>
       <c r="R21">
-        <v>0.1264582079387879</v>
+        <v>0.12648227289179581</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -3625,28 +3736,28 @@
         <v>1.9998083024111244E-2</v>
       </c>
       <c r="B22">
-        <v>7.9999999999960422E-2</v>
+        <v>7.9999999999977797E-2</v>
       </c>
       <c r="C22">
-        <v>2.4607140471137514</v>
+        <v>2.4607134617885431</v>
       </c>
       <c r="D22">
-        <v>4.4657955198495324E-2</v>
+        <v>4.4657955198512699E-2</v>
       </c>
       <c r="E22">
-        <v>3.9579738108237456E-14</v>
+        <v>2.220960075234407E-14</v>
       </c>
       <c r="F22">
-        <v>0.26729345395673082</v>
+        <v>0.26729351310643173</v>
       </c>
       <c r="G22">
-        <v>2.7544990132752793E-2</v>
+        <v>2.655305918638852E-2</v>
       </c>
       <c r="H22">
-        <v>0.3718250002176654</v>
+        <v>0.37281704729437759</v>
       </c>
       <c r="I22">
-        <v>3.9577432380187527E-14</v>
+        <v>2.2204943639415854E-14</v>
       </c>
       <c r="J22">
         <v>3.8163808997580695</v>
@@ -3658,22 +3769,22 @@
         <v>911747954.02784622</v>
       </c>
       <c r="M22">
-        <v>0.9943721618267416</v>
+        <v>0.99437216182671762</v>
       </c>
       <c r="N22">
-        <v>0.96042882071302771</v>
+        <v>0.96042882358742254</v>
       </c>
       <c r="O22">
-        <v>0.99545328220916307</v>
+        <v>0.99545327999674993</v>
       </c>
       <c r="P22">
-        <v>0.10664431575469255</v>
+        <v>0.10664431575955506</v>
       </c>
       <c r="Q22">
-        <v>0.28177654334197055</v>
+        <v>0.28177653343532372</v>
       </c>
       <c r="R22">
-        <v>9.576477951739458E-2</v>
+        <v>9.5764802955078374E-2</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -3721,7 +3832,7 @@
       </c>
       <c r="T23" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U23" t="str">
         <f t="shared" si="0"/>
@@ -3798,7 +3909,7 @@
       </c>
       <c r="T24" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Lower</v>
       </c>
       <c r="U24" t="str">
         <f t="shared" si="0"/>
@@ -3986,7 +4097,7 @@
       </c>
       <c r="T27" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Lower</v>
       </c>
       <c r="U27" t="str">
         <f t="shared" si="0"/>
@@ -4015,27 +4126,27 @@
       </c>
       <c r="C28">
         <f>AVERAGE(B$1:B$3)</f>
-        <v>7.7628151949548294E-3</v>
+        <v>3.6597166972760207E-3</v>
       </c>
       <c r="D28">
         <f>AVERAGE(B$4:B$6)</f>
-        <v>1.5652619320196723E-2</v>
+        <v>1.2969578710698102E-2</v>
       </c>
       <c r="E28">
         <f>AVERAGE(B$7:B$12,B$17:B$19)</f>
-        <v>3.1877715078838673E-2</v>
+        <v>3.9850373025406699E-2</v>
       </c>
       <c r="F28">
         <f>AVERAGE(B$13:B$16)</f>
-        <v>7.1800442735511141E-3</v>
+        <v>1.7436370403402304E-2</v>
       </c>
       <c r="G28">
         <f>B$20</f>
-        <v>3.6610391490975655E-2</v>
+        <v>3.661038817423995E-2</v>
       </c>
       <c r="H28">
         <f>AVERAGE(B$21:B$22)</f>
-        <v>7.9999999999958091E-2</v>
+        <v>7.9999999999977797E-2</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="2"/>
@@ -4047,7 +4158,7 @@
       </c>
       <c r="P28" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="0"/>
@@ -4063,7 +4174,7 @@
       </c>
       <c r="T28" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U28" t="str">
         <f t="shared" si="0"/>
@@ -4089,23 +4200,23 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>STDEV(B$1:B$3)/SQRT(COUNT(B$1:B$3))</f>
-        <v>4.0251366925833192E-3</v>
+        <v>1.3632467423976377E-4</v>
       </c>
       <c r="D29">
         <f>STDEV(B$4:B$6)/SQRT(COUNT(B$4:B$6))</f>
-        <v>2.7125592049724646E-3</v>
+        <v>2.8102841025300172E-3</v>
       </c>
       <c r="E29">
         <f>STDEV(B$7:B$12,B$17:B$19)/SQRT(COUNT(B$7:B$12,B$17:B$19))</f>
-        <v>1.020338152597138E-2</v>
+        <v>1.0181144930654133E-2</v>
       </c>
       <c r="F29">
         <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
-        <v>1.2628005908930579E-3</v>
+        <v>9.1957167148318739E-3</v>
       </c>
       <c r="H29">
         <f>STDEV(B$21:B$22)/SQRT(COUNT(B$21:B$22))</f>
-        <v>2.3314683517128283E-15</v>
+        <v>0</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="2"/>
@@ -4183,7 +4294,7 @@
       </c>
       <c r="T30" t="str">
         <f t="shared" si="0"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
       <c r="U30" t="str">
         <f t="shared" si="0"/>
@@ -4243,7 +4354,7 @@
       </c>
       <c r="R31" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="0"/>
@@ -4280,27 +4391,27 @@
       </c>
       <c r="D32">
         <f>AVERAGE(C$1:C$3)</f>
-        <v>0.18644681781516462</v>
+        <v>0.19023535438688108</v>
       </c>
       <c r="E32">
         <f>AVERAGE(C$4:C$6)</f>
-        <v>0.10830361431781865</v>
+        <v>0.11098762168381754</v>
       </c>
       <c r="F32">
         <f>AVERAGE(C$7:C$12,C$17:C$19)</f>
-        <v>0.31987813077949645</v>
+        <v>0.31184021552856422</v>
       </c>
       <c r="G32">
         <f>AVERAGE(C$13:C$16)</f>
-        <v>0.13500420570165667</v>
+        <v>0.12473897964381199</v>
       </c>
       <c r="H32">
         <f>C$20</f>
-        <v>0.58530338882665311</v>
+        <v>0.58530339194918313</v>
       </c>
       <c r="I32">
         <f>AVERAGE(C$21:C$22)</f>
-        <v>2.4742725399485348</v>
+        <v>2.4738863416288659</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="2"/>
@@ -4328,7 +4439,7 @@
       </c>
       <c r="T32" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="0"/>
@@ -4354,23 +4465,23 @@
     <row r="33" spans="4:31" x14ac:dyDescent="0.25">
       <c r="D33">
         <f>STDEV(C$1:C$3)/SQRT(COUNT(C$1:C$3))</f>
-        <v>3.333055685917452E-2</v>
+        <v>3.4764251947037965E-2</v>
       </c>
       <c r="E33">
         <f>STDEV(C$4:C$6)/SQRT(COUNT(C$4:C$6))</f>
-        <v>0.10686105900654044</v>
+        <v>0.10709949468666879</v>
       </c>
       <c r="F33">
         <f>STDEV(C$7:C$12,C$17:C$19)/SQRT(COUNT(C$7:C$12,C$17:C$19))</f>
-        <v>0.21639331380716118</v>
+        <v>0.21648529436558617</v>
       </c>
       <c r="G33">
         <f>STDEV(C$13:C$16)/SQRT(COUNT(C$13:C$16))</f>
-        <v>8.308345143476073E-2</v>
+        <v>7.3357716046404037E-2</v>
       </c>
       <c r="I33">
         <f>STDEV(C$21:C$22)/SQRT(COUNT(C$21:C$22))</f>
-        <v>1.3558492834783385E-2</v>
+        <v>1.3172879840323004E-2</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="2"/>
@@ -4398,7 +4509,7 @@
       </c>
       <c r="T33" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Lower</v>
       </c>
       <c r="U33" t="str">
         <f t="shared" si="0"/>
@@ -4448,7 +4559,7 @@
       </c>
       <c r="T34" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U34" t="str">
         <f t="shared" si="0"/>
@@ -4516,7 +4627,7 @@
       </c>
       <c r="T35" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U35" t="str">
         <f t="shared" si="0"/>
@@ -4545,19 +4656,19 @@
       </c>
       <c r="E36">
         <f>AVERAGE(D$1:D$3)</f>
-        <v>5.9478069732144784E-2</v>
+        <v>5.9621023719336724E-2</v>
       </c>
       <c r="F36">
         <f>AVERAGE(D$4:D$6)</f>
-        <v>5.8638143866693325E-2</v>
+        <v>5.8426894246005306E-2</v>
       </c>
       <c r="G36">
         <f>AVERAGE(D$7:D$12,D$17:D$19)</f>
-        <v>5.4113227781183867E-2</v>
+        <v>5.408192058558043E-2</v>
       </c>
       <c r="H36">
         <f>AVERAGE(D$13:D$16)</f>
-        <v>6.7431541842067871E-2</v>
+        <v>6.7749360389357263E-2</v>
       </c>
       <c r="I36">
         <f>D$20</f>
@@ -4565,7 +4676,7 @@
       </c>
       <c r="J36">
         <f>AVERAGE(D$21:D$22)</f>
-        <v>4.4012991540984973E-2</v>
+        <v>4.4012991541004708E-2</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="2"/>
@@ -4593,7 +4704,7 @@
       </c>
       <c r="T36" t="str">
         <f t="shared" si="0"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
       <c r="U36" t="str">
         <f t="shared" si="0"/>
@@ -4619,23 +4730,23 @@
     <row r="37" spans="4:31" x14ac:dyDescent="0.25">
       <c r="E37">
         <f>STDEV(D$1:D$3)/SQRT(COUNT(D$1:D$3))</f>
-        <v>2.0650131275029578E-2</v>
+        <v>2.0792372896380848E-2</v>
       </c>
       <c r="F37">
         <f>STDEV(D$4:D$6)/SQRT(COUNT(D$4:D$6))</f>
-        <v>1.6872030165327383E-2</v>
+        <v>1.7123224610862724E-2</v>
       </c>
       <c r="G37">
         <f>STDEV(D$7:D$12,D$17:D$19)/SQRT(COUNT(D$7:D$12,D$17:D$19))</f>
-        <v>5.1472832085554948E-3</v>
+        <v>5.1216710439505198E-3</v>
       </c>
       <c r="H37">
         <f>STDEV(D$13:D$16)/SQRT(COUNT(D$13:D$16))</f>
-        <v>1.5821047065794618E-2</v>
+        <v>1.5627247705565079E-2</v>
       </c>
       <c r="J37">
         <f>STDEV(D$21:D$22)/SQRT(COUNT(D$21:D$22))</f>
-        <v>6.4496365751035001E-4</v>
+        <v>6.4496365750799079E-4</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="2"/>
@@ -4717,7 +4828,7 @@
       </c>
       <c r="U38" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="0"/>
@@ -4781,7 +4892,7 @@
       </c>
       <c r="T39" t="str">
         <f t="shared" si="2"/>
-        <v>Lower</v>
+        <v>Upper</v>
       </c>
       <c r="U39" t="str">
         <f t="shared" si="2"/>
@@ -4810,19 +4921,19 @@
       </c>
       <c r="F40">
         <f>AVERAGE(E$1:E$3)</f>
-        <v>1.8216400216183155E-2</v>
+        <v>2.2210033221700154E-14</v>
       </c>
       <c r="G40">
         <f>AVERAGE(E$4:E$6)</f>
-        <v>2.8535466002487506E-6</v>
+        <v>2.8172663076369224E-7</v>
       </c>
       <c r="H40">
         <f>AVERAGE(E$7:E$12,E$17:E$19)</f>
-        <v>2.394278890071078E-2</v>
+        <v>4.0146854743199973E-4</v>
       </c>
       <c r="I40">
         <f>AVERAGE(E$13:E$16)</f>
-        <v>2.2295863458111093E-4</v>
+        <v>4.4129444733917032E-6</v>
       </c>
       <c r="J40">
         <f>E$20</f>
@@ -4830,7 +4941,7 @@
       </c>
       <c r="K40">
         <f>AVERAGE(E$21:E$22)</f>
-        <v>3.0962468201823E-14</v>
+        <v>2.2207396253646659E-14</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="2"/>
@@ -4858,7 +4969,7 @@
       </c>
       <c r="T40" t="str">
         <f t="shared" si="2"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U40" t="str">
         <f t="shared" si="2"/>
@@ -4884,23 +4995,23 @@
     <row r="41" spans="4:31" x14ac:dyDescent="0.25">
       <c r="F41">
         <f>STDEV(E$1:E$3)/SQRT(COUNT(E$1:E$3))</f>
-        <v>1.8216400216151726E-2</v>
+        <v>4.8250618270174104E-18</v>
       </c>
       <c r="G41">
         <f>STDEV(E$4:E$6)/SQRT(COUNT(E$4:E$6))</f>
-        <v>2.8535465570765901E-6</v>
+        <v>2.8172660276019622E-7</v>
       </c>
       <c r="H41">
         <f>STDEV(E$7:E$12,E$17:E$19)/SQRT(COUNT(E$7:E$12,E$17:E$19))</f>
-        <v>1.3687503622056138E-2</v>
+        <v>2.8632212313389749E-4</v>
       </c>
       <c r="I41">
         <f>STDEV(E$13:E$16)/SQRT(COUNT(E$13:E$16))</f>
-        <v>2.2295863455890644E-4</v>
+        <v>4.4127585456074152E-6</v>
       </c>
       <c r="K41">
         <f>STDEV(E$21:E$22)/SQRT(COUNT(E$21:E$22))</f>
-        <v>8.6172699064144549E-15</v>
+        <v>2.2044986974114701E-18</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="2"/>
@@ -4912,27 +5023,27 @@
       </c>
       <c r="P41" t="str">
         <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="Q41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="R41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="S41" t="str">
+        <f t="shared" si="2"/>
+        <v>Ok</v>
+      </c>
+      <c r="T41" t="str">
+        <f t="shared" si="2"/>
         <v>Lower</v>
       </c>
-      <c r="Q41" t="str">
-        <f t="shared" si="2"/>
-        <v>Ok</v>
-      </c>
-      <c r="R41" t="str">
-        <f t="shared" si="2"/>
-        <v>Ok</v>
-      </c>
-      <c r="S41" t="str">
-        <f t="shared" si="2"/>
-        <v>Ok</v>
-      </c>
-      <c r="T41" t="str">
+      <c r="U41" t="str">
         <f t="shared" si="2"/>
         <v>Lower</v>
-      </c>
-      <c r="U41" t="str">
-        <f t="shared" si="2"/>
-        <v>Ok</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="2"/>
@@ -5046,7 +5157,7 @@
       </c>
       <c r="T43" t="str">
         <f t="shared" si="2"/>
-        <v>Upper</v>
+        <v>Lower</v>
       </c>
       <c r="U43" t="str">
         <f t="shared" si="2"/>
@@ -5075,27 +5186,27 @@
       </c>
       <c r="G44">
         <f>AVERAGE(F$1:F$3)</f>
-        <v>0.34970880651974651</v>
+        <v>0.14700895503484715</v>
       </c>
       <c r="H44">
         <f>AVERAGE(F$4:F$6)</f>
-        <v>0.65427814759042635</v>
+        <v>0.51874426073426694</v>
       </c>
       <c r="I44">
         <f>AVERAGE(F$7:F$12,F$17:F$19)</f>
-        <v>0.29264641929465679</v>
+        <v>0.67733097633142481</v>
       </c>
       <c r="J44">
         <f>AVERAGE(F$13:F$16)</f>
-        <v>0.12137635598704148</v>
+        <v>0.55341627633490109</v>
       </c>
       <c r="K44">
         <f>F$20</f>
-        <v>0.13494302069264516</v>
+        <v>0.13494299556910744</v>
       </c>
       <c r="L44">
         <f>AVERAGE(F$21:F$22)</f>
-        <v>0.24221572593574936</v>
+        <v>0.24225139350649832</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="2"/>
@@ -5123,7 +5234,7 @@
       </c>
       <c r="T44" t="str">
         <f t="shared" si="2"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U44" t="str">
         <f t="shared" si="2"/>
@@ -5149,23 +5260,23 @@
     <row r="45" spans="4:31" x14ac:dyDescent="0.25">
       <c r="G45">
         <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
-        <v>0.20417348892883633</v>
+        <v>3.7887236211488991E-2</v>
       </c>
       <c r="H45">
         <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
-        <v>0.14430652595370547</v>
+        <v>0.12579716058654763</v>
       </c>
       <c r="I45">
         <f>STDEV(F$7:F$12,F$17:F$19)/SQRT(COUNT(F$7:F$12,F$17:F$19))</f>
-        <v>9.7833579515523295E-2</v>
+        <v>0.34452837581693579</v>
       </c>
       <c r="J45">
         <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
-        <v>3.2790536732440492E-2</v>
+        <v>0.44401386483779698</v>
       </c>
       <c r="L45">
         <f>STDEV(F$21:F$22)/SQRT(COUNT(F$21:F$22))</f>
-        <v>2.5077728020981439E-2</v>
+        <v>2.5042119599933226E-2</v>
       </c>
       <c r="N45" t="s">
         <v>17</v>
@@ -5248,49 +5359,49 @@
       </c>
       <c r="H48">
         <f>AVERAGE(G$1:G$3)</f>
-        <v>2.73260671823909E-2</v>
+        <v>2.6612095404732927E-2</v>
       </c>
       <c r="I48">
         <f>AVERAGE(G$4:G$6)</f>
-        <v>2.8011185058795168E-2</v>
+        <v>2.7473079382476524E-2</v>
       </c>
       <c r="J48">
         <f>AVERAGE(G$7:G$12,G$17:G$19)</f>
-        <v>2.7412729097984943E-2</v>
+        <v>2.7283317623498213E-2</v>
       </c>
       <c r="K48">
         <f>AVERAGE(G$13:G$16)</f>
-        <v>2.7253356968366522E-2</v>
+        <v>2.7369710249433226E-2</v>
       </c>
       <c r="L48">
         <f>G$20</f>
-        <v>2.6749603680624949E-2</v>
+        <v>2.6595818555612983E-2</v>
       </c>
       <c r="M48">
         <f>AVERAGE(G$21:G$22)</f>
-        <v>2.7778097264555691E-2</v>
+        <v>2.654766832169313E-2</v>
       </c>
     </row>
     <row r="49" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H49">
         <f>STDEV(G$1:G$3)/SQRT(COUNT(G$1:G$3))</f>
-        <v>4.3285808175431712E-4</v>
+        <v>4.5088837848277105E-5</v>
       </c>
       <c r="I49">
         <f>STDEV(G$4:G$6)/SQRT(COUNT(G$4:G$6))</f>
-        <v>1.9390289566935655E-8</v>
+        <v>3.7252970632583378E-4</v>
       </c>
       <c r="J49">
         <f>STDEV(G$7:G$12,G$17:G$19)/SQRT(COUNT(G$7:G$12,G$17:G$19))</f>
-        <v>2.1992645045035698E-4</v>
+        <v>1.9591704856672309E-4</v>
       </c>
       <c r="K49">
         <f>STDEV(G$13:G$16)/SQRT(COUNT(G$13:G$16))</f>
-        <v>4.2057692456981722E-4</v>
+        <v>2.9674052868955972E-4</v>
       </c>
       <c r="M49">
         <f>STDEV(G$21:G$22)/SQRT(COUNT(G$21:G$22))</f>
-        <v>2.3310713180289648E-4</v>
+        <v>5.3908646953891581E-6</v>
       </c>
     </row>
     <row r="51" spans="8:17" x14ac:dyDescent="0.25">
@@ -5319,49 +5430,49 @@
       </c>
       <c r="I52">
         <f>AVERAGE(H$1:H$3)</f>
-        <v>0.33676364162104067</v>
+        <v>7.5917629324230532E-2</v>
       </c>
       <c r="J52">
         <f>AVERAGE(H$4:H$6)</f>
-        <v>0.52871370637837634</v>
+        <v>0.39118585551184881</v>
       </c>
       <c r="K52">
         <f>AVERAGE(H$7:H$12,H$17:H$19)</f>
-        <v>0.35202956097484767</v>
+        <v>1.4556807367818019</v>
       </c>
       <c r="L52">
         <f>AVERAGE(H$13:H$16)</f>
-        <v>0.39700132959747969</v>
+        <v>2.6891949704917932</v>
       </c>
       <c r="M52">
         <f>H$20</f>
-        <v>0.20570831653393457</v>
+        <v>0.20586204465426139</v>
       </c>
       <c r="N52">
         <f>AVERAGE(H$21:H$22)</f>
-        <v>0.32496288700538134</v>
+        <v>0.32625927521033604</v>
       </c>
     </row>
     <row r="53" spans="8:17" x14ac:dyDescent="0.25">
       <c r="I53">
         <f>STDEV(H$1:H$3)/SQRT(COUNT(H$1:H$3))</f>
-        <v>0.23163722971978087</v>
+        <v>2.1967251752266336E-2</v>
       </c>
       <c r="J53">
         <f>STDEV(H$4:H$6)/SQRT(COUNT(H$4:H$6))</f>
-        <v>0.17811549460051718</v>
+        <v>0.14380117024004904</v>
       </c>
       <c r="K53">
         <f>STDEV(H$7:H$12,H$17:H$19)/SQRT(COUNT(H$7:H$12,H$17:H$19))</f>
-        <v>0.10012302584846257</v>
+        <v>1.0473379060285419</v>
       </c>
       <c r="L53">
         <f>STDEV(H$13:H$16)/SQRT(COUNT(H$13:H$16))</f>
-        <v>0.17684975535891814</v>
+        <v>2.4385643271491557</v>
       </c>
       <c r="N53">
         <f>STDEV(H$21:H$22)/SQRT(COUNT(H$21:H$22))</f>
-        <v>4.686211321228409E-2</v>
+        <v>4.6557772084041354E-2</v>
       </c>
     </row>
     <row r="55" spans="8:17" x14ac:dyDescent="0.25">
@@ -5390,49 +5501,49 @@
       </c>
       <c r="J56">
         <f>AVERAGE(I$1:I$3)</f>
-        <v>2.1313035967041396E-2</v>
+        <v>4.7043281897724644E-2</v>
       </c>
       <c r="K56">
         <f>AVERAGE(I$4:I$6)</f>
-        <v>1.5658317457008599E-8</v>
+        <v>3.4991609077748002E-14</v>
       </c>
       <c r="L56">
         <f>AVERAGE(I$7:I$12,I$17:I$19)</f>
-        <v>2.1391054587768009E-6</v>
+        <v>7.4630219943887829E-4</v>
       </c>
       <c r="M56">
         <f>AVERAGE(I$13:I$16)</f>
-        <v>2.2223185683657231E-14</v>
+        <v>4.0530954529238379E-6</v>
       </c>
       <c r="N56">
         <f>I$20</f>
-        <v>2.2204512590459397E-14</v>
+        <v>2.2204503459977956E-14</v>
       </c>
       <c r="O56">
         <f>AVERAGE(I$21:I$22)</f>
-        <v>4.1924885515696976E-14</v>
+        <v>2.2204713856538582E-14</v>
       </c>
     </row>
     <row r="57" spans="8:17" x14ac:dyDescent="0.25">
       <c r="J57">
         <f>STDEV(I$1:I$3)/SQRT(COUNT(I$1:I$3))</f>
-        <v>2.1313007683674758E-2</v>
+        <v>4.7043281897702433E-2</v>
       </c>
       <c r="K57">
         <f>STDEV(I$4:I$6)/SQRT(COUNT(I$4:I$6))</f>
-        <v>1.5658286966554589E-8</v>
+        <v>6.3772773096146374E-15</v>
       </c>
       <c r="L57">
         <f>STDEV(I$7:I$12,I$17:I$19)/SQRT(COUNT(I$7:I$12,I$17:I$19))</f>
-        <v>2.1391054329560717E-6</v>
+        <v>7.4617681527279955E-4</v>
       </c>
       <c r="M57">
         <f>STDEV(I$13:I$16)/SQRT(COUNT(I$13:I$16))</f>
-        <v>1.8505736920024398E-17</v>
+        <v>4.0529326997889823E-6</v>
       </c>
       <c r="O57">
         <f>STDEV(I$21:I$22)/SQRT(COUNT(I$21:I$22))</f>
-        <v>2.3474531355094457E-15</v>
+        <v>2.2978287727198393E-19</v>
       </c>
     </row>
     <row r="59" spans="8:17" x14ac:dyDescent="0.25">
@@ -5674,49 +5785,49 @@
       </c>
       <c r="N72">
         <f>AVERAGE(M$1:M$3)</f>
-        <v>0.99662997443488333</v>
+        <v>0.99662997411815801</v>
       </c>
       <c r="O72">
         <f>AVERAGE(M$4:M$6)</f>
-        <v>0.9967850405466846</v>
+        <v>0.99678502774392774</v>
       </c>
       <c r="P72">
         <f>AVERAGE(M$7:M$12,M$17:M$19)</f>
-        <v>0.99459432650386681</v>
+        <v>0.9946243241560917</v>
       </c>
       <c r="Q72">
         <f>AVERAGE(M$13:M$16)</f>
-        <v>0.99613211434445725</v>
+        <v>0.99613211356786546</v>
       </c>
       <c r="R72">
         <f>M$20</f>
-        <v>0.99345692483621739</v>
+        <v>0.99345692483643755</v>
       </c>
       <c r="S72">
         <f>AVERAGE(M$21:M$22)</f>
-        <v>0.99082673550075717</v>
+        <v>0.99082673534324806</v>
       </c>
     </row>
     <row r="73" spans="12:21" x14ac:dyDescent="0.25">
       <c r="N73">
         <f>STDEV(M$1:M$3)/SQRT(COUNT(M$1:M$3))</f>
-        <v>4.933691554882847E-4</v>
+        <v>4.9336913887755639E-4</v>
       </c>
       <c r="O73">
         <f>STDEV(M$4:M$6)/SQRT(COUNT(M$4:M$6))</f>
-        <v>3.487027254717397E-4</v>
+        <v>3.486949347042988E-4</v>
       </c>
       <c r="P73">
         <f>STDEV(M$7:M$12,M$17:M$19)/SQRT(COUNT(M$7:M$12,M$17:M$19))</f>
-        <v>1.9763401377386942E-3</v>
+        <v>1.9810102119476331E-3</v>
       </c>
       <c r="Q73">
         <f>STDEV(M$13:M$16)/SQRT(COUNT(M$13:M$16))</f>
-        <v>1.6834057294362777E-3</v>
+        <v>1.6834148194512729E-3</v>
       </c>
       <c r="S73">
         <f>STDEV(M$21:M$22)/SQRT(COUNT(M$21:M$22))</f>
-        <v>3.5454263259844243E-3</v>
+        <v>3.5454264834695604E-3</v>
       </c>
     </row>
     <row r="75" spans="12:21" x14ac:dyDescent="0.25">
@@ -5745,49 +5856,49 @@
       </c>
       <c r="O76">
         <f>AVERAGE(N$1:N$3)</f>
-        <v>0.99448563887721486</v>
+        <v>0.99199938412162059</v>
       </c>
       <c r="P76">
         <f>AVERAGE(N$4:N$6)</f>
-        <v>0.97734671215134927</v>
+        <v>0.97541479470508063</v>
       </c>
       <c r="Q76">
         <f>AVERAGE(N$7:N$12,N$17:N$19)</f>
-        <v>0.97017670594544492</v>
+        <v>0.96965084484165076</v>
       </c>
       <c r="R76">
         <f>AVERAGE(N$13:N$16)</f>
-        <v>0.99023122230441996</v>
+        <v>0.99258746444793977</v>
       </c>
       <c r="S76">
         <f>N$20</f>
-        <v>0.98644924395872025</v>
+        <v>0.98644924290192071</v>
       </c>
       <c r="T76">
         <f>AVERAGE(N$21:N$22)</f>
-        <v>0.97245005477980517</v>
+        <v>0.97245198416071776</v>
       </c>
     </row>
     <row r="77" spans="12:21" x14ac:dyDescent="0.25">
       <c r="O77">
         <f>STDEV(N$1:N$3)/SQRT(COUNT(N$1:N$3))</f>
-        <v>1.7514647658219368E-3</v>
+        <v>3.3666505227571966E-3</v>
       </c>
       <c r="P77">
         <f>STDEV(N$4:N$6)/SQRT(COUNT(N$4:N$6))</f>
-        <v>8.9187282116430251E-3</v>
+        <v>1.0654580102394942E-2</v>
       </c>
       <c r="Q77">
         <f>STDEV(N$7:N$12,N$17:N$19)/SQRT(COUNT(N$7:N$12,N$17:N$19))</f>
-        <v>1.1036621543151463E-2</v>
+        <v>1.1875659785251722E-2</v>
       </c>
       <c r="R77">
         <f>STDEV(N$13:N$16)/SQRT(COUNT(N$13:N$16))</f>
-        <v>4.4038352314395221E-3</v>
+        <v>2.5055085561655724E-3</v>
       </c>
       <c r="T77">
         <f>STDEV(N$21:N$22)/SQRT(COUNT(N$21:N$22))</f>
-        <v>1.2021234066777409E-2</v>
+        <v>1.2023160573295222E-2</v>
       </c>
     </row>
     <row r="79" spans="12:21" x14ac:dyDescent="0.25">
@@ -5816,49 +5927,49 @@
       </c>
       <c r="P80">
         <f>AVERAGE(O$1:O$3)</f>
-        <v>0.9781553617306793</v>
+        <v>0.99642630127703191</v>
       </c>
       <c r="Q80">
         <f>AVERAGE(O$4:O$6)</f>
-        <v>0.98973561872133031</v>
+        <v>0.98562172652789837</v>
       </c>
       <c r="R80">
         <f>AVERAGE(O$7:O$12,O$17:O$19)</f>
-        <v>0.9858769698484533</v>
+        <v>0.97622736868249915</v>
       </c>
       <c r="S80">
         <f>AVERAGE(O$13:O$16)</f>
-        <v>0.97245256207522279</v>
+        <v>0.96792446357023321</v>
       </c>
       <c r="T80">
         <f>O$20</f>
-        <v>0.99602689555396506</v>
+        <v>0.99602689796079291</v>
       </c>
       <c r="U80">
         <f>AVERAGE(O$21:O$22)</f>
-        <v>0.99394564744955127</v>
+        <v>0.9939440085543001</v>
       </c>
     </row>
     <row r="81" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P81">
         <f>STDEV(O$1:O$3)/SQRT(COUNT(O$1:O$3))</f>
-        <v>1.4876928817410639E-2</v>
+        <v>7.903214212686805E-4</v>
       </c>
       <c r="Q81">
         <f>STDEV(O$4:O$6)/SQRT(COUNT(O$4:O$6))</f>
-        <v>4.8162956211966141E-3</v>
+        <v>9.0723300721945472E-3</v>
       </c>
       <c r="R81">
         <f>STDEV(O$7:O$12,O$17:O$19)/SQRT(COUNT(O$7:O$12,O$17:O$19))</f>
-        <v>5.1348258298138999E-3</v>
+        <v>1.2129818847755281E-2</v>
       </c>
       <c r="S81">
         <f>STDEV(O$13:O$16)/SQRT(COUNT(O$13:O$16))</f>
-        <v>1.0093839421714677E-2</v>
+        <v>9.1385974951318887E-3</v>
       </c>
       <c r="U81">
         <f>STDEV(O$21:O$22)/SQRT(COUNT(O$21:O$22))</f>
-        <v>1.5076347596117976E-3</v>
+        <v>1.5092714424497777E-3</v>
       </c>
     </row>
     <row r="83" spans="16:24" x14ac:dyDescent="0.25">
@@ -5887,49 +5998,49 @@
       </c>
       <c r="Q84">
         <f>AVERAGE(P$1:P$3)</f>
-        <v>8.2770293824527566E-2</v>
+        <v>8.2769960386286354E-2</v>
       </c>
       <c r="R84">
         <f>AVERAGE(P$4:P$6)</f>
-        <v>8.1747171416990311E-2</v>
+        <v>8.1747176174903999E-2</v>
       </c>
       <c r="S84">
         <f>AVERAGE(P$7:P$12,P$17:P$19)</f>
-        <v>0.10170067444147866</v>
+        <v>9.6618096060557532E-2</v>
       </c>
       <c r="T84">
         <f>AVERAGE(P$13:P$16)</f>
-        <v>8.0488341980152048E-2</v>
+        <v>8.0488259007867796E-2</v>
       </c>
       <c r="U84">
         <f>P$20</f>
-        <v>0.11612890078225724</v>
+        <v>0.11612890077785666</v>
       </c>
       <c r="V84">
         <f>AVERAGE(P$21:P$22)</f>
-        <v>0.13277519176134384</v>
+        <v>0.13277519443340902</v>
       </c>
     </row>
     <row r="85" spans="16:24" x14ac:dyDescent="0.25">
       <c r="Q85">
         <f>STDEV(P$1:P$3)/SQRT(COUNT(P$1:P$3))</f>
-        <v>6.1726601843257499E-3</v>
+        <v>6.1728202303740097E-3</v>
       </c>
       <c r="R85">
         <f>STDEV(P$4:P$6)/SQRT(COUNT(P$4:P$6))</f>
-        <v>4.7620696293343284E-3</v>
+        <v>4.7620664425895532E-3</v>
       </c>
       <c r="S85">
         <f>STDEV(P$7:P$12,P$17:P$19)/SQRT(COUNT(P$7:P$12,P$17:P$19))</f>
-        <v>1.6051518650224569E-2</v>
+        <v>1.5214270543208034E-2</v>
       </c>
       <c r="T85">
         <f>STDEV(P$13:P$16)/SQRT(COUNT(P$13:P$16))</f>
-        <v>2.0142318456974902E-2</v>
+        <v>2.014243603928605E-2</v>
       </c>
       <c r="V85">
         <f>STDEV(P$21:P$22)/SQRT(COUNT(P$21:P$22))</f>
-        <v>2.613087600665143E-2</v>
+        <v>2.6130878673853903E-2</v>
       </c>
     </row>
     <row r="87" spans="16:24" x14ac:dyDescent="0.25">
@@ -5958,49 +6069,49 @@
       </c>
       <c r="R88">
         <f>AVERAGE(Q$1:Q$3)</f>
-        <v>0.10365340206265559</v>
+        <v>0.12003209288401152</v>
       </c>
       <c r="S88">
         <f>AVERAGE(Q$4:Q$6)</f>
-        <v>0.20693036796603156</v>
+        <v>0.21343844914888963</v>
       </c>
       <c r="T88">
         <f>AVERAGE(Q$7:Q$12,Q$17:Q$19)</f>
-        <v>0.22507778652062205</v>
+        <v>0.21495956670453156</v>
       </c>
       <c r="U88">
         <f>AVERAGE(Q$13:Q$16)</f>
-        <v>0.13693586421858409</v>
+        <v>0.12579060832283959</v>
       </c>
       <c r="V88">
         <f>Q$20</f>
-        <v>0.16359251960162435</v>
+        <v>0.16359252591784523</v>
       </c>
       <c r="W88">
         <f>AVERAGE(Q$21:Q$22)</f>
-        <v>0.22934211796905202</v>
+        <v>0.22933142053717082</v>
       </c>
     </row>
     <row r="89" spans="16:24" x14ac:dyDescent="0.25">
       <c r="R89">
         <f>STDEV(Q$1:Q$3)/SQRT(COUNT(Q$1:Q$3))</f>
-        <v>1.9940906766864917E-2</v>
+        <v>2.9915209911607666E-2</v>
       </c>
       <c r="S89">
         <f>STDEV(Q$4:Q$6)/SQRT(COUNT(Q$4:Q$6))</f>
-        <v>3.7920776097689957E-2</v>
+        <v>4.3580024502883882E-2</v>
       </c>
       <c r="T89">
         <f>STDEV(Q$7:Q$12,Q$17:Q$19)/SQRT(COUNT(Q$7:Q$12,Q$17:Q$19))</f>
-        <v>5.2115587357412181E-2</v>
+        <v>4.9563045357193969E-2</v>
       </c>
       <c r="U89">
         <f>STDEV(Q$13:Q$16)/SQRT(COUNT(Q$13:Q$16))</f>
-        <v>3.4359512504840789E-2</v>
+        <v>2.5182325466262E-2</v>
       </c>
       <c r="W89">
         <f>STDEV(Q$21:Q$22)/SQRT(COUNT(Q$21:Q$22))</f>
-        <v>5.2434425372918522E-2</v>
+        <v>5.2445112898152908E-2</v>
       </c>
     </row>
     <row r="91" spans="16:24" x14ac:dyDescent="0.25">
@@ -6029,49 +6140,49 @@
       </c>
       <c r="S92">
         <f>AVERAGE(R$1:R$3)</f>
-        <v>0.19873190886854161</v>
+        <v>9.8876526846989221E-2</v>
       </c>
       <c r="T92">
         <f>AVERAGE(R$4:R$6)</f>
-        <v>0.14330733974915608</v>
+        <v>0.15989821775497828</v>
       </c>
       <c r="U92">
         <f>AVERAGE(R$7:R$12,R$17:R$19)</f>
-        <v>0.20903655881569599</v>
+        <v>0.1863577766352795</v>
       </c>
       <c r="V92">
         <f>AVERAGE(R$13:R$16)</f>
-        <v>0.24230094927599533</v>
+        <v>0.24531984414001679</v>
       </c>
       <c r="W92">
         <f>R$20</f>
-        <v>0.10046396988442108</v>
+        <v>0.10046394420079181</v>
       </c>
       <c r="X92">
         <f>AVERAGE(R$21:R$22)</f>
-        <v>0.11111149372809123</v>
+        <v>0.1111235379234371</v>
       </c>
     </row>
     <row r="93" spans="16:24" x14ac:dyDescent="0.25">
       <c r="S93">
         <f>STDEV(R$1:R$3)/SQRT(COUNT(R$1:R$3))</f>
-        <v>6.0196540838655041E-2</v>
+        <v>1.6225282641834871E-2</v>
       </c>
       <c r="T93">
         <f>STDEV(R$4:R$6)/SQRT(COUNT(R$4:R$6))</f>
-        <v>2.8992593597623836E-2</v>
+        <v>4.7075848425480959E-2</v>
       </c>
       <c r="U93">
         <f>STDEV(R$7:R$12,R$17:R$19)/SQRT(COUNT(R$7:R$12,R$17:R$19))</f>
-        <v>6.9352999322950609E-2</v>
+        <v>4.367031583618889E-2</v>
       </c>
       <c r="V93">
         <f>STDEV(R$13:R$16)/SQRT(COUNT(R$13:R$16))</f>
-        <v>3.7510887070126314E-2</v>
+        <v>4.2744543922925191E-2</v>
       </c>
       <c r="X93">
         <f>STDEV(R$21:R$22)/SQRT(COUNT(R$21:R$22))</f>
-        <v>1.5346714210696614E-2</v>
+        <v>1.5358734968358647E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverting repo to previous initial condition that worked slightly better
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation_moredata.xlsx
+++ b/Lacex_summary_FinalConfirmation_moredata.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FD8119-4A71-4C1C-B1D1-DA0EB215ACB0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BFFAC9-89A5-4BD0-825D-75787A35DFA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B075899B-8E8B-4489-B096-777C4BA97E2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -262,16 +265,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.5384056711341255E-4</c:v>
+                    <c:v>1.3632467423976377E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7821996996424904E-3</c:v>
+                    <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0379987715457955E-2</c:v>
+                    <c:v>1.0181144930654133E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.6416840859272169E-3</c:v>
+                    <c:v>9.1957167148318739E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -283,16 +286,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.5384056711341255E-4</c:v>
+                    <c:v>1.3632467423976377E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7821996996424904E-3</c:v>
+                    <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0379987715457955E-2</c:v>
+                    <c:v>1.0181144930654133E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.6416840859272169E-3</c:v>
+                    <c:v>9.1957167148318739E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -338,16 +341,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.6349270531761137E-3</c:v>
+                  <c:v>3.6597166972760207E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5890787210518401E-2</c:v>
+                  <c:v>1.2969578710698102E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.860466689820248E-2</c:v>
+                  <c:v>3.9850373025406699E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6284104580458269E-2</c:v>
+                  <c:v>1.7436370403402304E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,16 +619,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.2095893884320664E-2</c:v>
+                    <c:v>3.7887236211488991E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.13947133847608845</c:v>
+                    <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.33459226592417918</c:v>
+                    <c:v>0.34452837581693579</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.42920219363787993</c:v>
+                    <c:v>0.44401386483779698</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -637,16 +640,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.2095893884320664E-2</c:v>
+                    <c:v>3.7887236211488991E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.13947133847608845</c:v>
+                    <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.33459226592417918</c:v>
+                    <c:v>0.34452837581693579</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.42920219363787993</c:v>
+                    <c:v>0.44401386483779698</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -692,16 +695,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.13093022863689935</c:v>
+                  <c:v>0.14700895503484715</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67407664196283246</c:v>
+                  <c:v>0.51874426073426694</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60897305684494307</c:v>
+                  <c:v>0.67733097633142481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50454767474270834</c:v>
+                  <c:v>0.55341627633490109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2049,6 +2052,114 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="27">
+          <cell r="C27" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="E27" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>kMCT4</v>
+          </cell>
+          <cell r="C28">
+            <v>9.2535545750464687E-2</v>
+          </cell>
+          <cell r="D28">
+            <v>0.3541415185008206</v>
+          </cell>
+          <cell r="E28">
+            <v>0.75444268232926348</v>
+          </cell>
+          <cell r="F28">
+            <v>0.16916415025152015</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>1.2057455739979463E-2</v>
+          </cell>
+          <cell r="D29">
+            <v>5.7309495294150879E-2</v>
+          </cell>
+          <cell r="E29">
+            <v>0.39928208436858398</v>
+          </cell>
+          <cell r="F29">
+            <v>0.13741088889033834</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="D31" t="str">
+            <v>HK-2</v>
+          </cell>
+          <cell r="E31" t="str">
+            <v>UMRC6</v>
+          </cell>
+          <cell r="F31" t="str">
+            <v>UOK262</v>
+          </cell>
+          <cell r="G31" t="str">
+            <v>UOK + DIDS</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32" t="str">
+            <v>R1L</v>
+          </cell>
+          <cell r="D32">
+            <v>7.384890314233869E-2</v>
+          </cell>
+          <cell r="E32">
+            <v>5.0263555960985945E-2</v>
+          </cell>
+          <cell r="F32">
+            <v>6.3109847044927683E-2</v>
+          </cell>
+          <cell r="G32">
+            <v>8.0357873156810505E-2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="D33">
+            <v>2.3803754511435734E-2</v>
+          </cell>
+          <cell r="E33">
+            <v>2.3947765296666392E-2</v>
+          </cell>
+          <cell r="F33">
+            <v>1.0466686942143609E-2</v>
+          </cell>
+          <cell r="G33">
+            <v>1.4625933793160245E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2348,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5426EC7D-B74E-4953-AA3A-EC81D60A2FE4}">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,28 +2470,28 @@
         <v>2.0781114759556379E-2</v>
       </c>
       <c r="B1">
-        <v>3.4051314896244222E-3</v>
+        <v>3.4795161265732725E-3</v>
       </c>
       <c r="C1">
-        <v>0.12122997477940826</v>
+        <v>0.12115537047460399</v>
       </c>
       <c r="D1">
-        <v>3.5353019423418279E-2</v>
+        <v>3.5353019394421974E-2</v>
       </c>
       <c r="E1">
-        <v>3.5032077433530219E-14</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F1">
-        <v>0.17376065956773284</v>
+        <v>0.22199757443326015</v>
       </c>
       <c r="G1">
-        <v>2.732384362429989E-2</v>
+        <v>2.670202489455735E-2</v>
       </c>
       <c r="H1">
-        <v>0.11208695025091296</v>
+        <v>0.1193170263614496</v>
       </c>
       <c r="I1">
-        <v>7.517205021117454E-2</v>
+        <v>0.1411298456931295</v>
       </c>
       <c r="J1">
         <v>2.356211808499348</v>
@@ -2392,22 +2503,22 @@
         <v>254686091.39268142</v>
       </c>
       <c r="M1">
-        <v>0.99715195422500225</v>
+        <v>0.99715195462511363</v>
       </c>
       <c r="N1">
-        <v>0.99782537303159224</v>
+        <v>0.99785346972528499</v>
       </c>
       <c r="O1">
-        <v>0.99458423185560285</v>
+        <v>0.99488532535510454</v>
       </c>
       <c r="P1">
-        <v>7.6353436475485426E-2</v>
+        <v>7.6353436469702843E-2</v>
       </c>
       <c r="Q1">
-        <v>6.5596543368419288E-2</v>
+        <v>6.5139118584084318E-2</v>
       </c>
       <c r="R1">
-        <v>0.13277123063117841</v>
+        <v>0.13102591930261462</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -2415,25 +2526,25 @@
         <v>1.9731495213395425E-2</v>
       </c>
       <c r="B2">
-        <v>3.9270147316681648E-3</v>
+        <v>3.9270147990883662E-3</v>
       </c>
       <c r="C2">
-        <v>0.21794698589561248</v>
+        <v>0.21794698582814859</v>
       </c>
       <c r="D2">
         <v>0.10099996196568557</v>
       </c>
       <c r="E2">
-        <v>2.2207006181785035E-14</v>
+        <v>2.2205996670362198E-14</v>
       </c>
       <c r="F2">
-        <v>0.1189411056466711</v>
+        <v>0.11894110934795486</v>
       </c>
       <c r="G2">
-        <v>2.6545144648840752E-2</v>
+        <v>2.6561340578606808E-2</v>
       </c>
       <c r="H2">
-        <v>4.8313843189307086E-2</v>
+        <v>4.8297651990673832E-2</v>
       </c>
       <c r="I2">
         <v>2.2204460492503131E-14</v>
@@ -2451,19 +2562,19 @@
         <v>0.99709416769265702</v>
       </c>
       <c r="N2">
-        <v>0.9861913224738349</v>
+        <v>0.98619132265690701</v>
       </c>
       <c r="O2">
-        <v>0.99689204572409751</v>
+        <v>0.99689204548862798</v>
       </c>
       <c r="P2">
         <v>7.6844094339646424E-2</v>
       </c>
       <c r="Q2">
-        <v>0.16808999503267194</v>
+        <v>0.16808999389977516</v>
       </c>
       <c r="R2">
-        <v>7.8981904721114105E-2</v>
+        <v>7.8981907325062134E-2</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -2471,28 +2582,28 @@
         <v>2.0365465865092722E-2</v>
       </c>
       <c r="B3">
-        <v>3.5726349382357537E-3</v>
+        <v>3.5726191661664243E-3</v>
       </c>
       <c r="C3">
-        <v>0.2316036910738298</v>
+        <v>0.23160370685789064</v>
       </c>
       <c r="D3">
         <v>4.2510089797902627E-2</v>
       </c>
       <c r="E3">
-        <v>3.6974843312995153E-14</v>
+        <v>2.2219642502235133E-14</v>
       </c>
       <c r="F3">
-        <v>0.10008892069629409</v>
+        <v>0.10008818132332642</v>
       </c>
       <c r="G3">
-        <v>2.6957084497640692E-2</v>
+        <v>2.6572920741034615E-2</v>
       </c>
       <c r="H3">
-        <v>5.975525792047981E-2</v>
+        <v>6.0138209620568157E-2</v>
       </c>
       <c r="I3">
-        <v>2.2239921080696078E-14</v>
+        <v>2.2230487406924265E-14</v>
       </c>
       <c r="J3">
         <v>2.8545008818278075</v>
@@ -2504,22 +2615,22 @@
         <v>491427690.54543257</v>
       </c>
       <c r="M3">
-        <v>0.99564380003670983</v>
+        <v>0.99564380003670339</v>
       </c>
       <c r="N3">
-        <v>0.9919534257548297</v>
+        <v>0.99195335998266976</v>
       </c>
       <c r="O3">
-        <v>0.99750141224334987</v>
+        <v>0.9975015329873631</v>
       </c>
       <c r="P3">
-        <v>9.5112350349509434E-2</v>
+        <v>9.5112350349509781E-2</v>
       </c>
       <c r="Q3">
-        <v>0.126866633952642</v>
+        <v>0.12686716616817512</v>
       </c>
       <c r="R3">
-        <v>8.6623300587525903E-2</v>
+        <v>8.6621753913290897E-2</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -2527,28 +2638,28 @@
         <v>1.9994972552697242E-2</v>
       </c>
       <c r="B4">
-        <v>1.6051065267185829E-2</v>
+        <v>8.2261049334318315E-3</v>
       </c>
       <c r="C4">
-        <v>1.0000022204460493E-8</v>
+        <v>7.8238786162331871E-3</v>
       </c>
       <c r="D4">
-        <v>4.0405897725987308E-2</v>
+        <v>4.1448382824856529E-2</v>
       </c>
       <c r="E4">
-        <v>2.2205466852843756E-14</v>
+        <v>8.4517983628408446E-7</v>
       </c>
       <c r="F4">
-        <v>0.81841703661902854</v>
+        <v>0.38417933083549277</v>
       </c>
       <c r="G4">
-        <v>2.8010085625219078E-2</v>
+        <v>2.801117129673817E-2</v>
       </c>
       <c r="H4">
-        <v>0.73823005382669471</v>
+        <v>0.30888130275024206</v>
       </c>
       <c r="I4">
-        <v>2.2205412607912549E-14</v>
+        <v>4.1254209297634721E-14</v>
       </c>
       <c r="J4">
         <v>5.740537779224173</v>
@@ -2560,22 +2671,22 @@
         <v>142097848.58194768</v>
       </c>
       <c r="M4">
-        <v>0.99706206615205151</v>
+        <v>0.99706208406329411</v>
       </c>
       <c r="N4">
-        <v>0.96119274191953841</v>
+        <v>0.95451182918462252</v>
       </c>
       <c r="O4">
-        <v>0.98291648660889086</v>
+        <v>0.96755342148890255</v>
       </c>
       <c r="P4">
-        <v>7.8465809877410864E-2</v>
+        <v>7.8465803659368477E-2</v>
       </c>
       <c r="Q4">
-        <v>0.2761452440478131</v>
+        <v>0.29835113413949227</v>
       </c>
       <c r="R4">
-        <v>0.18486028972555796</v>
+        <v>0.25391303933089066</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
@@ -2610,28 +2721,28 @@
         <v>2.023647882476649E-2</v>
       </c>
       <c r="B5">
-        <v>1.8894386257415872E-2</v>
+        <v>1.7952384844695909E-2</v>
       </c>
       <c r="C5">
-        <v>0.32419781914033352</v>
+        <v>0.32513897643519724</v>
       </c>
       <c r="D5">
-        <v>9.2672934501803195E-2</v>
+        <v>9.267293693911316E-2</v>
       </c>
       <c r="E5">
-        <v>2.3460876580385628E-14</v>
+        <v>3.37910782375764E-14</v>
       </c>
       <c r="F5">
-        <v>0.8086215883030321</v>
+        <v>0.77012992110925338</v>
       </c>
       <c r="G5">
-        <v>2.6801903709279411E-2</v>
+        <v>2.6757739839081779E-2</v>
       </c>
       <c r="H5">
-        <v>0.71180128710139112</v>
+        <v>0.67099227523245808</v>
       </c>
       <c r="I5">
-        <v>3.0092834442942541E-14</v>
+        <v>4.1482880168662724E-14</v>
       </c>
       <c r="J5">
         <v>3.2019451544874276</v>
@@ -2643,22 +2754,22 @@
         <v>629017289.17440271</v>
       </c>
       <c r="M5">
-        <v>0.99609224823705544</v>
+        <v>0.99609224845038047</v>
       </c>
       <c r="N5">
-        <v>0.98240156166577464</v>
+        <v>0.98228022729653697</v>
       </c>
       <c r="O5">
-        <v>0.99308936725435504</v>
+        <v>0.99321581530579128</v>
       </c>
       <c r="P5">
-        <v>9.1131006274282944E-2</v>
+        <v>9.1131006252957447E-2</v>
       </c>
       <c r="Q5">
-        <v>0.18738598496643616</v>
+        <v>0.18801244877525125</v>
       </c>
       <c r="R5">
-        <v>0.1183008863292794</v>
+        <v>0.11728586191248075</v>
       </c>
       <c r="T5" s="1">
         <f>1/51</f>
@@ -2699,28 +2810,28 @@
         <v>2.0231218059161282E-2</v>
       </c>
       <c r="B6">
-        <v>1.2726910106953503E-2</v>
+        <v>1.2730246353966567E-2</v>
       </c>
       <c r="C6">
-        <v>3.9262099635869452E-7</v>
+        <v>1.0000022208952447E-8</v>
       </c>
       <c r="D6">
-        <v>4.2735381218773294E-2</v>
+        <v>4.1159362974046244E-2</v>
       </c>
       <c r="E6">
-        <v>4.3163856395249785E-14</v>
+        <v>2.2215914010445092E-14</v>
       </c>
       <c r="F6">
-        <v>0.39519130096643657</v>
+        <v>0.40192353025805466</v>
       </c>
       <c r="G6">
-        <v>2.7914609547690962E-2</v>
+        <v>2.7650327011609629E-2</v>
       </c>
       <c r="H6">
-        <v>0.19223745318517815</v>
+        <v>0.19368398855284627</v>
       </c>
       <c r="I6">
-        <v>3.7106049119008891E-14</v>
+        <v>2.2237737766946569E-14</v>
       </c>
       <c r="J6">
         <v>4.8009905427717481</v>
@@ -2732,22 +2843,22 @@
         <v>149956135.49829885</v>
       </c>
       <c r="M6">
-        <v>0.99720079053297539</v>
+        <v>0.99720075071810876</v>
       </c>
       <c r="N6">
-        <v>0.98937681215168038</v>
+        <v>0.98945232763408242</v>
       </c>
       <c r="O6">
-        <v>0.99606513120227036</v>
+        <v>0.99609594278900127</v>
       </c>
       <c r="P6">
-        <v>7.564470311663718E-2</v>
+        <v>7.5644718612386044E-2</v>
       </c>
       <c r="Q6">
-        <v>0.15424621825810061</v>
+        <v>0.1539517645319253</v>
       </c>
       <c r="R6">
-        <v>0.10882340635197844</v>
+        <v>0.10849575202156349</v>
       </c>
       <c r="T6" s="1">
         <f>1/47</f>
@@ -2785,28 +2896,28 @@
         <v>2.0352218032308276E-2</v>
       </c>
       <c r="B7">
-        <v>1.1336382617505315E-2</v>
+        <v>1.1336378651585302E-2</v>
       </c>
       <c r="C7">
-        <v>1.6568057864995902E-2</v>
+        <v>1.6568061839038396E-2</v>
       </c>
       <c r="D7">
         <v>4.5873244781070611E-2</v>
       </c>
       <c r="E7">
-        <v>2.2204774261040089E-14</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F7">
-        <v>7.6265694669369222E-2</v>
+        <v>7.6265635306323493E-2</v>
       </c>
       <c r="G7">
-        <v>2.7240389063140396E-2</v>
+        <v>2.7659978894551168E-2</v>
       </c>
       <c r="H7">
-        <v>9.8952990442264521E-2</v>
+        <v>9.8533251240757375E-2</v>
       </c>
       <c r="I7">
-        <v>2.2204810715020714E-14</v>
+        <v>2.2204979238374094E-14</v>
       </c>
       <c r="J7">
         <v>1.952898836424503</v>
@@ -2818,22 +2929,22 @@
         <v>132744891.08503906</v>
       </c>
       <c r="M7">
-        <v>0.99900216768482641</v>
+        <v>0.99900216768483463</v>
       </c>
       <c r="N7">
-        <v>0.99812720889057349</v>
+        <v>0.99812720704547231</v>
       </c>
       <c r="O7">
-        <v>0.99659961459637558</v>
+        <v>0.9965996225501188</v>
       </c>
       <c r="P7">
-        <v>4.4448064950340267E-2</v>
+        <v>4.4448064950350752E-2</v>
       </c>
       <c r="Q7">
-        <v>6.3844900926967249E-2</v>
+        <v>6.3844926603594698E-2</v>
       </c>
       <c r="R7">
-        <v>9.1231954181312011E-2</v>
+        <v>9.123185443573037E-2</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -2841,28 +2952,28 @@
         <v>2.0420572162940933E-2</v>
       </c>
       <c r="B8">
-        <v>2.2011934505815449E-2</v>
+        <v>2.8455085625926618E-2</v>
       </c>
       <c r="C8">
-        <v>0.20827938728691545</v>
+        <v>0.19463910134944526</v>
       </c>
       <c r="D8">
-        <v>6.5007089336341681E-2</v>
+        <v>6.5007089083382458E-2</v>
       </c>
       <c r="E8">
-        <v>8.9208063376918056E-2</v>
+        <v>2.4898037270932147E-3</v>
       </c>
       <c r="F8">
-        <v>7.6601709490296599E-2</v>
+        <v>0.23965150048870829</v>
       </c>
       <c r="G8">
-        <v>2.6703305794011801E-2</v>
+        <v>2.7079786776221599E-2</v>
       </c>
       <c r="H8">
-        <v>0.12457751891307292</v>
+        <v>0.57170256654956031</v>
       </c>
       <c r="I8">
-        <v>2.220457512437045E-14</v>
+        <v>9.941866654942422E-7</v>
       </c>
       <c r="J8">
         <v>2.4430206679346318</v>
@@ -2874,22 +2985,22 @@
         <v>457955160.74923623</v>
       </c>
       <c r="M8">
-        <v>0.99838221935482696</v>
+        <v>0.99837928576034285</v>
       </c>
       <c r="N8">
-        <v>0.99734885462159295</v>
+        <v>0.99840550035107978</v>
       </c>
       <c r="O8">
-        <v>0.99710079822105546</v>
+        <v>0.97812854760325485</v>
       </c>
       <c r="P8">
-        <v>5.7537209676407366E-2</v>
+        <v>5.751194069035951E-2</v>
       </c>
       <c r="Q8">
-        <v>7.2381879410750777E-2</v>
+        <v>5.6148136508280842E-2</v>
       </c>
       <c r="R8">
-        <v>7.7702571183904307E-2</v>
+        <v>0.21109361441809982</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -2897,28 +3008,28 @@
         <v>1.9856607624304978E-2</v>
       </c>
       <c r="B9">
-        <v>6.7683336719467871E-2</v>
+        <v>6.9060525830266173E-2</v>
       </c>
       <c r="C9">
-        <v>0.25938823711915393</v>
+        <v>0.25801108459089117</v>
       </c>
       <c r="D9">
-        <v>7.4391016723786826E-2</v>
+        <v>7.4230058620422631E-2</v>
       </c>
       <c r="E9">
-        <v>4.4408912382628466E-14</v>
+        <v>2.9250814687839763E-14</v>
       </c>
       <c r="F9">
-        <v>3.1670181536522732</v>
+        <v>3.2253352307515293</v>
       </c>
       <c r="G9">
-        <v>2.7978664586538051E-2</v>
+        <v>2.8011204478663298E-2</v>
       </c>
       <c r="H9">
-        <v>9.5779288954257709</v>
+        <v>9.750654659613712</v>
       </c>
       <c r="I9">
-        <v>1.008157718193232E-8</v>
+        <v>8.9507003447047568E-9</v>
       </c>
       <c r="J9">
         <v>4.3363113643580764</v>
@@ -2930,22 +3041,22 @@
         <v>1205583684.8478703</v>
       </c>
       <c r="M9">
-        <v>0.99455792353124206</v>
+        <v>0.99455792352757189</v>
       </c>
       <c r="N9">
-        <v>0.95888031079665836</v>
+        <v>0.95888050748856335</v>
       </c>
       <c r="O9">
-        <v>0.98176146977008782</v>
+        <v>0.98176164041495118</v>
       </c>
       <c r="P9">
-        <v>0.1039864926028133</v>
+        <v>0.10398649260370561</v>
       </c>
       <c r="Q9">
-        <v>0.29760869582762572</v>
+        <v>0.29760772423271709</v>
       </c>
       <c r="R9">
-        <v>0.19874313896567022</v>
+        <v>0.19874222923660653</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -2953,28 +3064,28 @@
         <v>1.9607843138025917E-2</v>
       </c>
       <c r="B10">
-        <v>8.5119473619457552E-3</v>
+        <v>1.2323139929023586E-2</v>
       </c>
       <c r="C10">
-        <v>1.9399955151039799E-2</v>
+        <v>1.5598276110641449E-2</v>
       </c>
       <c r="D10">
-        <v>6.2308359763502116E-2</v>
+        <v>6.230835978644024E-2</v>
       </c>
       <c r="E10">
-        <v>2.5726034712820844E-14</v>
+        <v>1.0730907695642397E-3</v>
       </c>
       <c r="F10">
-        <v>0.85422746925330084</v>
+        <v>1.2599420336012488</v>
       </c>
       <c r="G10">
-        <v>2.6974649245169208E-2</v>
+        <v>2.7334357934778661E-2</v>
       </c>
       <c r="H10">
-        <v>0.96199074142762309</v>
+        <v>1.4553538898315348</v>
       </c>
       <c r="I10">
-        <v>4.2443305708748955E-14</v>
+        <v>4.0807233768722193E-14</v>
       </c>
       <c r="J10">
         <v>3.6193816110419976</v>
@@ -2986,22 +3097,22 @@
         <v>83209857.156356871</v>
       </c>
       <c r="M10">
-        <v>0.99668268122338344</v>
+        <v>0.99668267063118265</v>
       </c>
       <c r="N10">
-        <v>0.98894164108493654</v>
+        <v>0.98967172348163557</v>
       </c>
       <c r="O10">
-        <v>0.99227300006859998</v>
+        <v>0.99072332294345355</v>
       </c>
       <c r="P10">
-        <v>8.1022431710243079E-2</v>
+        <v>8.1022592759074114E-2</v>
       </c>
       <c r="Q10">
-        <v>0.15054796811491605</v>
+        <v>0.1457665294218416</v>
       </c>
       <c r="R10">
-        <v>0.12394731426021756</v>
+        <v>0.13578312841773169</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -3009,10 +3120,10 @@
         <v>1.9607868588388273E-2</v>
       </c>
       <c r="B11">
-        <v>1.6018888618765357E-2</v>
+        <v>1.601888853618769E-2</v>
       </c>
       <c r="C11">
-        <v>0.16415849116945941</v>
+        <v>0.1641584912521373</v>
       </c>
       <c r="D11">
         <v>4.5283825219602628E-2</v>
@@ -3021,16 +3132,16 @@
         <v>2.2204460492503131E-14</v>
       </c>
       <c r="F11">
-        <v>0.11219420996088636</v>
+        <v>0.11219420894660005</v>
       </c>
       <c r="G11">
-        <v>2.7907712805762291E-2</v>
+        <v>2.6739389223432025E-2</v>
       </c>
       <c r="H11">
-        <v>0.1912830956572997</v>
+        <v>0.19245141659030984</v>
       </c>
       <c r="I11">
-        <v>2.220678713283788E-14</v>
+        <v>2.2206781588809361E-14</v>
       </c>
       <c r="J11">
         <v>2.8612100103634148</v>
@@ -3042,22 +3153,22 @@
         <v>44059879.020455331</v>
       </c>
       <c r="M11">
-        <v>0.99213822043396527</v>
+        <v>0.99213822043396482</v>
       </c>
       <c r="N11">
-        <v>0.9941083818611266</v>
+        <v>0.99410838184506134</v>
       </c>
       <c r="O11">
-        <v>0.9931954834310559</v>
+        <v>0.99319548348425291</v>
       </c>
       <c r="P11">
-        <v>0.1244693135745752</v>
+        <v>0.12446931357457527</v>
       </c>
       <c r="Q11">
-        <v>0.11716632909466702</v>
+        <v>0.11716632920010855</v>
       </c>
       <c r="R11">
-        <v>0.14608669120313791</v>
+        <v>0.14608669072309458</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -3065,28 +3176,28 @@
         <v>1.9955136692618142E-2</v>
       </c>
       <c r="B12">
-        <v>7.9999999925458518E-2</v>
+        <v>7.9999999969555299E-2</v>
       </c>
       <c r="C12">
-        <v>2.0255347403533834</v>
+        <v>2.025498154431006</v>
       </c>
       <c r="D12">
-        <v>3.743080798212025E-2</v>
+        <v>3.7430807982120715E-2</v>
       </c>
       <c r="E12">
-        <v>8.7712000008480648E-11</v>
+        <v>4.813190262085224E-11</v>
       </c>
       <c r="F12">
-        <v>0.17802086871048331</v>
+        <v>0.17802513032889813</v>
       </c>
       <c r="G12">
-        <v>2.7254606660231238E-2</v>
+        <v>2.6557682885802104E-2</v>
       </c>
       <c r="H12">
-        <v>0.37298046554230757</v>
+        <v>0.37369127504783234</v>
       </c>
       <c r="I12">
-        <v>4.2061220201406451E-14</v>
+        <v>4.2438187820793242E-14</v>
       </c>
       <c r="J12">
         <v>5.3408895358905601</v>
@@ -3098,22 +3209,22 @@
         <v>1300249383.1199305</v>
       </c>
       <c r="M12">
-        <v>0.97974716407633577</v>
+        <v>0.97974716357598268</v>
       </c>
       <c r="N12">
-        <v>0.92111109262738655</v>
+        <v>0.92111167361335022</v>
       </c>
       <c r="O12">
-        <v>0.9665478692100018</v>
+        <v>0.96654862729160018</v>
       </c>
       <c r="P12">
-        <v>0.20055742264008816</v>
+        <v>0.20055742706207924</v>
       </c>
       <c r="Q12">
-        <v>0.38893113536251583</v>
+        <v>0.38892998015242602</v>
       </c>
       <c r="R12">
-        <v>0.2554218925098875</v>
+        <v>0.25541943931821498</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -3121,28 +3232,28 @@
         <v>1.9932134010064936E-2</v>
       </c>
       <c r="B13">
-        <v>8.6303588037475228E-3</v>
+        <v>8.6403546782031753E-3</v>
       </c>
       <c r="C13">
-        <v>7.0006500510403802E-2</v>
+        <v>6.9996504707704105E-2</v>
       </c>
       <c r="D13">
-        <v>4.1170586868978926E-2</v>
+        <v>4.117029077902333E-2</v>
       </c>
       <c r="E13">
-        <v>5.5658565145741159E-10</v>
+        <v>5.5774294888870558E-10</v>
       </c>
       <c r="F13">
-        <v>0.14683860166190704</v>
+        <v>0.14710121465685502</v>
       </c>
       <c r="G13">
-        <v>2.7468048982434077E-2</v>
+        <v>2.7606148348276426E-2</v>
       </c>
       <c r="H13">
-        <v>0.48074592166083729</v>
+        <v>0.48172107020411004</v>
       </c>
       <c r="I13">
-        <v>3.1217319623019556E-14</v>
+        <v>3.1310055328609909E-14</v>
       </c>
       <c r="J13">
         <v>4.079138265678818</v>
@@ -3154,22 +3265,22 @@
         <v>566450101.24093688</v>
       </c>
       <c r="M13">
-        <v>0.99898533074447748</v>
+        <v>0.99898533074451068</v>
       </c>
       <c r="N13">
-        <v>0.99700310027273165</v>
+        <v>0.99701139548014506</v>
       </c>
       <c r="O13">
-        <v>0.94962356518139168</v>
+        <v>0.949541110127199</v>
       </c>
       <c r="P13">
-        <v>4.4815903611918569E-2</v>
+        <v>4.4815903611969979E-2</v>
       </c>
       <c r="Q13">
-        <v>8.2496491770333358E-2</v>
+        <v>8.2400008207427697E-2</v>
       </c>
       <c r="R13">
-        <v>0.32487242852744064</v>
+        <v>0.32512088803992523</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -3177,28 +3288,28 @@
         <v>1.9701617767527744E-2</v>
       </c>
       <c r="B14">
-        <v>4.8531921077507928E-3</v>
+        <v>4.8323620306448935E-3</v>
       </c>
       <c r="C14">
-        <v>5.4349210188096514E-3</v>
+        <v>5.4563962150907331E-3</v>
       </c>
       <c r="D14">
-        <v>4.0812904714290117E-2</v>
+        <v>4.0812904702452656E-2</v>
       </c>
       <c r="E14">
-        <v>2.2205657938482613E-14</v>
+        <v>1.7651220104339856E-5</v>
       </c>
       <c r="F14">
-        <v>3.196791962289873E-2</v>
+        <v>3.1617351973594027E-2</v>
       </c>
       <c r="G14">
-        <v>2.6888850517590504E-2</v>
+        <v>2.725000798928098E-2</v>
       </c>
       <c r="H14">
-        <v>5.0314473731856428E-2</v>
+        <v>4.7124138988605048E-2</v>
       </c>
       <c r="I14">
-        <v>2.2206387416510339E-14</v>
+        <v>1.6211893547391038E-5</v>
       </c>
       <c r="J14">
         <v>4.5658015908569123</v>
@@ -3210,22 +3321,22 @@
         <v>350999697.1980691</v>
       </c>
       <c r="M14">
-        <v>0.9920818371300687</v>
+        <v>0.99208181807768536</v>
       </c>
       <c r="N14">
-        <v>0.99509847735677082</v>
+        <v>0.99508377256621872</v>
       </c>
       <c r="O14">
-        <v>0.99223511727108593</v>
+        <v>0.99253225813286505</v>
       </c>
       <c r="P14">
-        <v>0.12573147808382509</v>
+        <v>0.12573170714751689</v>
       </c>
       <c r="Q14">
-        <v>0.10222338418604916</v>
+        <v>0.10237015179103715</v>
       </c>
       <c r="R14">
-        <v>0.12736077698237508</v>
+        <v>0.12637696756741412</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -3233,28 +3344,28 @@
         <v>1.9647451233942632E-2</v>
       </c>
       <c r="B15">
-        <v>9.627872480943607E-3</v>
+        <v>1.1560450572118007E-2</v>
       </c>
       <c r="C15">
-        <v>8.9047001675236492E-2</v>
+        <v>8.4848356183085338E-2</v>
       </c>
       <c r="D15">
-        <v>8.8738460064248847E-2</v>
+        <v>8.8738451615117273E-2</v>
       </c>
       <c r="E15">
-        <v>5.6390850247455285E-2</v>
+        <v>2.407360763413255E-14</v>
       </c>
       <c r="F15">
-        <v>4.9463066903380537E-2</v>
+        <v>0.15210747569666191</v>
       </c>
       <c r="G15">
-        <v>2.6531612173443107E-2</v>
+        <v>2.6611480178405034E-2</v>
       </c>
       <c r="H15">
-        <v>1.7749446787341829E-2</v>
+        <v>0.22793467277447976</v>
       </c>
       <c r="I15">
-        <v>2.2204460492503134E-14</v>
+        <v>3.8305931461935391E-14</v>
       </c>
       <c r="J15">
         <v>6.1031742274447058</v>
@@ -3266,22 +3377,22 @@
         <v>621934179.43162954</v>
       </c>
       <c r="M15">
-        <v>0.99881950192869984</v>
+        <v>0.99882163160938198</v>
       </c>
       <c r="N15">
-        <v>0.99064358139121333</v>
+        <v>0.99270388667667397</v>
       </c>
       <c r="O15">
-        <v>0.99551992106544251</v>
+        <v>0.96037915720805644</v>
       </c>
       <c r="P15">
-        <v>4.8333595585898143E-2</v>
+        <v>4.8286264033468369E-2</v>
       </c>
       <c r="Q15">
-        <v>0.13658324134745867</v>
+        <v>0.12081206714507217</v>
       </c>
       <c r="R15">
-        <v>9.4634382892265181E-2</v>
+        <v>0.28282810134363656</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -3289,28 +3400,28 @@
         <v>2.0254106371624593E-2</v>
       </c>
       <c r="B16">
-        <v>4.2024994929391157E-2</v>
+        <v>4.4712314332643145E-2</v>
       </c>
       <c r="C16">
-        <v>0.34134196746157353</v>
+        <v>0.33865466146936779</v>
       </c>
       <c r="D16">
-        <v>0.10027579446088565</v>
+        <v>0.10027579446083579</v>
       </c>
       <c r="E16">
-        <v>2.9855443318929956E-14</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F16">
-        <v>1.7899211107826469</v>
+        <v>1.8828390630124936</v>
       </c>
       <c r="G16">
-        <v>2.7971494228706484E-2</v>
+        <v>2.8011204481770472E-2</v>
       </c>
       <c r="H16">
-        <v>9.4849226840399314</v>
+        <v>9.9999999999999787</v>
       </c>
       <c r="I16">
-        <v>2.6571694255680331E-2</v>
+        <v>4.8819468832966442E-10</v>
       </c>
       <c r="J16">
         <v>2.8975994027540488</v>
@@ -3322,22 +3433,22 @@
         <v>818269300.73777747</v>
       </c>
       <c r="M16">
-        <v>0.99463967383740048</v>
+        <v>0.99463967383988361</v>
       </c>
       <c r="N16">
-        <v>0.98554427788440924</v>
+        <v>0.985550803068721</v>
       </c>
       <c r="O16">
-        <v>0.96926536999337842</v>
+        <v>0.96924532881281233</v>
       </c>
       <c r="P16">
-        <v>0.10311916123842756</v>
+        <v>0.10311916123851592</v>
       </c>
       <c r="Q16">
-        <v>0.1976119229343552</v>
+        <v>0.19758020614782132</v>
       </c>
       <c r="R16">
-        <v>0.24689019208859553</v>
+        <v>0.24695341960909117</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -3345,28 +3456,28 @@
         <v>2.0450312385911232E-2</v>
       </c>
       <c r="B17">
-        <v>9.3435384200383689E-3</v>
+        <v>8.923362709430319E-3</v>
       </c>
       <c r="C17">
-        <v>1.1050665543482184E-3</v>
+        <v>1.5268678764787176E-3</v>
       </c>
       <c r="D17">
-        <v>4.2219008518471456E-2</v>
+        <v>4.1485128594566129E-2</v>
       </c>
       <c r="E17">
-        <v>2.220696738411126E-14</v>
+        <v>5.0322381980571912E-5</v>
       </c>
       <c r="F17">
-        <v>0.21221525779359884</v>
+        <v>0.20035088574662624</v>
       </c>
       <c r="G17">
-        <v>2.7170384351094545E-2</v>
+        <v>2.8011204470866559E-2</v>
       </c>
       <c r="H17">
-        <v>8.9267209506379522E-2</v>
+        <v>7.8836529817834081E-2</v>
       </c>
       <c r="I17">
-        <v>2.2211782591808451E-14</v>
+        <v>4.4177389542715639E-14</v>
       </c>
       <c r="J17">
         <v>4.9944093087717132</v>
@@ -3378,22 +3489,22 @@
         <v>87097810.529802099</v>
       </c>
       <c r="M17">
-        <v>0.99683911484766763</v>
+        <v>0.99683910813226995</v>
       </c>
       <c r="N17">
-        <v>0.98740155673778607</v>
+        <v>0.9867659528053907</v>
       </c>
       <c r="O17">
-        <v>0.99844606140128356</v>
+        <v>0.99860625939314263</v>
       </c>
       <c r="P17">
-        <v>8.2129029009645013E-2</v>
+        <v>8.2129228260778453E-2</v>
       </c>
       <c r="Q17">
-        <v>0.16423494191797422</v>
+        <v>0.16814307852940949</v>
       </c>
       <c r="R17">
-        <v>7.1876583365455757E-2</v>
+        <v>6.8346251598520716E-2</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -3401,28 +3512,28 @@
         <v>1.9778014887334602E-2</v>
       </c>
       <c r="B18">
-        <v>5.2535973914847801E-2</v>
+        <v>5.2535975976707519E-2</v>
       </c>
       <c r="C18">
-        <v>0.1220885500548423</v>
+        <v>0.12208854799275491</v>
       </c>
       <c r="D18">
         <v>7.614398766366591E-2</v>
       </c>
       <c r="E18">
-        <v>2.2204575762001667E-14</v>
+        <v>2.2204554673015353E-14</v>
       </c>
       <c r="F18">
-        <v>0.72928379746225713</v>
+        <v>0.72928382779249157</v>
       </c>
       <c r="G18">
-        <v>2.7178228651287956E-2</v>
+        <v>2.7631055008154236E-2</v>
       </c>
       <c r="H18">
-        <v>0.58035583052288708</v>
+        <v>0.57990303234465335</v>
       </c>
       <c r="I18">
-        <v>2.2204460492503131E-14</v>
+        <v>2.2204460492503134E-14</v>
       </c>
       <c r="J18">
         <v>3.2428732950368784</v>
@@ -3434,22 +3545,22 @@
         <v>776346501.63544285</v>
       </c>
       <c r="M18">
-        <v>0.9970477573193044</v>
+        <v>0.99704775731930395</v>
       </c>
       <c r="N18">
-        <v>0.9785036595683777</v>
+        <v>0.97850365971070608</v>
       </c>
       <c r="O18">
-        <v>0.99708218393044046</v>
+        <v>0.99708218383603886</v>
       </c>
       <c r="P18">
-        <v>7.8493392353228636E-2</v>
+        <v>7.8493392353228289E-2</v>
       </c>
       <c r="Q18">
-        <v>0.20798423455190898</v>
+        <v>0.20798423390640772</v>
       </c>
       <c r="R18">
-        <v>7.9032399686020688E-2</v>
+        <v>7.9032400824502233E-2</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -3460,25 +3571,25 @@
         <v>7.9999999999977797E-2</v>
       </c>
       <c r="C19">
-        <v>8.4733541986995835E-3</v>
+        <v>8.4733543146847997E-3</v>
       </c>
       <c r="D19">
         <v>3.8974783538952548E-2</v>
       </c>
       <c r="E19">
-        <v>2.2204473620092633E-14</v>
+        <v>2.2204473777882011E-14</v>
       </c>
       <c r="F19">
-        <v>7.493035061202255E-2</v>
+        <v>7.4930334020398101E-2</v>
       </c>
       <c r="G19">
         <v>2.6525198939014245E-2</v>
       </c>
       <c r="H19">
-        <v>1.0000022204483692E-8</v>
+        <v>1.0000022204521512E-8</v>
       </c>
       <c r="I19">
-        <v>6.7157354651310678E-3</v>
+        <v>6.715716657390027E-3</v>
       </c>
       <c r="J19">
         <v>2.8613040667312468</v>
@@ -3490,22 +3601,22 @@
         <v>13771138.993237138</v>
       </c>
       <c r="M19">
-        <v>0.99722462033685133</v>
+        <v>0.99722462033937131</v>
       </c>
       <c r="N19">
-        <v>0.90128298590350586</v>
+        <v>0.90128299723359717</v>
       </c>
       <c r="O19">
-        <v>0.88340065021593372</v>
+        <v>0.8834006306256792</v>
       </c>
       <c r="P19">
-        <v>9.6944412788679282E-2</v>
+        <v>9.6944412290866436E-2</v>
       </c>
       <c r="Q19">
-        <v>0.48904518101962768</v>
+        <v>0.48904516178599816</v>
       </c>
       <c r="R19">
-        <v>0.4914843489655748</v>
+        <v>0.49148438074501466</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -3513,10 +3624,10 @@
         <v>2.025226724750458E-2</v>
       </c>
       <c r="B20">
-        <v>3.6610394237411199E-2</v>
+        <v>3.661038817423995E-2</v>
       </c>
       <c r="C20">
-        <v>0.58530338624016431</v>
+        <v>0.58530339194918313</v>
       </c>
       <c r="D20">
         <v>4.2860723219890554E-2</v>
@@ -3525,16 +3636,16 @@
         <v>9.9999999999977801E-2</v>
       </c>
       <c r="F20">
-        <v>0.13494304149684497</v>
+        <v>0.13494299556910744</v>
       </c>
       <c r="G20">
-        <v>2.6697220441904895E-2</v>
+        <v>2.6595818555612983E-2</v>
       </c>
       <c r="H20">
-        <v>0.20576074697735836</v>
+        <v>0.20586204465426139</v>
       </c>
       <c r="I20">
-        <v>2.2204520153601782E-14</v>
+        <v>2.2204503459977956E-14</v>
       </c>
       <c r="J20">
         <v>2.4328816932437634</v>
@@ -3546,22 +3657,22 @@
         <v>898068381.93210459</v>
       </c>
       <c r="M20">
-        <v>0.99345692483603432</v>
+        <v>0.99345692483643755</v>
       </c>
       <c r="N20">
-        <v>0.98644924483382412</v>
+        <v>0.98644924290192071</v>
       </c>
       <c r="O20">
-        <v>0.99602689356091656</v>
+        <v>0.99602689796079291</v>
       </c>
       <c r="P20">
-        <v>0.11612890078590109</v>
+        <v>0.11612890077785666</v>
       </c>
       <c r="Q20">
-        <v>0.16359251437137434</v>
+        <v>0.16359252591784523</v>
       </c>
       <c r="R20">
-        <v>0.10046399115229929</v>
+        <v>0.10046394420079181</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -3569,28 +3680,28 @@
         <v>1.9645457395348342E-2</v>
       </c>
       <c r="B21">
-        <v>7.999999969639035E-2</v>
+        <v>7.9999999999977797E-2</v>
       </c>
       <c r="C21">
-        <v>2.4876344378921567</v>
+        <v>2.4870592214691891</v>
       </c>
       <c r="D21">
         <v>4.3368027883496717E-2</v>
       </c>
       <c r="E21">
-        <v>1.3998598631217543E-11</v>
+        <v>2.2205191754949247E-14</v>
       </c>
       <c r="F21">
-        <v>0.21715615093832816</v>
+        <v>0.21720927390656489</v>
       </c>
       <c r="G21">
-        <v>2.8011204417167476E-2</v>
+        <v>2.6542277456997741E-2</v>
       </c>
       <c r="H21">
-        <v>0.27813434933478431</v>
+        <v>0.27970150312629444</v>
       </c>
       <c r="I21">
-        <v>4.4407599454196846E-14</v>
+        <v>2.220448407366131E-14</v>
       </c>
       <c r="J21">
         <v>2.9741152430411644</v>
@@ -3602,22 +3713,22 @@
         <v>1569235476.0781155</v>
       </c>
       <c r="M21">
-        <v>0.98728130909460743</v>
+        <v>0.98728130885977849</v>
       </c>
       <c r="N21">
-        <v>0.98447227112887148</v>
+        <v>0.98447514473401299</v>
       </c>
       <c r="O21">
-        <v>0.99243717845547119</v>
+        <v>0.99243473711185037</v>
       </c>
       <c r="P21">
-        <v>0.15890606912614766</v>
+        <v>0.15890607310726296</v>
       </c>
       <c r="Q21">
-        <v>0.1769022454805079</v>
+        <v>0.17688630763901789</v>
       </c>
       <c r="R21">
-        <v>0.1264643359454091</v>
+        <v>0.12648227289179581</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -3628,25 +3739,25 @@
         <v>7.9999999999977797E-2</v>
       </c>
       <c r="C22">
-        <v>2.460712875654123</v>
+        <v>2.4607134617885431</v>
       </c>
       <c r="D22">
         <v>4.4657955198512699E-2</v>
       </c>
       <c r="E22">
-        <v>2.2205001040125017E-14</v>
+        <v>2.220960075234407E-14</v>
       </c>
       <c r="F22">
-        <v>0.26729357793174779</v>
+        <v>0.26729351310643173</v>
       </c>
       <c r="G22">
-        <v>2.7270617048256635E-2</v>
+        <v>2.655305918638852E-2</v>
       </c>
       <c r="H22">
-        <v>0.37209960909669204</v>
+        <v>0.37281704729437759</v>
       </c>
       <c r="I22">
-        <v>2.2204460492503131E-14</v>
+        <v>2.2204943639415854E-14</v>
       </c>
       <c r="J22">
         <v>3.8163808997580695</v>
@@ -3658,22 +3769,22 @@
         <v>911747954.02784622</v>
       </c>
       <c r="M22">
-        <v>0.99437216182669408</v>
+        <v>0.99437216182671762</v>
       </c>
       <c r="N22">
-        <v>0.96042882673898133</v>
+        <v>0.96042882358742254</v>
       </c>
       <c r="O22">
-        <v>0.9954532776458449</v>
+        <v>0.99545327999674993</v>
       </c>
       <c r="P22">
-        <v>0.10664431576442432</v>
+        <v>0.10664431575955506</v>
       </c>
       <c r="Q22">
-        <v>0.28177652324731872</v>
+        <v>0.28177653343532372</v>
       </c>
       <c r="R22">
-        <v>9.5764827670516667E-2</v>
+        <v>9.5764802955078374E-2</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -3721,7 +3832,7 @@
       </c>
       <c r="T23" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U23" t="str">
         <f t="shared" si="0"/>
@@ -3868,7 +3979,7 @@
       </c>
       <c r="T25" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U25" t="str">
         <f t="shared" si="0"/>
@@ -3902,7 +4013,7 @@
       </c>
       <c r="P26" t="str">
         <f t="shared" si="0"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="0"/>
@@ -3986,7 +4097,7 @@
       </c>
       <c r="T27" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U27" t="str">
         <f t="shared" si="0"/>
@@ -4015,27 +4126,27 @@
       </c>
       <c r="C28">
         <f>AVERAGE(B$1:B$3)</f>
-        <v>3.6349270531761137E-3</v>
+        <v>3.6597166972760207E-3</v>
       </c>
       <c r="D28">
         <f>AVERAGE(B$4:B$6)</f>
-        <v>1.5890787210518401E-2</v>
+        <v>1.2969578710698102E-2</v>
       </c>
       <c r="E28">
         <f>AVERAGE(B$7:B$12,B$17:B$19)</f>
-        <v>3.860466689820248E-2</v>
+        <v>3.9850373025406699E-2</v>
       </c>
       <c r="F28">
         <f>AVERAGE(B$13:B$16)</f>
-        <v>1.6284104580458269E-2</v>
+        <v>1.7436370403402304E-2</v>
       </c>
       <c r="G28">
         <f>B$20</f>
-        <v>3.6610394237411199E-2</v>
+        <v>3.661038817423995E-2</v>
       </c>
       <c r="H28">
         <f>AVERAGE(B$21:B$22)</f>
-        <v>7.9999999848184067E-2</v>
+        <v>7.9999999999977797E-2</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="2"/>
@@ -4047,7 +4158,7 @@
       </c>
       <c r="P28" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="0"/>
@@ -4063,7 +4174,7 @@
       </c>
       <c r="T28" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Ok</v>
       </c>
       <c r="U28" t="str">
         <f t="shared" si="0"/>
@@ -4089,23 +4200,23 @@
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>STDEV(B$1:B$3)/SQRT(COUNT(B$1:B$3))</f>
-        <v>1.5384056711341255E-4</v>
+        <v>1.3632467423976377E-4</v>
       </c>
       <c r="D29">
         <f>STDEV(B$4:B$6)/SQRT(COUNT(B$4:B$6))</f>
-        <v>1.7821996996424904E-3</v>
+        <v>2.8102841025300172E-3</v>
       </c>
       <c r="E29">
         <f>STDEV(B$7:B$12,B$17:B$19)/SQRT(COUNT(B$7:B$12,B$17:B$19))</f>
-        <v>1.0379987715457955E-2</v>
+        <v>1.0181144930654133E-2</v>
       </c>
       <c r="F29">
         <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
-        <v>8.6416840859272169E-3</v>
+        <v>9.1957167148318739E-3</v>
       </c>
       <c r="H29">
         <f>STDEV(B$21:B$22)/SQRT(COUNT(B$21:B$22))</f>
-        <v>1.5179372342410973E-10</v>
+        <v>0</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="2"/>
@@ -4183,7 +4294,7 @@
       </c>
       <c r="T30" t="str">
         <f t="shared" si="0"/>
-        <v>Lower</v>
+        <v>Ok</v>
       </c>
       <c r="U30" t="str">
         <f t="shared" si="0"/>
@@ -4280,27 +4391,27 @@
       </c>
       <c r="D32">
         <f>AVERAGE(C$1:C$3)</f>
-        <v>0.19026021724961684</v>
+        <v>0.19023535438688108</v>
       </c>
       <c r="E32">
         <f>AVERAGE(C$4:C$6)</f>
-        <v>0.1080660739204507</v>
+        <v>0.11098762168381754</v>
       </c>
       <c r="F32">
         <f>AVERAGE(C$7:C$12,C$17:C$19)</f>
-        <v>0.31388842663920424</v>
+        <v>0.31184021552856422</v>
       </c>
       <c r="G32">
         <f>AVERAGE(C$13:C$16)</f>
-        <v>0.12645759766650588</v>
+        <v>0.12473897964381199</v>
       </c>
       <c r="H32">
         <f>C$20</f>
-        <v>0.58530338624016431</v>
+        <v>0.58530339194918313</v>
       </c>
       <c r="I32">
         <f>AVERAGE(C$21:C$22)</f>
-        <v>2.4741736567731398</v>
+        <v>2.4738863416288659</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="2"/>
@@ -4354,23 +4465,23 @@
     <row r="33" spans="4:31" x14ac:dyDescent="0.25">
       <c r="D33">
         <f>STDEV(C$1:C$3)/SQRT(COUNT(C$1:C$3))</f>
-        <v>3.4739541259219485E-2</v>
+        <v>3.4764251947037965E-2</v>
       </c>
       <c r="E33">
         <f>STDEV(C$4:C$6)/SQRT(COUNT(C$4:C$6))</f>
-        <v>0.10806587260999787</v>
+        <v>0.10709949468666879</v>
       </c>
       <c r="F33">
         <f>STDEV(C$7:C$12,C$17:C$19)/SQRT(COUNT(C$7:C$12,C$17:C$19))</f>
-        <v>0.21632336737711033</v>
+        <v>0.21648529436558617</v>
       </c>
       <c r="G33">
         <f>STDEV(C$13:C$16)/SQRT(COUNT(C$13:C$16))</f>
-        <v>7.3828664096759575E-2</v>
+        <v>7.3357716046404037E-2</v>
       </c>
       <c r="I33">
         <f>STDEV(C$21:C$22)/SQRT(COUNT(C$21:C$22))</f>
-        <v>1.3460781119016829E-2</v>
+        <v>1.3172879840323004E-2</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="2"/>
@@ -4398,7 +4509,7 @@
       </c>
       <c r="T33" t="str">
         <f t="shared" si="0"/>
-        <v>Upper</v>
+        <v>Lower</v>
       </c>
       <c r="U33" t="str">
         <f t="shared" si="0"/>
@@ -4448,7 +4559,7 @@
       </c>
       <c r="T34" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U34" t="str">
         <f t="shared" si="0"/>
@@ -4545,19 +4656,19 @@
       </c>
       <c r="E36">
         <f>AVERAGE(D$1:D$3)</f>
-        <v>5.9621023729002159E-2</v>
+        <v>5.9621023719336724E-2</v>
       </c>
       <c r="F36">
         <f>AVERAGE(D$4:D$6)</f>
-        <v>5.8604737815521259E-2</v>
+        <v>5.8426894246005306E-2</v>
       </c>
       <c r="G36">
         <f>AVERAGE(D$7:D$12,D$17:D$19)</f>
-        <v>5.4181347058612668E-2</v>
+        <v>5.408192058558043E-2</v>
       </c>
       <c r="H36">
         <f>AVERAGE(D$13:D$16)</f>
-        <v>6.7749436527100887E-2</v>
+        <v>6.7749360389357263E-2</v>
       </c>
       <c r="I36">
         <f>D$20</f>
@@ -4619,19 +4730,19 @@
     <row r="37" spans="4:31" x14ac:dyDescent="0.25">
       <c r="E37">
         <f>STDEV(D$1:D$3)/SQRT(COUNT(D$1:D$3))</f>
-        <v>2.0792372890740287E-2</v>
+        <v>2.0792372896380848E-2</v>
       </c>
       <c r="F37">
         <f>STDEV(D$4:D$6)/SQRT(COUNT(D$4:D$6))</f>
-        <v>1.704736678030936E-2</v>
+        <v>1.7123224610862724E-2</v>
       </c>
       <c r="G37">
         <f>STDEV(D$7:D$12,D$17:D$19)/SQRT(COUNT(D$7:D$12,D$17:D$19))</f>
-        <v>5.1060170071972532E-3</v>
+        <v>5.1216710439505198E-3</v>
       </c>
       <c r="H37">
         <f>STDEV(D$13:D$16)/SQRT(COUNT(D$13:D$16))</f>
-        <v>1.5627206683460862E-2</v>
+        <v>1.5627247705565079E-2</v>
       </c>
       <c r="J37">
         <f>STDEV(D$21:D$22)/SQRT(COUNT(D$21:D$22))</f>
@@ -4717,7 +4828,7 @@
       </c>
       <c r="U38" t="str">
         <f t="shared" si="0"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="0"/>
@@ -4781,7 +4892,7 @@
       </c>
       <c r="T39" t="str">
         <f t="shared" si="2"/>
-        <v>Ok</v>
+        <v>Upper</v>
       </c>
       <c r="U39" t="str">
         <f t="shared" si="2"/>
@@ -4810,19 +4921,19 @@
       </c>
       <c r="F40">
         <f>AVERAGE(E$1:E$3)</f>
-        <v>3.14046423094368E-14</v>
+        <v>2.2210033221700154E-14</v>
       </c>
       <c r="G40">
         <f>AVERAGE(E$4:E$6)</f>
-        <v>2.9610066609493058E-14</v>
+        <v>2.8172663076369224E-7</v>
       </c>
       <c r="H40">
         <f>AVERAGE(E$7:E$12,E$17:E$19)</f>
-        <v>9.9120070516456917E-3</v>
+        <v>4.0146854743199973E-4</v>
       </c>
       <c r="I40">
         <f>AVERAGE(E$13:E$16)</f>
-        <v>1.409771270102325E-2</v>
+        <v>4.4129444733917032E-6</v>
       </c>
       <c r="J40">
         <f>E$20</f>
@@ -4830,7 +4941,7 @@
       </c>
       <c r="K40">
         <f>AVERAGE(E$21:E$22)</f>
-        <v>7.010401816128834E-12</v>
+        <v>2.2207396253646659E-14</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="2"/>
@@ -4884,23 +4995,23 @@
     <row r="41" spans="4:31" x14ac:dyDescent="0.25">
       <c r="F41">
         <f>STDEV(E$1:E$3)/SQRT(COUNT(E$1:E$3))</f>
-        <v>4.6328885002813328E-15</v>
+        <v>4.8250618270174104E-18</v>
       </c>
       <c r="G41">
         <f>STDEV(E$4:E$6)/SQRT(COUNT(E$4:E$6))</f>
-        <v>6.7865780911876414E-15</v>
+        <v>2.8172660276019622E-7</v>
       </c>
       <c r="H41">
         <f>STDEV(E$7:E$12,E$17:E$19)/SQRT(COUNT(E$7:E$12,E$17:E$19))</f>
-        <v>9.912007040659046E-3</v>
+        <v>2.8632212313389749E-4</v>
       </c>
       <c r="I41">
         <f>STDEV(E$13:E$16)/SQRT(COUNT(E$13:E$16))</f>
-        <v>1.4097712515477347E-2</v>
+        <v>4.4127585456074152E-6</v>
       </c>
       <c r="K41">
         <f>STDEV(E$21:E$22)/SQRT(COUNT(E$21:E$22))</f>
-        <v>6.9881968150887084E-12</v>
+        <v>2.2044986974114701E-18</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="2"/>
@@ -5046,7 +5157,7 @@
       </c>
       <c r="T43" t="str">
         <f t="shared" si="2"/>
-        <v>Upper</v>
+        <v>Lower</v>
       </c>
       <c r="U43" t="str">
         <f t="shared" si="2"/>
@@ -5075,27 +5186,27 @@
       </c>
       <c r="G44">
         <f>AVERAGE(F$1:F$3)</f>
-        <v>0.13093022863689935</v>
+        <v>0.14700895503484715</v>
       </c>
       <c r="H44">
         <f>AVERAGE(F$4:F$6)</f>
-        <v>0.67407664196283246</v>
+        <v>0.51874426073426694</v>
       </c>
       <c r="I44">
         <f>AVERAGE(F$7:F$12,F$17:F$19)</f>
-        <v>0.60897305684494307</v>
+        <v>0.67733097633142481</v>
       </c>
       <c r="J44">
         <f>AVERAGE(F$13:F$16)</f>
-        <v>0.50454767474270834</v>
+        <v>0.55341627633490109</v>
       </c>
       <c r="K44">
         <f>F$20</f>
-        <v>0.13494304149684497</v>
+        <v>0.13494299556910744</v>
       </c>
       <c r="L44">
         <f>AVERAGE(F$21:F$22)</f>
-        <v>0.24222486443503799</v>
+        <v>0.24225139350649832</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="2"/>
@@ -5123,7 +5234,7 @@
       </c>
       <c r="T44" t="str">
         <f t="shared" si="2"/>
-        <v>Ok</v>
+        <v>Lower</v>
       </c>
       <c r="U44" t="str">
         <f t="shared" si="2"/>
@@ -5149,23 +5260,23 @@
     <row r="45" spans="4:31" x14ac:dyDescent="0.25">
       <c r="G45">
         <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
-        <v>2.2095893884320664E-2</v>
+        <v>3.7887236211488991E-2</v>
       </c>
       <c r="H45">
         <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
-        <v>0.13947133847608845</v>
+        <v>0.12579716058654763</v>
       </c>
       <c r="I45">
         <f>STDEV(F$7:F$12,F$17:F$19)/SQRT(COUNT(F$7:F$12,F$17:F$19))</f>
-        <v>0.33459226592417918</v>
+        <v>0.34452837581693579</v>
       </c>
       <c r="J45">
         <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
-        <v>0.42920219363787993</v>
+        <v>0.44401386483779698</v>
       </c>
       <c r="L45">
         <f>STDEV(F$21:F$22)/SQRT(COUNT(F$21:F$22))</f>
-        <v>2.5068713496709742E-2</v>
+        <v>2.5042119599933226E-2</v>
       </c>
       <c r="N45" t="s">
         <v>17</v>
@@ -5248,49 +5359,49 @@
       </c>
       <c r="H48">
         <f>AVERAGE(G$1:G$3)</f>
-        <v>2.694202425692711E-2</v>
+        <v>2.6612095404732927E-2</v>
       </c>
       <c r="I48">
         <f>AVERAGE(G$4:G$6)</f>
-        <v>2.7575532960729815E-2</v>
+        <v>2.7473079382476524E-2</v>
       </c>
       <c r="J48">
         <f>AVERAGE(G$7:G$12,G$17:G$19)</f>
-        <v>2.7214793344027752E-2</v>
+        <v>2.7283317623498213E-2</v>
       </c>
       <c r="K48">
         <f>AVERAGE(G$13:G$16)</f>
-        <v>2.7215001475543541E-2</v>
+        <v>2.7369710249433226E-2</v>
       </c>
       <c r="L48">
         <f>G$20</f>
-        <v>2.6697220441904895E-2</v>
+        <v>2.6595818555612983E-2</v>
       </c>
       <c r="M48">
         <f>AVERAGE(G$21:G$22)</f>
-        <v>2.7640910732712055E-2</v>
+        <v>2.654766832169313E-2</v>
       </c>
     </row>
     <row r="49" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H49">
         <f>STDEV(G$1:G$3)/SQRT(COUNT(G$1:G$3))</f>
-        <v>2.249171193521747E-4</v>
+        <v>4.5088837848277105E-5</v>
       </c>
       <c r="I49">
         <f>STDEV(G$4:G$6)/SQRT(COUNT(G$4:G$6))</f>
-        <v>3.8779530011327079E-4</v>
+        <v>3.7252970632583378E-4</v>
       </c>
       <c r="J49">
         <f>STDEV(G$7:G$12,G$17:G$19)/SQRT(COUNT(G$7:G$12,G$17:G$19))</f>
-        <v>1.6090090020469541E-4</v>
+        <v>1.9591704856672309E-4</v>
       </c>
       <c r="K49">
         <f>STDEV(G$13:G$16)/SQRT(COUNT(G$13:G$16))</f>
-        <v>3.175045553387866E-4</v>
+        <v>2.9674052868955972E-4</v>
       </c>
       <c r="M49">
         <f>STDEV(G$21:G$22)/SQRT(COUNT(G$21:G$22))</f>
-        <v>3.7029368445542013E-4</v>
+        <v>5.3908646953891581E-6</v>
       </c>
     </row>
     <row r="51" spans="8:17" x14ac:dyDescent="0.25">
@@ -5319,49 +5430,49 @@
       </c>
       <c r="I52">
         <f>AVERAGE(H$1:H$3)</f>
-        <v>7.3385350453566617E-2</v>
+        <v>7.5917629324230532E-2</v>
       </c>
       <c r="J52">
         <f>AVERAGE(H$4:H$6)</f>
-        <v>0.547422931371088</v>
+        <v>0.39118585551184881</v>
       </c>
       <c r="K52">
         <f>AVERAGE(H$7:H$12,H$17:H$19)</f>
-        <v>1.3330374174930695</v>
+        <v>1.4556807367818019</v>
       </c>
       <c r="L52">
         <f>AVERAGE(H$13:H$16)</f>
-        <v>2.5084331315549919</v>
+        <v>2.6891949704917932</v>
       </c>
       <c r="M52">
         <f>H$20</f>
-        <v>0.20576074697735836</v>
+        <v>0.20586204465426139</v>
       </c>
       <c r="N52">
         <f>AVERAGE(H$21:H$22)</f>
-        <v>0.32511697921573818</v>
+        <v>0.32625927521033604</v>
       </c>
     </row>
     <row r="53" spans="8:17" x14ac:dyDescent="0.25">
       <c r="I53">
         <f>STDEV(H$1:H$3)/SQRT(COUNT(H$1:H$3))</f>
-        <v>1.9630646643434373E-2</v>
+        <v>2.1967251752266336E-2</v>
       </c>
       <c r="J53">
         <f>STDEV(H$4:H$6)/SQRT(COUNT(H$4:H$6))</f>
-        <v>0.1777565403046821</v>
+        <v>0.14380117024004904</v>
       </c>
       <c r="K53">
         <f>STDEV(H$7:H$12,H$17:H$19)/SQRT(COUNT(H$7:H$12,H$17:H$19))</f>
-        <v>1.0355825368958771</v>
+        <v>1.0473379060285419</v>
       </c>
       <c r="L53">
         <f>STDEV(H$13:H$16)/SQRT(COUNT(H$13:H$16))</f>
-        <v>2.3278884289309234</v>
+        <v>2.4385643271491557</v>
       </c>
       <c r="N53">
         <f>STDEV(H$21:H$22)/SQRT(COUNT(H$21:H$22))</f>
-        <v>4.6982629880953752E-2</v>
+        <v>4.6557772084041354E-2</v>
       </c>
     </row>
     <row r="55" spans="8:17" x14ac:dyDescent="0.25">
@@ -5390,49 +5501,49 @@
       </c>
       <c r="J56">
         <f>AVERAGE(I$1:I$3)</f>
-        <v>2.5057350070406329E-2</v>
+        <v>4.7043281897724644E-2</v>
       </c>
       <c r="K56">
         <f>AVERAGE(I$4:I$6)</f>
-        <v>2.9801432056621328E-14</v>
+        <v>3.4991609077748002E-14</v>
       </c>
       <c r="L56">
         <f>AVERAGE(I$7:I$12,I$17:I$19)</f>
-        <v>7.4619394965597628E-4</v>
+        <v>7.4630219943887829E-4</v>
       </c>
       <c r="M56">
         <f>AVERAGE(I$13:I$16)</f>
-        <v>6.6429235639389895E-3</v>
+        <v>4.0530954529238379E-6</v>
       </c>
       <c r="N56">
         <f>I$20</f>
-        <v>2.2204520153601782E-14</v>
+        <v>2.2204503459977956E-14</v>
       </c>
       <c r="O56">
         <f>AVERAGE(I$21:I$22)</f>
-        <v>3.3306029973349988E-14</v>
+        <v>2.2204713856538582E-14</v>
       </c>
     </row>
     <row r="57" spans="8:17" x14ac:dyDescent="0.25">
       <c r="J57">
         <f>STDEV(I$1:I$3)/SQRT(COUNT(I$1:I$3))</f>
-        <v>2.5057350070384107E-2</v>
+        <v>4.7043281897702433E-2</v>
       </c>
       <c r="K57">
         <f>STDEV(I$4:I$6)/SQRT(COUNT(I$4:I$6))</f>
-        <v>4.3039101842402032E-15</v>
+        <v>6.3772773096146374E-15</v>
       </c>
       <c r="L57">
         <f>STDEV(I$7:I$12,I$17:I$19)/SQRT(COUNT(I$7:I$12,I$17:I$19))</f>
-        <v>7.4619268943521401E-4</v>
+        <v>7.4617681527279955E-4</v>
       </c>
       <c r="M57">
         <f>STDEV(I$13:I$16)/SQRT(COUNT(I$13:I$16))</f>
-        <v>6.6429235639137805E-3</v>
+        <v>4.0529326997889823E-6</v>
       </c>
       <c r="O57">
         <f>STDEV(I$21:I$22)/SQRT(COUNT(I$21:I$22))</f>
-        <v>1.1101569480846858E-14</v>
+        <v>2.2978287727198393E-19</v>
       </c>
     </row>
     <row r="59" spans="8:17" x14ac:dyDescent="0.25">
@@ -5674,49 +5785,49 @@
       </c>
       <c r="N72">
         <f>AVERAGE(M$1:M$3)</f>
-        <v>0.9966299739847897</v>
+        <v>0.99662997411815801</v>
       </c>
       <c r="O72">
         <f>AVERAGE(M$4:M$6)</f>
-        <v>0.99678503497402737</v>
+        <v>0.99678502774392774</v>
       </c>
       <c r="P72">
         <f>AVERAGE(M$7:M$12,M$17:M$19)</f>
-        <v>0.99462465208982254</v>
+        <v>0.9946243241560917</v>
       </c>
       <c r="Q72">
         <f>AVERAGE(M$13:M$16)</f>
-        <v>0.9961315859101616</v>
+        <v>0.99613211356786546</v>
       </c>
       <c r="R72">
         <f>M$20</f>
-        <v>0.99345692483603432</v>
+        <v>0.99345692483643755</v>
       </c>
       <c r="S72">
         <f>AVERAGE(M$21:M$22)</f>
-        <v>0.99082673546065081</v>
+        <v>0.99082673534324806</v>
       </c>
     </row>
     <row r="73" spans="12:21" x14ac:dyDescent="0.25">
       <c r="N73">
         <f>STDEV(M$1:M$3)/SQRT(COUNT(M$1:M$3))</f>
-        <v>4.9336906832299571E-4</v>
+        <v>4.9336913887755639E-4</v>
       </c>
       <c r="O73">
         <f>STDEV(M$4:M$6)/SQRT(COUNT(M$4:M$6))</f>
-        <v>3.4870054519549912E-4</v>
+        <v>3.486949347042988E-4</v>
       </c>
       <c r="P73">
         <f>STDEV(M$7:M$12,M$17:M$19)/SQRT(COUNT(M$7:M$12,M$17:M$19))</f>
-        <v>1.9810876721650956E-3</v>
+        <v>1.9810102119476331E-3</v>
       </c>
       <c r="Q73">
         <f>STDEV(M$13:M$16)/SQRT(COUNT(M$13:M$16))</f>
-        <v>1.6831275183621052E-3</v>
+        <v>1.6834148194512729E-3</v>
       </c>
       <c r="S73">
         <f>STDEV(M$21:M$22)/SQRT(COUNT(M$21:M$22))</f>
-        <v>3.545426366043325E-3</v>
+        <v>3.5454264834695604E-3</v>
       </c>
     </row>
     <row r="75" spans="12:21" x14ac:dyDescent="0.25">
@@ -5745,49 +5856,49 @@
       </c>
       <c r="O76">
         <f>AVERAGE(N$1:N$3)</f>
-        <v>0.99199004042008554</v>
+        <v>0.99199938412162059</v>
       </c>
       <c r="P76">
         <f>AVERAGE(N$4:N$6)</f>
-        <v>0.97765703857899788</v>
+        <v>0.97541479470508063</v>
       </c>
       <c r="Q76">
         <f>AVERAGE(N$7:N$12,N$17:N$19)</f>
-        <v>0.96952285467688271</v>
+        <v>0.96965084484165076</v>
       </c>
       <c r="R76">
         <f>AVERAGE(N$13:N$16)</f>
-        <v>0.99207235922628123</v>
+        <v>0.99258746444793977</v>
       </c>
       <c r="S76">
         <f>N$20</f>
-        <v>0.98644924483382412</v>
+        <v>0.98644924290192071</v>
       </c>
       <c r="T76">
         <f>AVERAGE(N$21:N$22)</f>
-        <v>0.97245054893392635</v>
+        <v>0.97245198416071776</v>
       </c>
     </row>
     <row r="77" spans="12:21" x14ac:dyDescent="0.25">
       <c r="O77">
         <f>STDEV(N$1:N$3)/SQRT(COUNT(N$1:N$3))</f>
-        <v>3.3585110078921065E-3</v>
+        <v>3.3666505227571966E-3</v>
       </c>
       <c r="P77">
         <f>STDEV(N$4:N$6)/SQRT(COUNT(N$4:N$6))</f>
-        <v>8.4748319197353733E-3</v>
+        <v>1.0654580102394942E-2</v>
       </c>
       <c r="Q77">
         <f>STDEV(N$7:N$12,N$17:N$19)/SQRT(COUNT(N$7:N$12,N$17:N$19))</f>
-        <v>1.1836840879492742E-2</v>
+        <v>1.1875659785251722E-2</v>
       </c>
       <c r="R77">
         <f>STDEV(N$13:N$16)/SQRT(COUNT(N$13:N$16))</f>
-        <v>2.5515820307361482E-3</v>
+        <v>2.5055085561655724E-3</v>
       </c>
       <c r="T77">
         <f>STDEV(N$21:N$22)/SQRT(COUNT(N$21:N$22))</f>
-        <v>1.2021722194945071E-2</v>
+        <v>1.2023160573295222E-2</v>
       </c>
     </row>
     <row r="79" spans="12:21" x14ac:dyDescent="0.25">
@@ -5816,49 +5927,49 @@
       </c>
       <c r="P80">
         <f>AVERAGE(O$1:O$3)</f>
-        <v>0.99632589660768345</v>
+        <v>0.99642630127703191</v>
       </c>
       <c r="Q80">
         <f>AVERAGE(O$4:O$6)</f>
-        <v>0.99069032835517212</v>
+        <v>0.98562172652789837</v>
       </c>
       <c r="R80">
         <f>AVERAGE(O$7:O$12,O$17:O$19)</f>
-        <v>0.9784896812049817</v>
+        <v>0.97622736868249915</v>
       </c>
       <c r="S80">
         <f>AVERAGE(O$13:O$16)</f>
-        <v>0.97666099337782453</v>
+        <v>0.96792446357023321</v>
       </c>
       <c r="T80">
         <f>O$20</f>
-        <v>0.99602689356091656</v>
+        <v>0.99602689796079291</v>
       </c>
       <c r="U80">
         <f>AVERAGE(O$21:O$22)</f>
-        <v>0.99394522805065799</v>
+        <v>0.9939440085543001</v>
       </c>
     </row>
     <row r="81" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P81">
         <f>STDEV(O$1:O$3)/SQRT(COUNT(O$1:O$3))</f>
-        <v>8.8842162854062181E-4</v>
+        <v>7.903214212686805E-4</v>
       </c>
       <c r="Q81">
         <f>STDEV(O$4:O$6)/SQRT(COUNT(O$4:O$6))</f>
-        <v>3.9807141063966864E-3</v>
+        <v>9.0723300721945472E-3</v>
       </c>
       <c r="R81">
         <f>STDEV(O$7:O$12,O$17:O$19)/SQRT(COUNT(O$7:O$12,O$17:O$19))</f>
-        <v>1.2371426206038684E-2</v>
+        <v>1.2129818847755281E-2</v>
       </c>
       <c r="S81">
         <f>STDEV(O$13:O$16)/SQRT(COUNT(O$13:O$16))</f>
-        <v>1.0739065203309861E-2</v>
+        <v>9.1385974951318887E-3</v>
       </c>
       <c r="U81">
         <f>STDEV(O$21:O$22)/SQRT(COUNT(O$21:O$22))</f>
-        <v>1.5080495951868553E-3</v>
+        <v>1.5092714424497777E-3</v>
       </c>
     </row>
     <row r="83" spans="16:24" x14ac:dyDescent="0.25">
@@ -5887,49 +5998,49 @@
       </c>
       <c r="Q84">
         <f>AVERAGE(P$1:P$3)</f>
-        <v>8.2769960388213756E-2</v>
+        <v>8.2769960386286354E-2</v>
       </c>
       <c r="R84">
         <f>AVERAGE(P$4:P$6)</f>
-        <v>8.1747173089443667E-2</v>
+        <v>8.1747176174903999E-2</v>
       </c>
       <c r="S84">
         <f>AVERAGE(P$7:P$12,P$17:P$19)</f>
-        <v>9.6620863256224487E-2</v>
+        <v>9.6618096060557532E-2</v>
       </c>
       <c r="T84">
         <f>AVERAGE(P$13:P$16)</f>
-        <v>8.0500034630017342E-2</v>
+        <v>8.0488259007867796E-2</v>
       </c>
       <c r="U84">
         <f>P$20</f>
-        <v>0.11612890078590109</v>
+        <v>0.11612890077785666</v>
       </c>
       <c r="V84">
         <f>AVERAGE(P$21:P$22)</f>
-        <v>0.13277519244528599</v>
+        <v>0.13277519443340902</v>
       </c>
     </row>
     <row r="85" spans="16:24" x14ac:dyDescent="0.25">
       <c r="Q85">
         <f>STDEV(P$1:P$3)/SQRT(COUNT(P$1:P$3))</f>
-        <v>6.1728202293721036E-3</v>
+        <v>6.1728202303740097E-3</v>
       </c>
       <c r="R85">
         <f>STDEV(P$4:P$6)/SQRT(COUNT(P$4:P$6))</f>
-        <v>4.7620690450541538E-3</v>
+        <v>4.7620664425895532E-3</v>
       </c>
       <c r="S85">
         <f>STDEV(P$7:P$12,P$17:P$19)/SQRT(COUNT(P$7:P$12,P$17:P$19))</f>
-        <v>1.5213373196767974E-2</v>
+        <v>1.5214270543208034E-2</v>
       </c>
       <c r="T85">
         <f>STDEV(P$13:P$16)/SQRT(COUNT(P$13:P$16))</f>
-        <v>2.0136089848698226E-2</v>
+        <v>2.014243603928605E-2</v>
       </c>
       <c r="V85">
         <f>STDEV(P$21:P$22)/SQRT(COUNT(P$21:P$22))</f>
-        <v>2.6130876680861656E-2</v>
+        <v>2.6130878673853903E-2</v>
       </c>
     </row>
     <row r="87" spans="16:24" x14ac:dyDescent="0.25">
@@ -5958,49 +6069,49 @@
       </c>
       <c r="R88">
         <f>AVERAGE(Q$1:Q$3)</f>
-        <v>0.12018439078457772</v>
+        <v>0.12003209288401152</v>
       </c>
       <c r="S88">
         <f>AVERAGE(Q$4:Q$6)</f>
-        <v>0.20592581575744995</v>
+        <v>0.21343844914888963</v>
       </c>
       <c r="T88">
         <f>AVERAGE(Q$7:Q$12,Q$17:Q$19)</f>
-        <v>0.21686058513632819</v>
+        <v>0.21495956670453156</v>
       </c>
       <c r="U88">
         <f>AVERAGE(Q$13:Q$16)</f>
-        <v>0.12972876005954909</v>
+        <v>0.12579060832283959</v>
       </c>
       <c r="V88">
         <f>Q$20</f>
-        <v>0.16359251437137434</v>
+        <v>0.16359252591784523</v>
       </c>
       <c r="W88">
         <f>AVERAGE(Q$21:Q$22)</f>
-        <v>0.22933938436391332</v>
+        <v>0.22933142053717082</v>
       </c>
     </row>
     <row r="89" spans="16:24" x14ac:dyDescent="0.25">
       <c r="R89">
         <f>STDEV(Q$1:Q$3)/SQRT(COUNT(Q$1:Q$3))</f>
-        <v>2.9775359996877627E-2</v>
+        <v>2.9915209911607666E-2</v>
       </c>
       <c r="S89">
         <f>STDEV(Q$4:Q$6)/SQRT(COUNT(Q$4:Q$6))</f>
-        <v>3.6389728937525907E-2</v>
+        <v>4.3580024502883882E-2</v>
       </c>
       <c r="T89">
         <f>STDEV(Q$7:Q$12,Q$17:Q$19)/SQRT(COUNT(Q$7:Q$12,Q$17:Q$19))</f>
-        <v>4.8831546850354256E-2</v>
+        <v>4.9563045357193969E-2</v>
       </c>
       <c r="U89">
         <f>STDEV(Q$13:Q$16)/SQRT(COUNT(Q$13:Q$16))</f>
-        <v>2.5236449475082544E-2</v>
+        <v>2.5182325466262E-2</v>
       </c>
       <c r="W89">
         <f>STDEV(Q$21:Q$22)/SQRT(COUNT(Q$21:Q$22))</f>
-        <v>5.2437138883405364E-2</v>
+        <v>5.2445112898152908E-2</v>
       </c>
     </row>
     <row r="91" spans="16:24" x14ac:dyDescent="0.25">
@@ -6029,49 +6140,49 @@
       </c>
       <c r="S92">
         <f>AVERAGE(R$1:R$3)</f>
-        <v>9.9458811979939485E-2</v>
+        <v>9.8876526846989221E-2</v>
       </c>
       <c r="T92">
         <f>AVERAGE(R$4:R$6)</f>
-        <v>0.13732819413560529</v>
+        <v>0.15989821775497828</v>
       </c>
       <c r="U92">
         <f>AVERAGE(R$7:R$12,R$17:R$19)</f>
-        <v>0.17061409936902006</v>
+        <v>0.1863577766352795</v>
       </c>
       <c r="V92">
         <f>AVERAGE(R$13:R$16)</f>
-        <v>0.19843944512266912</v>
+        <v>0.24531984414001679</v>
       </c>
       <c r="W92">
         <f>R$20</f>
-        <v>0.10046399115229929</v>
+        <v>0.10046394420079181</v>
       </c>
       <c r="X92">
         <f>AVERAGE(R$21:R$22)</f>
-        <v>0.11111458180796288</v>
+        <v>0.1111235379234371</v>
       </c>
     </row>
     <row r="93" spans="16:24" x14ac:dyDescent="0.25">
       <c r="S93">
         <f>STDEV(R$1:R$3)/SQRT(COUNT(R$1:R$3))</f>
-        <v>1.6801643371937947E-2</v>
+        <v>1.6225282641834871E-2</v>
       </c>
       <c r="T93">
         <f>STDEV(R$4:R$6)/SQRT(COUNT(R$4:R$6))</f>
-        <v>2.3923006639769231E-2</v>
+        <v>4.7075848425480959E-2</v>
       </c>
       <c r="U93">
         <f>STDEV(R$7:R$12,R$17:R$19)/SQRT(COUNT(R$7:R$12,R$17:R$19))</f>
-        <v>4.5152686356285339E-2</v>
+        <v>4.367031583618889E-2</v>
       </c>
       <c r="V93">
         <f>STDEV(R$13:R$16)/SQRT(COUNT(R$13:R$16))</f>
-        <v>5.3354507919078031E-2</v>
+        <v>4.2744543922925191E-2</v>
       </c>
       <c r="X93">
         <f>STDEV(R$21:R$22)/SQRT(COUNT(R$21:R$22))</f>
-        <v>1.5349754137446209E-2</v>
+        <v>1.5358734968358647E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made minor spreadsheet changes and got finalized in vivo data, got synthetic scripts ready to run
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation_moredata.xlsx
+++ b/Lacex_summary_FinalConfirmation_moredata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C71E6BC-F677-47C2-989C-BC89F2858420}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6C6E18-E144-45D6-B209-E7F0ACAE6C3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B075899B-8E8B-4489-B096-777C4BA97E2A}"/>
+    <workbookView xWindow="6090" yWindow="5250" windowWidth="12150" windowHeight="3300" xr2:uid="{B075899B-8E8B-4489-B096-777C4BA97E2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9778,8 +9778,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13808,7 +13808,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>